<commit_message>
website: added links to email list and ipmpack. updated the ipmpub excel file
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@516 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="204">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -629,6 +629,12 @@
   </si>
   <si>
     <t>Trends Ecol Evol</t>
+  </si>
+  <si>
+    <t>Adler, Dalgleish &amp; Ellner</t>
+  </si>
+  <si>
+    <t>Alder PB, Dalgleish HJ &amp; Ellner SP (2012) Forecasting plant community impacts of climate variability and change: when do competitive interactions matter? Journal of Ecology 100: 478-487</t>
   </si>
 </sst>
 </file>
@@ -710,8 +716,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="259">
+  <cellStyleXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -990,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="259">
+  <cellStyles count="265">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1120,6 +1132,9 @@
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1249,6 +1264,9 @@
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1264,7 +1282,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1304,43 +1322,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2012</c:v>
+                  <c:v>2012.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,43 +1370,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1403,11 +1421,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="162045952"/>
-        <c:axId val="162047872"/>
+        <c:axId val="569503032"/>
+        <c:axId val="569509944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162045952"/>
+        <c:axId val="569503032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1453,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162047872"/>
+        <c:crossAx val="569509944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162047872"/>
+        <c:axId val="569509944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162045952"/>
+        <c:crossAx val="569503032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,12 +1508,12 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2147,254 +2165,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B57" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="56">
-        <item x="9"/>
-        <item x="8"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="20"/>
-        <item x="19"/>
-        <item x="0"/>
-        <item x="11"/>
-        <item x="35"/>
-        <item x="18"/>
-        <item m="1" x="52"/>
-        <item x="16"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="24"/>
-        <item x="26"/>
-        <item x="32"/>
-        <item x="36"/>
-        <item x="30"/>
-        <item x="22"/>
-        <item x="5"/>
-        <item m="1" x="54"/>
-        <item x="2"/>
-        <item x="37"/>
-        <item x="23"/>
-        <item x="12"/>
-        <item x="10"/>
-        <item x="21"/>
-        <item x="15"/>
-        <item x="6"/>
-        <item x="38"/>
-        <item x="29"/>
-        <item x="28"/>
-        <item x="17"/>
-        <item x="39"/>
-        <item x="27"/>
-        <item x="3"/>
-        <item x="25"/>
-        <item x="1"/>
-        <item m="1" x="53"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="31"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="53">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BG19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -2694,6 +2464,254 @@
     <i t="grand">
       <x/>
     </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:B57" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="56">
+        <item x="9"/>
+        <item x="8"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="0"/>
+        <item x="11"/>
+        <item x="35"/>
+        <item x="18"/>
+        <item m="1" x="52"/>
+        <item x="16"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="24"/>
+        <item x="26"/>
+        <item x="32"/>
+        <item x="36"/>
+        <item x="30"/>
+        <item x="22"/>
+        <item x="5"/>
+        <item m="1" x="54"/>
+        <item x="2"/>
+        <item x="37"/>
+        <item x="23"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="21"/>
+        <item x="15"/>
+        <item x="6"/>
+        <item x="38"/>
+        <item x="29"/>
+        <item x="28"/>
+        <item x="17"/>
+        <item x="39"/>
+        <item x="27"/>
+        <item x="3"/>
+        <item x="25"/>
+        <item x="1"/>
+        <item m="1" x="53"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="31"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="53">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -3029,26 +3047,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.875" customWidth="1"/>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3071,7 +3089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3091,7 +3109,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3131,7 +3149,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -3151,138 +3169,138 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>2012</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>2012</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>2012</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>2012</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C10">
         <v>2010</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>86</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
         <v>191</v>
-      </c>
-      <c r="C7">
-        <v>2011</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8">
-        <v>2011</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9">
-        <v>2003</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10">
-        <v>2004</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>200</v>
       </c>
       <c r="C11">
         <v>2011</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>123</v>
+        <v>87</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C12">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>85</v>
@@ -3291,95 +3309,95 @@
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C13">
-        <v>2011</v>
+        <v>2003</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C14">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C15">
         <v>2011</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>2009</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
+        <v>2010</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>196</v>
       </c>
       <c r="C17">
         <v>2011</v>
@@ -3388,267 +3406,264 @@
         <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>196</v>
       </c>
       <c r="C18">
-        <v>2009</v>
-      </c>
-      <c r="D18" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
         <v>196</v>
       </c>
       <c r="C19">
+        <v>2011</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2009</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>2011</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22">
+        <v>2009</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23">
         <v>2000</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G23" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C20">
+      <c r="C24">
         <v>2006</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="C25">
         <v>2007</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="9" t="s">
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
         <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>2011</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C23">
-        <v>2002</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24">
-        <v>2010</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25">
-        <v>2008</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26">
+        <v>2011</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27">
+        <v>2002</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28">
         <v>2010</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>2008</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
         <v>21</v>
-      </c>
-      <c r="C27">
-        <v>2012</v>
-      </c>
-      <c r="D27" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" t="s">
-        <v>126</v>
-      </c>
-      <c r="F27" t="s">
-        <v>190</v>
-      </c>
-      <c r="G27" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>196</v>
-      </c>
-      <c r="C28">
-        <v>2011</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29">
-        <v>2012</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" t="s">
-        <v>196</v>
       </c>
       <c r="C30">
         <v>2010</v>
@@ -3657,38 +3672,41 @@
         <v>10</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>43</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>44</v>
+        <v>126</v>
+      </c>
+      <c r="E31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" t="s">
+        <v>190</v>
       </c>
       <c r="G31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="C32">
         <v>2011</v>
@@ -3697,133 +3715,133 @@
         <v>10</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33">
+        <v>2012</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34">
+        <v>2010</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35">
+        <v>2008</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>2011</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G36" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
         <v>92</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>194</v>
-      </c>
-      <c r="C33">
-        <v>2009</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>89</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34">
-        <v>2009</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35">
-        <v>2009</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" t="s">
-        <v>196</v>
-      </c>
-      <c r="C36">
-        <v>2009</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" t="s">
-        <v>196</v>
       </c>
       <c r="C37">
         <v>2009</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="G37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>196</v>
+        <v>84</v>
       </c>
       <c r="C38">
         <v>2009</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -3837,13 +3855,13 @@
         <v>10</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G39" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -3857,13 +3875,13 @@
         <v>10</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -3877,13 +3895,13 @@
         <v>10</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G41" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -3897,13 +3915,13 @@
         <v>10</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G42" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3917,13 +3935,13 @@
         <v>10</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>106</v>
       </c>
@@ -3937,38 +3955,38 @@
         <v>10</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G44" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="C45">
         <v>2009</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="G45" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C46">
         <v>2009</v>
@@ -3977,38 +3995,38 @@
         <v>10</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="G46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C47">
-        <v>2007</v>
-      </c>
-      <c r="D47" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="G47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C48">
         <v>2009</v>
@@ -4017,78 +4035,78 @@
         <v>10</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="G48" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>193</v>
+        <v>121</v>
       </c>
       <c r="C49">
-        <v>2012</v>
-      </c>
-      <c r="D49" s="2" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D49" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="G49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="C50">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>201</v>
       </c>
       <c r="C51">
-        <v>2010</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>85</v>
+        <v>2007</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="C52">
         <v>2009</v>
@@ -4097,287 +4115,284 @@
         <v>10</v>
       </c>
       <c r="E52" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53">
+        <v>2012</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>2011</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>2010</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>2009</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G56" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>54</v>
       </c>
-      <c r="C53">
+      <c r="C57">
         <v>2009</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="9" t="s">
+      <c r="D57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G57" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
         <v>124</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>194</v>
       </c>
-      <c r="C54">
+      <c r="C58">
         <v>2012</v>
       </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="9" t="s">
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G58" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>191</v>
-      </c>
-      <c r="C55">
-        <v>2009</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G55" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" t="s">
-        <v>197</v>
-      </c>
-      <c r="C56">
-        <v>2002</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G56" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57">
-        <v>2006</v>
-      </c>
-      <c r="D57" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>93</v>
-      </c>
-      <c r="B58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58">
-        <v>2006</v>
-      </c>
-      <c r="D58" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" t="s">
-        <v>118</v>
       </c>
       <c r="C59">
         <v>2009</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F59" t="s">
-        <v>127</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C60">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
-      </c>
-      <c r="C61" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <v>2006</v>
+      </c>
+      <c r="D61" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
         <v>28</v>
       </c>
       <c r="C62">
+        <v>2006</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63">
+        <v>2009</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F63" t="s">
+        <v>127</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" t="s">
+        <v>196</v>
+      </c>
+      <c r="C64">
+        <v>2005</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" t="s">
+        <v>28</v>
+      </c>
+      <c r="C66">
         <v>2010</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F62" t="s">
-        <v>127</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63">
-        <v>2010</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64">
-        <v>2010</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" t="s">
-        <v>21</v>
-      </c>
-      <c r="C65">
-        <v>2005</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>181</v>
-      </c>
-      <c r="B66" t="s">
-        <v>182</v>
-      </c>
-      <c r="C66">
-        <v>2012</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>126</v>
@@ -4388,196 +4403,199 @@
       <c r="F66" t="s">
         <v>127</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67">
+        <v>2010</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68">
+        <v>2010</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <v>2005</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" t="s">
+        <v>182</v>
+      </c>
+      <c r="C70">
+        <v>2012</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
         <v>68</v>
-      </c>
-      <c r="B67" t="s">
-        <v>196</v>
-      </c>
-      <c r="C67">
-        <v>2011</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>119</v>
-      </c>
-      <c r="B68" t="s">
-        <v>194</v>
-      </c>
-      <c r="C68">
-        <v>2012</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" t="s">
-        <v>198</v>
-      </c>
-      <c r="C69">
-        <v>2012</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>28</v>
-      </c>
-      <c r="C70">
-        <v>2009</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>72</v>
       </c>
       <c r="B71" t="s">
         <v>196</v>
       </c>
       <c r="C71">
+        <v>2011</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72">
+        <v>2012</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" t="s">
+        <v>198</v>
+      </c>
+      <c r="C73">
+        <v>2012</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74">
+        <v>2009</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75">
         <v>2006</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="9" t="s">
+      <c r="D75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>73</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B76" t="s">
         <v>196</v>
-      </c>
-      <c r="C72">
-        <v>2010</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>74</v>
-      </c>
-      <c r="B73" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73">
-        <v>2010</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G73" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74">
-        <v>2010</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>21</v>
-      </c>
-      <c r="C75">
-        <v>2010</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" t="s">
-        <v>21</v>
       </c>
       <c r="C76">
         <v>2010</v>
@@ -4586,13 +4604,13 @@
         <v>10</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -4606,13 +4624,13 @@
         <v>10</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -4626,9 +4644,89 @@
         <v>10</v>
       </c>
       <c r="E78" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>2010</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80">
+        <v>2010</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="s">
+        <v>21</v>
+      </c>
+      <c r="C81">
+        <v>2010</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <v>2010</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="G82" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4637,7 +4735,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4654,68 +4752,68 @@
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.125" customWidth="1"/>
-    <col min="35" max="35" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" customWidth="1"/>
+    <col min="35" max="35" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.875" customWidth="1"/>
-    <col min="47" max="47" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.83203125" customWidth="1"/>
+    <col min="47" max="47" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.375" customWidth="1"/>
-    <col min="59" max="59" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.33203125" customWidth="1"/>
+    <col min="59" max="59" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59">
       <c r="A3" s="4" t="s">
         <v>94</v>
       </c>
@@ -4726,7 +4824,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59">
       <c r="A4" s="4" t="s">
         <v>96</v>
       </c>
@@ -4896,7 +4994,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
@@ -4964,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5032,7 +5130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -5100,7 +5198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59">
       <c r="A8" s="5" t="s">
         <v>75</v>
       </c>
@@ -5168,7 +5266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59">
       <c r="A9" s="5" t="s">
         <v>90</v>
       </c>
@@ -5238,7 +5336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -5312,7 +5410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -5380,7 +5478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
@@ -5450,7 +5548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59">
       <c r="A13" s="5" t="s">
         <v>76</v>
       </c>
@@ -5560,7 +5658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -5664,7 +5762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -5754,7 +5852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5826,7 +5924,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -5894,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:59">
       <c r="A18" s="5" t="s">
         <v>55</v>
       </c>
@@ -5958,7 +6056,7 @@
       <c r="BF18" s="6"/>
       <c r="BG18" s="6"/>
     </row>
-    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:59">
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
@@ -6128,7 +6226,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:59">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -6136,7 +6234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:59">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -6144,7 +6242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:59">
       <c r="A22" s="5" t="s">
         <v>67</v>
       </c>
@@ -6152,7 +6250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:59">
       <c r="A23" s="5" t="s">
         <v>82</v>
       </c>
@@ -6166,7 +6264,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:59">
       <c r="A24" s="5" t="s">
         <v>87</v>
       </c>
@@ -6180,7 +6278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:59">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -6194,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:59">
       <c r="A26" s="5" t="s">
         <v>78</v>
       </c>
@@ -6208,7 +6306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:59">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -6222,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:59">
       <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
@@ -6236,7 +6334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:59">
       <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
@@ -6250,7 +6348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:59">
       <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
@@ -6264,7 +6362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:59">
       <c r="A31" s="5" t="s">
         <v>40</v>
       </c>
@@ -6278,7 +6376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:59">
       <c r="A32" s="5" t="s">
         <v>19</v>
       </c>
@@ -6292,7 +6390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>79</v>
       </c>
@@ -6306,7 +6404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>65</v>
       </c>
@@ -6320,7 +6418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
@@ -6334,7 +6432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>11</v>
       </c>
@@ -6348,7 +6446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
@@ -6357,7 +6455,7 @@
       </c>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>62</v>
       </c>
@@ -6365,7 +6463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>88</v>
       </c>
@@ -6373,7 +6471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>56</v>
       </c>
@@ -6381,7 +6479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
@@ -6389,7 +6487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>34</v>
       </c>
@@ -6397,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
@@ -6405,7 +6503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
@@ -6413,7 +6511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>104</v>
       </c>
@@ -6421,7 +6519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
         <v>107</v>
       </c>
@@ -6429,7 +6527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>108</v>
       </c>
@@ -6437,7 +6535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>109</v>
       </c>
@@ -6445,7 +6543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="5" t="s">
         <v>110</v>
       </c>
@@ -6453,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="5" t="s">
         <v>111</v>
       </c>
@@ -6461,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="5" t="s">
         <v>112</v>
       </c>
@@ -6469,7 +6567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
@@ -6477,7 +6575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="5" t="s">
         <v>114</v>
       </c>
@@ -6485,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="5" t="s">
         <v>115</v>
       </c>
@@ -6493,7 +6591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="5" t="s">
         <v>116</v>
       </c>
@@ -6501,7 +6599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="5" t="s">
         <v>123</v>
       </c>
@@ -6509,7 +6607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="5" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
added Ferrer-Cervantes to IPMliteraturelist
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@519 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="-25605" yWindow="-435" windowWidth="25605" windowHeight="18240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="208">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -635,6 +635,18 @@
   </si>
   <si>
     <t>Alder PB, Dalgleish HJ &amp; Ellner SP (2012) Forecasting plant community impacts of climate variability and change: when do competitive interactions matter? Journal of Ecology 100: 478-487</t>
+  </si>
+  <si>
+    <t>Ferrer-Cervantes, Mendez-Gonzalez, Quintana-Ascencio, Dorantes, Dzib &amp; Duran</t>
+  </si>
+  <si>
+    <t>Popul Ecol</t>
+  </si>
+  <si>
+    <t>Mammillaria gaumeri</t>
+  </si>
+  <si>
+    <t>Ferrer-Cervantes, M.E., Méndez-González, M.E., Quintana-Ascencio, P.-F., Dorantes, A., Dzib, G. &amp; Durán, R. (2012) Population dynamics of the cactus Mammillaria gaumeri: an integral projection model approach. Population Ecology, 54, 321-334.</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1294,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1322,43 +1334,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>2000.0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2001.0</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2002.0</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2003.0</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2004.0</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2005.0</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2006.0</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2007.0</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2008.0</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2009.0</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2010.0</c:v>
+                  <c:v>2010</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2011.0</c:v>
+                  <c:v>2011</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2012.0</c:v>
+                  <c:v>2012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1370,43 +1382,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1421,11 +1433,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="569503032"/>
-        <c:axId val="569509944"/>
+        <c:axId val="123836288"/>
+        <c:axId val="154723072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="569503032"/>
+        <c:axId val="123836288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,7 +1465,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569509944"/>
+        <c:crossAx val="154723072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1473,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="569509944"/>
+        <c:axId val="154723072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569503032"/>
+        <c:crossAx val="123836288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1513,7 +1525,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2165,7 +2177,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BG19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -2478,7 +2490,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:B57" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -3047,26 +3059,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:D9"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.875" customWidth="1"/>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3089,7 +3101,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -3109,7 +3121,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -3129,7 +3141,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -3149,7 +3161,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -3169,7 +3181,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -3189,7 +3201,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -3209,7 +3221,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>202</v>
       </c>
@@ -3229,7 +3241,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -3249,7 +3261,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3269,7 +3281,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -3312,7 +3324,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3332,7 +3344,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3352,7 +3364,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -3372,7 +3384,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3392,7 +3404,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -3412,7 +3424,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3444,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3452,7 +3464,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3472,7 +3484,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3492,7 +3504,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -3512,7 +3524,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -3552,7 +3564,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3572,261 +3584,261 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>204</v>
+      </c>
+      <c r="B26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26">
+        <v>2012</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G26" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>2011</v>
       </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>193</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>2002</v>
       </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="9" t="s">
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>35</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>195</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>2010</v>
       </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>2008</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>2008</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30">
-        <v>2010</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="10" t="s">
-        <v>125</v>
       </c>
       <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31">
+        <v>2010</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32">
         <v>2012</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>126</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>126</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>190</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>196</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>2011</v>
       </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="9" t="s">
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>102</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>103</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>2012</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" t="s">
-        <v>196</v>
-      </c>
-      <c r="C34">
-        <v>2010</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35">
+        <v>2010</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>43</v>
-      </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35">
-        <v>2008</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>45</v>
       </c>
       <c r="B36" t="s">
         <v>21</v>
       </c>
       <c r="C36">
+        <v>2008</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37">
         <v>2011</v>
       </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="9" t="s">
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>92</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>194</v>
-      </c>
-      <c r="C37">
-        <v>2009</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
       </c>
       <c r="C38">
         <v>2009</v>
@@ -3835,33 +3847,33 @@
         <v>10</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>196</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>2009</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -3875,13 +3887,13 @@
         <v>10</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -3895,13 +3907,13 @@
         <v>10</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G41" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -3915,13 +3927,13 @@
         <v>10</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G42" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3935,13 +3947,13 @@
         <v>10</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>106</v>
       </c>
@@ -3955,13 +3967,13 @@
         <v>10</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G44" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -3975,13 +3987,13 @@
         <v>10</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G45" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3995,13 +4007,13 @@
         <v>10</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G46" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -4015,13 +4027,13 @@
         <v>10</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G47" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -4035,173 +4047,173 @@
         <v>10</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>196</v>
       </c>
       <c r="C49">
         <v>2009</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="G49" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="C50">
         <v>2009</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" t="s">
         <v>10</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G50" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
         <v>201</v>
       </c>
       <c r="C51">
+        <v>2009</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" t="s">
+        <v>201</v>
+      </c>
+      <c r="C52">
         <v>2007</v>
       </c>
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="9" t="s">
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G52" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>191</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>2009</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="9" t="s">
+      <c r="D53" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>192</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>193</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>2012</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="9" t="s">
+      <c r="D54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G54" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>81</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>21</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>2011</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="9" t="s">
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>50</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>51</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>2010</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E56" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56">
-        <v>2009</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G56" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -4215,93 +4227,93 @@
         <v>10</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G57" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58">
+        <v>2009</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>124</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>194</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>2012</v>
       </c>
-      <c r="D58" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="9" t="s">
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>191</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>2009</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="9" t="s">
+      <c r="D60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G60" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>197</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>2002</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="9" t="s">
+      <c r="D61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G61" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>93</v>
-      </c>
-      <c r="B61" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61">
-        <v>2006</v>
-      </c>
-      <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>93</v>
       </c>
@@ -4315,101 +4327,98 @@
         <v>10</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="G62" s="11" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63">
+        <v>2006</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>117</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>118</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>2009</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>127</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G64" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>59</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>196</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>2005</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="9" t="s">
+      <c r="D65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="G65" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
-      <c r="A65" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>166</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>193</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>167</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="9" t="s">
+      <c r="D66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
-      <c r="A66" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>168</v>
-      </c>
-      <c r="B66" t="s">
-        <v>28</v>
-      </c>
-      <c r="C66">
-        <v>2010</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F66" t="s">
-        <v>127</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" t="s">
-        <v>63</v>
       </c>
       <c r="B67" t="s">
         <v>28</v>
@@ -4418,16 +4427,19 @@
         <v>2010</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>64</v>
+        <v>126</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F67" t="s">
+        <v>127</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -4441,64 +4453,61 @@
         <v>10</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69">
+        <v>2010</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>66</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>21</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>2005</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="9" t="s">
+      <c r="D70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="G70" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>181</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>182</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>2012</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F70" t="s">
-        <v>127</v>
-      </c>
-      <c r="G70" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B71" t="s">
-        <v>196</v>
-      </c>
-      <c r="C71">
-        <v>2011</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>126</v>
@@ -4506,19 +4515,22 @@
       <c r="E71" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G71" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="F71" t="s">
+        <v>127</v>
+      </c>
+      <c r="G71" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C72">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>126</v>
@@ -4527,15 +4539,15 @@
         <v>126</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C73">
         <v>2012</v>
@@ -4547,75 +4559,75 @@
         <v>126</v>
       </c>
       <c r="G73" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" t="s">
+        <v>198</v>
+      </c>
+      <c r="C74">
+        <v>2012</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G74" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>69</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>28</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>2009</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="9" t="s">
+      <c r="D75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>72</v>
-      </c>
-      <c r="B75" t="s">
-        <v>196</v>
-      </c>
-      <c r="C75">
-        <v>2006</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>73</v>
       </c>
       <c r="B76" t="s">
         <v>196</v>
       </c>
       <c r="C76">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="C77">
         <v>2010</v>
@@ -4624,13 +4636,13 @@
         <v>10</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -4644,13 +4656,13 @@
         <v>10</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G78" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -4664,13 +4676,13 @@
         <v>10</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G79" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -4684,13 +4696,13 @@
         <v>10</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -4704,13 +4716,13 @@
         <v>10</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -4724,9 +4736,29 @@
         <v>10</v>
       </c>
       <c r="E82" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>74</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>2010</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G82" s="11" t="s">
+      <c r="G83" s="11" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4752,68 +4784,68 @@
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.1640625" customWidth="1"/>
-    <col min="35" max="35" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.125" customWidth="1"/>
+    <col min="35" max="35" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.83203125" customWidth="1"/>
-    <col min="47" max="47" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.875" customWidth="1"/>
+    <col min="47" max="47" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.875" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.33203125" customWidth="1"/>
-    <col min="59" max="59" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.375" customWidth="1"/>
+    <col min="59" max="59" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:59">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>94</v>
       </c>
@@ -4824,7 +4856,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:59">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>96</v>
       </c>
@@ -4994,7 +5026,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:59">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
@@ -5062,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:59">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -5130,7 +5162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:59">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -5198,7 +5230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:59">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>75</v>
       </c>
@@ -5266,7 +5298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:59">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>90</v>
       </c>
@@ -5336,7 +5368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:59">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -5410,7 +5442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:59">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -5478,7 +5510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:59">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
@@ -5548,7 +5580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:59">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>76</v>
       </c>
@@ -5658,7 +5690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:59">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -5762,7 +5794,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:59">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -5852,7 +5884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:59">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5924,7 +5956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:59">
+    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -5992,7 +6024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:59">
+    <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>55</v>
       </c>
@@ -6056,7 +6088,7 @@
       <c r="BF18" s="6"/>
       <c r="BG18" s="6"/>
     </row>
-    <row r="19" spans="1:59">
+    <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>61</v>
       </c>
@@ -6226,7 +6258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:59">
+    <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>70</v>
       </c>
@@ -6234,7 +6266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:59">
+    <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>77</v>
       </c>
@@ -6242,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:59">
+    <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>67</v>
       </c>
@@ -6250,7 +6282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:59">
+    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>82</v>
       </c>
@@ -6264,7 +6296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:59">
+    <row r="24" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>87</v>
       </c>
@@ -6278,7 +6310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:59">
+    <row r="25" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -6292,7 +6324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:59">
+    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>78</v>
       </c>
@@ -6306,7 +6338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:59">
+    <row r="27" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -6320,7 +6352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:59">
+    <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
@@ -6334,7 +6366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:59">
+    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
@@ -6348,7 +6380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:59">
+    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>48</v>
       </c>
@@ -6362,7 +6394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:59">
+    <row r="31" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>40</v>
       </c>
@@ -6376,7 +6408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:59">
+    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>19</v>
       </c>
@@ -6390,7 +6422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>79</v>
       </c>
@@ -6404,7 +6436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>65</v>
       </c>
@@ -6418,7 +6450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
@@ -6432,7 +6464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>11</v>
       </c>
@@ -6446,7 +6478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
@@ -6455,7 +6487,7 @@
       </c>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>62</v>
       </c>
@@ -6463,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>88</v>
       </c>
@@ -6471,7 +6503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>56</v>
       </c>
@@ -6479,7 +6511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
@@ -6487,7 +6519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>34</v>
       </c>
@@ -6495,7 +6527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
@@ -6503,7 +6535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
@@ -6511,7 +6543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>104</v>
       </c>
@@ -6519,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>107</v>
       </c>
@@ -6527,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>108</v>
       </c>
@@ -6535,7 +6567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>109</v>
       </c>
@@ -6543,7 +6575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>110</v>
       </c>
@@ -6551,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>111</v>
       </c>
@@ -6559,7 +6591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>112</v>
       </c>
@@ -6567,7 +6599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
@@ -6575,7 +6607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>114</v>
       </c>
@@ -6583,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>115</v>
       </c>
@@ -6591,7 +6623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>116</v>
       </c>
@@ -6599,7 +6631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>123</v>
       </c>
@@ -6607,7 +6639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
added Dahlgren, J.P., García, M.B. & Ehrlén, J. (2011) Nonlinear relationships between vital rates and state variables in demographic models. Ecology, 92, 1181-7.
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@534 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="210">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Kolb, Dahlgren &amp; Ehrlen</t>
   </si>
   <si>
-    <t>Planta</t>
-  </si>
-  <si>
     <t>Phyteuma spicatum</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>Ovis aries</t>
   </si>
   <si>
-    <t>Dalhlgren &amp; Ehrlen</t>
-  </si>
-  <si>
     <t>J Ecol</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>J Math Biol</t>
   </si>
   <si>
-    <t>Garcia, Dahlgren &amp; Ehrlen</t>
-  </si>
-  <si>
     <t>Borderea pyrenaica</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
     <t>CLONAL</t>
   </si>
   <si>
-    <t>Hesse, Rees &amp; Muller-Scharer</t>
-  </si>
-  <si>
     <t>Jacquemyn, Brys &amp; Jongejans</t>
   </si>
   <si>
@@ -650,6 +638,21 @@
   </si>
   <si>
     <t>Plantae</t>
+  </si>
+  <si>
+    <t>Hesse, Rees &amp; Müller-Schärer</t>
+  </si>
+  <si>
+    <t>García, Dahlgren &amp; Ehrlén</t>
+  </si>
+  <si>
+    <t>Dahlgren &amp; Ehrlén</t>
+  </si>
+  <si>
+    <t>Dahlgren, García &amp; Ehrlén</t>
+  </si>
+  <si>
+    <t>Dahlgren JP, García MB &amp; Ehrlén J (2011) Nonlinear relationships between vital rates and state variables in demographic models. Ecology 92: 1181-1187</t>
   </si>
 </sst>
 </file>
@@ -1436,11 +1439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175760896"/>
-        <c:axId val="175764992"/>
+        <c:axId val="113140096"/>
+        <c:axId val="113142016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175760896"/>
+        <c:axId val="113140096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175764992"/>
+        <c:crossAx val="113142016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1476,7 +1479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175764992"/>
+        <c:axId val="113142016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175760896"/>
+        <c:crossAx val="113140096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2180,7 +2183,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BG19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -2493,7 +2496,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:B57" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -3062,13 +3065,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D75" sqref="D75:D83"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3098,313 +3101,313 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>2010</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
+      <c r="D2" t="s">
+        <v>204</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>2010</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
+      <c r="D3" t="s">
+        <v>204</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>2010</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>204</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>2010</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
+      <c r="D5" t="s">
+        <v>204</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>2012</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
+      <c r="D6" t="s">
+        <v>204</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>2012</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
+      <c r="D7" t="s">
+        <v>204</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>2012</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
+      <c r="D8" t="s">
+        <v>204</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>2012</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
+      <c r="D9" t="s">
+        <v>204</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
       </c>
       <c r="C10">
         <v>2010</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C11">
         <v>2011</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12">
         <v>2011</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C13">
         <v>2003</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C14">
         <v>2004</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C15">
         <v>2011</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
       </c>
       <c r="C16">
         <v>2010</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3412,19 +3415,19 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C17">
         <v>2011</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3432,19 +3435,19 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C18">
         <v>2011</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3452,1317 +3455,1337 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C19">
         <v>2011</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>2009</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>207</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>2011</v>
       </c>
       <c r="D21" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C22">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="D22" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>104</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C23">
-        <v>2000</v>
+        <v>2009</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="C24">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D25" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>204</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="D26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>206</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="C27">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>178</v>
+        <v>202</v>
+      </c>
+      <c r="G27" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>206</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>19</v>
       </c>
       <c r="C28">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="D28" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" t="s">
-        <v>143</v>
+        <v>28</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C29">
-        <v>2010</v>
+        <v>2002</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="C30">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C31">
+        <v>2008</v>
+      </c>
+      <c r="D31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32">
         <v>2010</v>
       </c>
-      <c r="D31" t="s">
-        <v>208</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32">
+      <c r="D32" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33">
         <v>2012</v>
       </c>
-      <c r="D32" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" t="s">
-        <v>190</v>
-      </c>
-      <c r="G32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" t="s">
-        <v>196</v>
-      </c>
-      <c r="C33">
-        <v>2011</v>
-      </c>
       <c r="D33" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>41</v>
+        <v>122</v>
+      </c>
+      <c r="E33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" t="s">
+        <v>186</v>
       </c>
       <c r="G33" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>192</v>
       </c>
       <c r="C34">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D34" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>179</v>
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="C35">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" t="s">
-        <v>150</v>
+        <v>10</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
       <c r="C36">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D37" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>19</v>
       </c>
       <c r="C38">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>190</v>
       </c>
       <c r="C39">
         <v>2009</v>
       </c>
       <c r="D39" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="C40">
         <v>2009</v>
       </c>
       <c r="D40" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C41">
         <v>2009</v>
       </c>
       <c r="D41" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C44">
         <v>2009</v>
       </c>
       <c r="D44" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C45">
         <v>2009</v>
       </c>
       <c r="D45" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G45" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C46">
         <v>2009</v>
       </c>
       <c r="D46" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G46" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C47">
         <v>2009</v>
       </c>
       <c r="D47" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B48" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C48">
         <v>2009</v>
       </c>
       <c r="D48" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G48" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C49">
         <v>2009</v>
       </c>
       <c r="D49" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G49" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>192</v>
       </c>
       <c r="C50">
         <v>2009</v>
       </c>
       <c r="D50" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="C51">
         <v>2009</v>
       </c>
       <c r="D51" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G51" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C52">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="B53" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C53">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="D53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G53" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C54">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D54" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G54" s="12" t="s">
-        <v>199</v>
+        <v>44</v>
+      </c>
+      <c r="G54" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
       <c r="C55">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D55" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G55" t="s">
-        <v>160</v>
+        <v>36</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>2010</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>85</v>
+        <v>2011</v>
+      </c>
+      <c r="D56" t="s">
+        <v>204</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="G56" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C57">
-        <v>2009</v>
-      </c>
-      <c r="D57" t="s">
-        <v>208</v>
+        <v>2010</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G57" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C58">
         <v>2009</v>
       </c>
       <c r="D58" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G58" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>124</v>
+        <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>50</v>
       </c>
       <c r="C59">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D59" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="G59" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C60">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D60" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C61">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="D61" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="C62">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="D62" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="11" t="s">
-        <v>186</v>
+        <v>30</v>
+      </c>
+      <c r="G62" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C63">
         <v>2006</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>26</v>
       </c>
       <c r="C64">
-        <v>2009</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F64" t="s">
-        <v>127</v>
+        <v>2006</v>
+      </c>
+      <c r="D64" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>114</v>
       </c>
       <c r="C65">
-        <v>2005</v>
-      </c>
-      <c r="D65" t="s">
-        <v>208</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>14</v>
+        <v>2009</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F65" t="s">
+        <v>123</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" t="s">
-        <v>167</v>
+        <v>192</v>
+      </c>
+      <c r="C66">
+        <v>2005</v>
       </c>
       <c r="D66" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67">
-        <v>2010</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F67" t="s">
-        <v>127</v>
+        <v>189</v>
+      </c>
+      <c r="C67" t="s">
+        <v>163</v>
+      </c>
+      <c r="D67" t="s">
+        <v>204</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C68">
         <v>2010</v>
       </c>
-      <c r="D68" t="s">
-        <v>208</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>64</v>
+      <c r="D68" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" t="s">
+        <v>123</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C69">
         <v>2010</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C70">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71">
+        <v>2005</v>
+      </c>
+      <c r="D71" t="s">
+        <v>204</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G71" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="B71" t="s">
-        <v>182</v>
-      </c>
-      <c r="C71">
-        <v>2012</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F71" t="s">
-        <v>127</v>
-      </c>
-      <c r="G71" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>177</v>
       </c>
       <c r="B72" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C72">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>171</v>
+        <v>122</v>
+      </c>
+      <c r="F72" t="s">
+        <v>123</v>
+      </c>
+      <c r="G72" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C73">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C74">
         <v>2012</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="C75">
-        <v>2009</v>
-      </c>
-      <c r="D75" t="s">
-        <v>208</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>70</v>
+        <v>2012</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>196</v>
+        <v>26</v>
       </c>
       <c r="C76">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="D76" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C77">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D77" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>192</v>
       </c>
       <c r="C78">
         <v>2010</v>
       </c>
       <c r="D78" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C79">
         <v>2010</v>
       </c>
       <c r="D79" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C80">
         <v>2010</v>
       </c>
       <c r="D80" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C81">
         <v>2010</v>
       </c>
       <c r="D81" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C82">
         <v>2010</v>
       </c>
       <c r="D82" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C83">
         <v>2010</v>
       </c>
       <c r="D83" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84">
+        <v>2010</v>
+      </c>
+      <c r="D84" t="s">
+        <v>204</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4770,7 +4793,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4850,188 +4873,188 @@
   <sheetData>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
         <v>71</v>
       </c>
-      <c r="J4" t="s">
-        <v>75</v>
-      </c>
       <c r="K4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="O4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="R4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="U4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="V4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="X4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Y4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Z4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="AA4" t="s">
         <v>2</v>
       </c>
       <c r="AB4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AC4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP4" t="s">
         <v>52</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AQ4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS4" t="s">
         <v>33</v>
       </c>
-      <c r="AE4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>36</v>
-      </c>
       <c r="AT4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AU4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW4" t="s">
         <v>104</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AX4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>107</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="BA4" t="s">
         <v>108</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BB4" t="s">
         <v>109</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BC4" t="s">
         <v>110</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BD4" t="s">
         <v>111</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BE4" t="s">
         <v>112</v>
       </c>
-      <c r="BB4" t="s">
-        <v>113</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>114</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>115</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>116</v>
-      </c>
       <c r="BF4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="BG4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -5099,7 +5122,7 @@
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
@@ -5167,7 +5190,7 @@
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
@@ -5235,7 +5258,7 @@
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
@@ -5303,7 +5326,7 @@
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
@@ -5373,7 +5396,7 @@
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
@@ -5515,7 +5538,7 @@
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
@@ -5585,7 +5608,7 @@
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -5695,7 +5718,7 @@
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6">
         <v>1</v>
@@ -5799,7 +5822,7 @@
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B15" s="6">
         <v>3</v>
@@ -5889,7 +5912,7 @@
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6">
         <v>4</v>
@@ -5961,13 +5984,13 @@
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="6">
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -6029,13 +6052,13 @@
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B18" s="6">
         <v>1</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -6093,13 +6116,13 @@
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G19" s="6">
         <v>1</v>
@@ -6263,7 +6286,7 @@
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B20" s="6">
         <v>2</v>
@@ -6271,7 +6294,7 @@
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -6279,7 +6302,7 @@
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -6287,7 +6310,7 @@
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -6296,12 +6319,12 @@
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B24" s="6">
         <v>1</v>
@@ -6329,7 +6352,7 @@
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
@@ -6343,7 +6366,7 @@
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" s="6">
         <v>1</v>
@@ -6357,7 +6380,7 @@
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" s="6">
         <v>3</v>
@@ -6371,7 +6394,7 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" s="6">
         <v>3</v>
@@ -6385,7 +6408,7 @@
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
@@ -6399,7 +6422,7 @@
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
@@ -6413,7 +6436,7 @@
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="6">
         <v>2</v>
@@ -6427,7 +6450,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B33" s="6">
         <v>1</v>
@@ -6441,7 +6464,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B34" s="6">
         <v>1</v>
@@ -6455,7 +6478,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
@@ -6469,7 +6492,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="6">
         <v>2</v>
@@ -6483,7 +6506,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
@@ -6492,7 +6515,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
@@ -6500,7 +6523,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B39" s="6">
         <v>1</v>
@@ -6508,7 +6531,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B40" s="6">
         <v>1</v>
@@ -6524,7 +6547,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B42" s="6">
         <v>1</v>
@@ -6532,7 +6555,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B43" s="6">
         <v>1</v>
@@ -6540,7 +6563,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B44" s="6">
         <v>3</v>
@@ -6548,7 +6571,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B45" s="6">
         <v>1</v>
@@ -6556,7 +6579,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B46" s="6">
         <v>1</v>
@@ -6564,7 +6587,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B47" s="6">
         <v>1</v>
@@ -6572,7 +6595,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B48" s="6">
         <v>1</v>
@@ -6580,7 +6603,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B49" s="6">
         <v>1</v>
@@ -6588,7 +6611,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B50" s="6">
         <v>1</v>
@@ -6596,7 +6619,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B51" s="6">
         <v>1</v>
@@ -6604,7 +6627,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
@@ -6612,7 +6635,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B53" s="6">
         <v>1</v>
@@ -6620,7 +6643,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B54" s="6">
         <v>1</v>
@@ -6628,7 +6651,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B55" s="6">
         <v>1</v>
@@ -6636,7 +6659,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B56" s="6">
         <v>1</v>
@@ -6644,7 +6667,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B57" s="6">
         <v>71</v>

</xml_diff>

<commit_message>
Updated references with new IPM papers
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@688 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27320" yWindow="-5900" windowWidth="28000" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="219">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -514,9 +514,6 @@
     <t>Salguero-Gomez &amp; Plotkin</t>
   </si>
   <si>
-    <t>Salguero-Gomez R, Siewert W, Casper BB &amp; Tielbörger K (Accepted) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B</t>
-  </si>
-  <si>
     <t>Shelton AO (2010) The ecological and evolutionary drivers of female-biased sex ratios: two-sex models of perennial seagrasses. The American Naturalist 175: 302-315</t>
   </si>
   <si>
@@ -577,9 +574,6 @@
     <t>Vindenes &amp;, Sæther B-E &amp; Engen S (In press) Effects of demographic structure on key properties of stochastic density-independent population dynamics</t>
   </si>
   <si>
-    <t>Just mention IPMs as future steps</t>
-  </si>
-  <si>
     <t>Ecol Monogr</t>
   </si>
   <si>
@@ -656,13 +650,73 @@
   </si>
   <si>
     <t>Ozgul A, Coulson T, Reynolds A, Cameron TC &amp; Benton TG (2012) Population responses to perturbations: the importance of trait-based analysis illustrated through a microcosm experiment. The American Naturalist 179: 582-594</t>
+  </si>
+  <si>
+    <t>In press</t>
+  </si>
+  <si>
+    <t>Salguero-Gomez R, Siewert W, Casper BB &amp; Tielbörger K (In press) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B</t>
+  </si>
+  <si>
+    <t>Jongejans, Skarpass &amp; Shea</t>
+  </si>
+  <si>
+    <t>PPEES</t>
+  </si>
+  <si>
+    <t>Jongejans E, Skarpaas O &amp; Shea K (2008) Dispersal, demography and spatial population models for conservation and control management. Perspectives in Plant Ecology, Evolution and Systematics 9: 153-170</t>
+  </si>
+  <si>
+    <t>IPMs as future steps</t>
+  </si>
+  <si>
+    <t>Shefferson &amp; Roach</t>
+  </si>
+  <si>
+    <t>Ecol</t>
+  </si>
+  <si>
+    <t>Plantago lanceolata</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shefferson R &amp; Roach D (2012) The triple helix of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Plantago lanceolata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: genetics and the environment interact to determine population dynamics. Ecology 4: 793-802</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -737,280 +791,290 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="269">
+  <cellStyleXfs count="279">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1022,12 +1086,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="269">
+  <cellStyles count="279">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1162,6 +1226,11 @@
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1296,6 +1365,11 @@
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1450,11 +1524,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="572708568"/>
-        <c:axId val="572715480"/>
+        <c:axId val="-2038828904"/>
+        <c:axId val="2082447736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="572708568"/>
+        <c:axId val="-2038828904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,14 +1550,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="572715480"/>
+        <c:crossAx val="2082447736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1491,7 +1564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572715480"/>
+        <c:axId val="2082447736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1513,14 +1586,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="572708568"/>
+        <c:crossAx val="-2038828904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2290,7 +2362,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:B59" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -2547,7 +2619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BI19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -3190,13 +3262,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3243,7 +3315,7 @@
         <v>2010</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>3</v>
@@ -3263,7 +3335,7 @@
         <v>2010</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1</v>
@@ -3283,7 +3355,7 @@
         <v>2010</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>2</v>
@@ -3303,7 +3375,7 @@
         <v>2010</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>82</v>
@@ -3314,7 +3386,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -3323,18 +3395,18 @@
         <v>2012</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -3343,18 +3415,18 @@
         <v>2012</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -3363,18 +3435,18 @@
         <v>2012</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -3383,13 +3455,13 @@
         <v>2012</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3403,7 +3475,7 @@
         <v>2010</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>13</v>
@@ -3417,7 +3489,7 @@
         <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C11">
         <v>2011</v>
@@ -3452,7 +3524,7 @@
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3460,13 +3532,13 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C13">
         <v>2003</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>15</v>
@@ -3480,13 +3552,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C14">
         <v>2004</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>15</v>
@@ -3500,7 +3572,7 @@
         <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15">
         <v>2011</v>
@@ -3537,122 +3609,122 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>2011</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19">
         <v>2011</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>133</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="C20">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>188</v>
       </c>
       <c r="C21">
         <v>2011</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C22">
         <v>2011</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3660,13 +3732,13 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C23">
         <v>2009</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>98</v>
@@ -3680,13 +3752,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C24">
         <v>2000</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>23</v>
@@ -3706,7 +3778,7 @@
         <v>2006</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>24</v>
@@ -3726,7 +3798,7 @@
         <v>2007</v>
       </c>
       <c r="D26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>24</v>
@@ -3737,27 +3809,27 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27">
         <v>2012</v>
       </c>
       <c r="D27" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -3766,13 +3838,13 @@
         <v>2011</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3780,13 +3852,13 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C29">
         <v>2002</v>
       </c>
       <c r="D29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>30</v>
@@ -3800,13 +3872,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C30">
         <v>2010</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>31</v>
@@ -3820,7 +3892,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -3829,7 +3901,7 @@
         <v>2008</v>
       </c>
       <c r="D31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>33</v>
@@ -3852,7 +3924,7 @@
         <v>2010</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>36</v>
@@ -3878,7 +3950,7 @@
         <v>120</v>
       </c>
       <c r="F33" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="G33" t="s">
         <v>142</v>
@@ -3889,13 +3961,13 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C34">
         <v>2011</v>
       </c>
       <c r="D34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>37</v>
@@ -3906,142 +3978,145 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>212</v>
       </c>
       <c r="C35">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>173</v>
+        <v>120</v>
+      </c>
+      <c r="F35" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>190</v>
+        <v>97</v>
       </c>
       <c r="C36">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D36" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G36" t="s">
-        <v>144</v>
+      <c r="G36" s="11" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="C37">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="D37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>19</v>
       </c>
       <c r="C38">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="C39">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="G39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="C40">
         <v>2009</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>78</v>
       </c>
       <c r="C41">
         <v>2009</v>
       </c>
       <c r="D41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G41" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -4049,16 +4124,16 @@
         <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G42" t="s">
         <v>148</v>
@@ -4069,16 +4144,16 @@
         <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
         <v>148</v>
@@ -4089,16 +4164,16 @@
         <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C44">
         <v>2009</v>
       </c>
       <c r="D44" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G44" t="s">
         <v>148</v>
@@ -4109,16 +4184,16 @@
         <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C45">
         <v>2009</v>
       </c>
       <c r="D45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G45" t="s">
         <v>148</v>
@@ -4129,16 +4204,16 @@
         <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C46">
         <v>2009</v>
       </c>
       <c r="D46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
         <v>148</v>
@@ -4149,16 +4224,16 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C47">
         <v>2009</v>
       </c>
       <c r="D47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G47" t="s">
         <v>148</v>
@@ -4169,16 +4244,16 @@
         <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C48">
         <v>2009</v>
       </c>
       <c r="D48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G48" t="s">
         <v>148</v>
@@ -4189,16 +4264,16 @@
         <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C49">
         <v>2009</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G49" t="s">
         <v>148</v>
@@ -4209,16 +4284,16 @@
         <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C50">
         <v>2009</v>
       </c>
       <c r="D50" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G50" t="s">
         <v>148</v>
@@ -4226,182 +4301,182 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>188</v>
       </c>
       <c r="C51">
         <v>2009</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="G51" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>115</v>
       </c>
       <c r="C52">
         <v>2009</v>
       </c>
       <c r="D52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G52" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C53">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D53" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G53" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C54">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="D54" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G54" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>186</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C55">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D55" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>193</v>
+        <v>44</v>
+      </c>
+      <c r="G55" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="C56">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D56" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G56" t="s">
-        <v>154</v>
+        <v>36</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>2010</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>79</v>
+        <v>2011</v>
+      </c>
+      <c r="D57" t="s">
+        <v>200</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="G57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C58">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>209</v>
+        <v>48</v>
       </c>
       <c r="G58" t="s">
-        <v>210</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C59">
-        <v>2009</v>
-      </c>
-      <c r="D59" t="s">
-        <v>202</v>
+        <v>2012</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>51</v>
+        <v>207</v>
       </c>
       <c r="G59" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -4415,10 +4490,10 @@
         <v>2009</v>
       </c>
       <c r="D60" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G60" t="s">
         <v>156</v>
@@ -4426,82 +4501,82 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>50</v>
       </c>
       <c r="C61">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D61" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="G61" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C62">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C63">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>189</v>
       </c>
       <c r="C64">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="D64" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>180</v>
+        <v>30</v>
+      </c>
+      <c r="G64" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -4515,104 +4590,101 @@
         <v>2006</v>
       </c>
       <c r="D65" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B66" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="C66">
-        <v>2009</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F66" t="s">
-        <v>121</v>
+        <v>2006</v>
+      </c>
+      <c r="D66" t="s">
+        <v>200</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
       <c r="C67">
-        <v>2005</v>
-      </c>
-      <c r="D67" t="s">
-        <v>202</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>13</v>
+        <v>2009</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" t="s">
+        <v>121</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
-      </c>
-      <c r="C68" t="s">
-        <v>161</v>
+        <v>188</v>
+      </c>
+      <c r="C68">
+        <v>2005</v>
       </c>
       <c r="D68" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69">
-        <v>2010</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F69" t="s">
-        <v>121</v>
+        <v>185</v>
+      </c>
+      <c r="C69" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" t="s">
+        <v>200</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>162</v>
       </c>
       <c r="B70" t="s">
         <v>26</v>
@@ -4620,105 +4692,105 @@
       <c r="C70">
         <v>2010</v>
       </c>
-      <c r="D70" t="s">
-        <v>202</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>58</v>
+      <c r="D70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F70" t="s">
+        <v>121</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>216</v>
       </c>
       <c r="C71">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>59</v>
+        <v>217</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>164</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C72">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>26</v>
       </c>
       <c r="C73">
-        <v>2012</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F73" t="s">
-        <v>121</v>
-      </c>
-      <c r="G73" t="s">
-        <v>177</v>
+        <v>2010</v>
+      </c>
+      <c r="D73" t="s">
+        <v>200</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>190</v>
+        <v>19</v>
       </c>
       <c r="C74">
-        <v>2011</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>120</v>
+        <v>2005</v>
+      </c>
+      <c r="D74" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C75">
         <v>2012</v>
@@ -4729,19 +4801,22 @@
       <c r="E75" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G75" s="11" t="s">
-        <v>183</v>
+      <c r="F75" t="s">
+        <v>121</v>
+      </c>
+      <c r="G75" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B76" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C76">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>120</v>
@@ -4750,107 +4825,107 @@
         <v>120</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="C77">
-        <v>2009</v>
-      </c>
-      <c r="D77" t="s">
-        <v>202</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>64</v>
+        <v>2012</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="B78" t="s">
         <v>190</v>
       </c>
       <c r="C78">
-        <v>2006</v>
-      </c>
-      <c r="D78" t="s">
-        <v>202</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>65</v>
+        <v>2012</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B79" t="s">
-        <v>190</v>
+        <v>26</v>
       </c>
       <c r="C79">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D79" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>64</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="C80">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D80" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="C81">
         <v>2010</v>
       </c>
       <c r="D81" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -4864,13 +4939,13 @@
         <v>2010</v>
       </c>
       <c r="D82" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -4884,13 +4959,13 @@
         <v>2010</v>
       </c>
       <c r="D83" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -4904,13 +4979,13 @@
         <v>2010</v>
       </c>
       <c r="D84" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -4924,13 +4999,53 @@
         <v>2010</v>
       </c>
       <c r="D85" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E85" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86">
+        <v>2010</v>
+      </c>
+      <c r="D86" t="s">
+        <v>200</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>68</v>
+      </c>
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87">
+        <v>2010</v>
+      </c>
+      <c r="D87" t="s">
+        <v>200</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G85" s="11" t="s">
-        <v>170</v>
+      <c r="G87" s="11" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4951,7 +5066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BI59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -5193,13 +5308,13 @@
         <v>117</v>
       </c>
       <c r="BF4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BG4" t="s">
         <v>120</v>
       </c>
       <c r="BH4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="BI4" t="s">
         <v>92</v>
@@ -6860,7 +6975,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B56" s="6">
         <v>1</v>
@@ -6876,7 +6991,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B58" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Rob messing up with Hyper and Crypta
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@713 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="-5900" windowWidth="28000" windowHeight="21000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27320" yWindow="-5900" windowWidth="28000" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId3"/>
+    <pivotCache cacheId="20" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1564,11 +1564,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2079698680"/>
-        <c:axId val="-2079692184"/>
+        <c:axId val="-2078826648"/>
+        <c:axId val="-2104585288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079698680"/>
+        <c:axId val="-2078826648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2079692184"/>
+        <c:crossAx val="-2104585288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1605,7 +1605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079692184"/>
+        <c:axId val="-2104585288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2079698680"/>
+        <c:crossAx val="-2078826648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2448,7 +2448,275 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:B62" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="61">
+        <item x="12"/>
+        <item x="9"/>
+        <item x="48"/>
+        <item x="50"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="51"/>
+        <item x="23"/>
+        <item m="1" x="57"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="47"/>
+        <item x="52"/>
+        <item x="46"/>
+        <item x="37"/>
+        <item x="5"/>
+        <item m="1" x="58"/>
+        <item x="2"/>
+        <item x="53"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="36"/>
+        <item x="19"/>
+        <item x="6"/>
+        <item x="54"/>
+        <item x="45"/>
+        <item x="44"/>
+        <item x="22"/>
+        <item x="55"/>
+        <item x="43"/>
+        <item x="3"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item m="1" x="59"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="56"/>
+        <item x="11"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="20"/>
+        <item x="39"/>
+        <item x="14"/>
+        <item x="49"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="58">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BL19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -2767,274 +3035,6 @@
     <i t="grand">
       <x/>
     </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B62" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="61">
-        <item x="12"/>
-        <item x="9"/>
-        <item x="48"/>
-        <item x="50"/>
-        <item x="25"/>
-        <item x="24"/>
-        <item x="0"/>
-        <item x="10"/>
-        <item x="51"/>
-        <item x="23"/>
-        <item m="1" x="57"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="47"/>
-        <item x="52"/>
-        <item x="46"/>
-        <item x="37"/>
-        <item x="5"/>
-        <item m="1" x="58"/>
-        <item x="2"/>
-        <item x="53"/>
-        <item x="38"/>
-        <item x="16"/>
-        <item x="13"/>
-        <item x="36"/>
-        <item x="19"/>
-        <item x="6"/>
-        <item x="54"/>
-        <item x="45"/>
-        <item x="44"/>
-        <item x="22"/>
-        <item x="55"/>
-        <item x="43"/>
-        <item x="3"/>
-        <item x="41"/>
-        <item x="1"/>
-        <item m="1" x="59"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="56"/>
-        <item x="11"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="20"/>
-        <item x="39"/>
-        <item x="14"/>
-        <item x="49"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="58">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -3372,11 +3372,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A85" sqref="A85:D85"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5254,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BL62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated latest paper on crocos
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@932 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15075" windowHeight="12465" tabRatio="500"/>
+    <workbookView xWindow="13660" yWindow="0" windowWidth="13660" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
-    <sheet name="Species count" sheetId="2" r:id="rId2"/>
+    <sheet name="Species statistics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="12" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="232">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -719,6 +718,30 @@
   </si>
   <si>
     <t>Williams JL, Miller TX &amp; Ellner SP (In press) Avoiding unintentional eviction from integral projection models. Ecology x: xxx-xxx</t>
+  </si>
+  <si>
+    <t>Eager, Rebarber &amp; Tenhumberg</t>
+  </si>
+  <si>
+    <t>Theor Ecol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eager EA, Rebarber R &amp; Tenhumberg B (2012) Choice of density-dependence seedling recruitment function affects predicted transient dynamics: a case study with Platte thistle.  Theoretical Ecology </t>
+  </si>
+  <si>
+    <t>Coulson</t>
+  </si>
+  <si>
+    <t>Coulson T (2012) Integral projection models, their construction and use in posing hypotheses in ecology. Oikos 121: 1337-1350</t>
+  </si>
+  <si>
+    <t>Wallace, Leslie &amp; Coulson</t>
+  </si>
+  <si>
+    <t>Crocodylus niloticus</t>
+  </si>
+  <si>
+    <t>Wallace W, Leslie A &amp; Coulson T. 2012. Re-evaluating the effect of harvesting regimes on Nile crocodiles using an integral projection models. In press</t>
   </si>
 </sst>
 </file>
@@ -800,8 +823,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="291">
+  <cellStyleXfs count="297">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1112,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="291">
+  <cellStyles count="297">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1258,6 +1287,9 @@
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1403,6 +1435,9 @@
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1418,7 +1453,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1476,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Species count'!$G$23</c:f>
+              <c:f>'Species statistics'!$G$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1453,7 +1488,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Species count'!$F$24:$F$37</c:f>
+              <c:f>'Species statistics'!$F$24:$F$37</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1503,51 +1538,51 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Species count'!$G$24:$G$37</c:f>
+              <c:f>'Species statistics'!$G$24:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1562,11 +1597,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="5767936"/>
-        <c:axId val="5769856"/>
+        <c:axId val="2063684232"/>
+        <c:axId val="2062696792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5767936"/>
+        <c:axId val="2063684232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,13 +1623,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5769856"/>
+        <c:crossAx val="2062696792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1602,7 +1638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5769856"/>
+        <c:axId val="2062696792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1624,13 +1660,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5767936"/>
+        <c:crossAx val="2063684232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1654,7 +1691,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1696,7 +1733,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41123.389869791667" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="91">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41170.522934953704" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="94">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="Original reference list"/>
   </cacheSource>
@@ -1729,7 +1766,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Species" numFmtId="0">
-      <sharedItems containsBlank="1" count="60">
+      <sharedItems containsBlank="1" count="61">
         <s v="Artemisia tripartita"/>
         <s v="Pseudoroegneria spicata"/>
         <s v="Hesperostipa comata"/>
@@ -1777,6 +1814,7 @@
         <s v="Phylospadix serrulatus"/>
         <s v="Phylospadix scouleri"/>
         <s v="Digitalis purpurea"/>
+        <s v="Crocodylus niloticus"/>
         <s v="Cynoglossum officinale"/>
         <s v="Anemone patens"/>
         <s v="Agrostics hyemalis"/>
@@ -1802,7 +1840,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="91">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="94">
   <r>
     <s v="Adler, Ellner &amp; Levine"/>
     <s v="Ecol Lett"/>
@@ -1895,6 +1933,13 @@
     <x v="7"/>
   </r>
   <r>
+    <s v="Coulson"/>
+    <s v="Oikos"/>
+    <x v="1"/>
+    <s v="Animalia"/>
+    <x v="6"/>
+  </r>
+  <r>
     <s v="Coulson, MacNulty, Stahler, von Holdt, Wayne &amp; Smith"/>
     <s v="Science"/>
     <x v="2"/>
@@ -1924,42 +1969,49 @@
   </r>
   <r>
     <s v="Dahlgren, García &amp; Ehrlén"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="2"/>
     <s v="Plantae"/>
     <x v="10"/>
   </r>
   <r>
     <s v="Dalgleish, Koons, Hooten, Moffet &amp; Adler"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="2"/>
     <s v="Plantae"/>
     <x v="1"/>
   </r>
   <r>
     <s v="Dalgleish, Koons, Hooten, Moffet &amp; Adler"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="2"/>
     <s v="Plantae"/>
     <x v="2"/>
   </r>
   <r>
     <s v="Dalgleish, Koons, Hooten, Moffet &amp; Adler"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="2"/>
     <s v="Plantae"/>
     <x v="0"/>
   </r>
   <r>
     <s v="de Valpine"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="11"/>
   </r>
   <r>
+    <s v="Eager, Rebarber &amp; Tenhumberg"/>
+    <s v="Theor Ecol"/>
+    <x v="1"/>
+    <s v="Plantae"/>
+    <x v="4"/>
+  </r>
+  <r>
     <s v="Easterling, Ellner &amp; Dixon"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="6"/>
     <s v="Plantae"/>
     <x v="12"/>
@@ -2092,70 +2144,70 @@
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="26"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="27"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="28"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="29"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="30"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="31"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="32"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="33"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="34"/>
   </r>
   <r>
     <s v="Metcalf, Horvitz, Tuljapurkar &amp; Clark"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="5"/>
     <s v="Plantae"/>
     <x v="35"/>
@@ -2295,7 +2347,7 @@
   </r>
   <r>
     <s v="Shefferson &amp; Roach"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="1"/>
     <s v="Plantae"/>
     <x v="43"/>
@@ -2350,43 +2402,50 @@
     <x v="20"/>
   </r>
   <r>
+    <s v="Wallace, Leslie &amp; Coulson"/>
+    <s v="J Anim Ecol"/>
+    <x v="1"/>
+    <s v="Animalia"/>
+    <x v="47"/>
+  </r>
+  <r>
     <s v="Williams"/>
     <s v="Am Nat"/>
     <x v="5"/>
     <s v="Plantae"/>
-    <x v="47"/>
+    <x v="48"/>
   </r>
   <r>
     <s v="Williams &amp; Crone"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="7"/>
     <s v="Plantae"/>
+    <x v="49"/>
+  </r>
+  <r>
+    <s v="Williams, Auge &amp; Maron"/>
+    <s v="Ecology"/>
+    <x v="0"/>
+    <s v="Plantae"/>
     <x v="48"/>
   </r>
   <r>
-    <s v="Williams, Auge &amp; Maron"/>
-    <s v="Ecol"/>
-    <x v="0"/>
-    <s v="Plantae"/>
-    <x v="47"/>
-  </r>
-  <r>
     <s v="Williams, Miller &amp; Ellner"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="9"/>
     <s v="Plantae"/>
+    <x v="50"/>
+  </r>
+  <r>
+    <s v="Williams, Miller &amp; Ellner"/>
+    <s v="Ecology"/>
+    <x v="9"/>
+    <s v="Plantae"/>
     <x v="49"/>
   </r>
   <r>
     <s v="Williams, Miller &amp; Ellner"/>
-    <s v="Ecol"/>
-    <x v="9"/>
-    <s v="Plantae"/>
-    <x v="48"/>
-  </r>
-  <r>
-    <s v="Williams, Miller &amp; Ellner"/>
-    <s v="Ecol"/>
+    <s v="Ecology"/>
     <x v="9"/>
     <s v="Plantae"/>
     <x v="36"/>
@@ -2396,106 +2455,106 @@
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="50"/>
+    <x v="51"/>
   </r>
   <r>
     <s v="Zuidema, Jongejans, Chien, During &amp; Schieving"/>
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="51"/>
+    <x v="52"/>
   </r>
   <r>
     <s v="Zuidema, Jongejans, Chien, During &amp; Schieving"/>
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="52"/>
+    <x v="53"/>
   </r>
   <r>
     <s v="Zuidema, Jongejans, Chien, During &amp; Schieving"/>
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="53"/>
+    <x v="54"/>
   </r>
   <r>
     <s v="Zuidema, Jongejans, Chien, During &amp; Schieving"/>
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="54"/>
+    <x v="55"/>
   </r>
   <r>
     <s v="Zuidema, Jongejans, Chien, During &amp; Schieving"/>
     <s v="J Ecol"/>
     <x v="0"/>
     <s v="Plantae"/>
-    <x v="55"/>
+    <x v="56"/>
   </r>
   <r>
     <m/>
     <m/>
     <x v="13"/>
     <m/>
-    <x v="56"/>
+    <x v="57"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B62" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:B63" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="61">
+      <items count="62">
         <item x="12"/>
         <item x="9"/>
-        <item x="48"/>
-        <item x="50"/>
+        <item x="49"/>
+        <item x="51"/>
         <item x="25"/>
         <item x="24"/>
         <item x="0"/>
         <item x="10"/>
-        <item x="51"/>
+        <item x="52"/>
         <item x="23"/>
-        <item m="1" x="57"/>
+        <item m="1" x="58"/>
         <item x="21"/>
         <item x="7"/>
         <item x="4"/>
         <item x="40"/>
         <item x="42"/>
-        <item x="47"/>
-        <item x="52"/>
+        <item x="48"/>
+        <item x="53"/>
         <item x="46"/>
         <item x="37"/>
         <item x="5"/>
-        <item m="1" x="58"/>
+        <item m="1" x="59"/>
         <item x="2"/>
-        <item x="53"/>
+        <item x="54"/>
         <item x="38"/>
         <item x="16"/>
         <item x="13"/>
         <item x="36"/>
         <item x="19"/>
         <item x="6"/>
-        <item x="54"/>
+        <item x="55"/>
         <item x="45"/>
         <item x="44"/>
         <item x="22"/>
-        <item x="55"/>
+        <item x="56"/>
         <item x="43"/>
         <item x="3"/>
         <item x="41"/>
         <item x="1"/>
-        <item m="1" x="59"/>
+        <item m="1" x="60"/>
         <item x="17"/>
         <item x="18"/>
-        <item x="56"/>
+        <item x="57"/>
         <item x="11"/>
         <item x="26"/>
         <item x="27"/>
@@ -2512,7 +2571,8 @@
         <item x="20"/>
         <item x="39"/>
         <item x="14"/>
-        <item x="49"/>
+        <item x="50"/>
+        <item x="47"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2520,7 +2580,7 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="58">
+  <rowItems count="59">
     <i>
       <x/>
     </i>
@@ -2691,6 +2751,9 @@
     </i>
     <i>
       <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
     </i>
     <i t="grand">
       <x/>
@@ -2712,8 +2775,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="F3:BL19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="F3:BM19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
@@ -2738,50 +2801,50 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="61">
+      <items count="62">
         <item x="12"/>
         <item x="9"/>
-        <item x="48"/>
-        <item x="50"/>
+        <item x="49"/>
+        <item x="51"/>
         <item x="25"/>
         <item x="24"/>
         <item x="0"/>
         <item x="10"/>
-        <item x="51"/>
+        <item x="52"/>
         <item x="23"/>
-        <item m="1" x="57"/>
+        <item m="1" x="58"/>
         <item x="21"/>
         <item x="7"/>
         <item x="4"/>
         <item x="40"/>
         <item x="42"/>
-        <item x="47"/>
-        <item x="52"/>
+        <item x="48"/>
+        <item x="53"/>
         <item x="46"/>
         <item x="37"/>
         <item x="5"/>
-        <item m="1" x="58"/>
+        <item m="1" x="59"/>
         <item x="2"/>
-        <item x="53"/>
+        <item x="54"/>
         <item x="38"/>
         <item x="16"/>
         <item x="13"/>
         <item x="36"/>
         <item x="19"/>
         <item x="6"/>
-        <item x="54"/>
+        <item x="55"/>
         <item x="45"/>
         <item x="44"/>
         <item x="22"/>
-        <item x="55"/>
+        <item x="56"/>
         <item x="43"/>
         <item x="3"/>
         <item x="41"/>
         <item x="1"/>
-        <item m="1" x="59"/>
+        <item m="1" x="60"/>
         <item x="17"/>
         <item x="18"/>
-        <item x="56"/>
+        <item x="57"/>
         <item x="11"/>
         <item x="26"/>
         <item x="27"/>
@@ -2798,7 +2861,8 @@
         <item x="20"/>
         <item x="39"/>
         <item x="14"/>
-        <item x="49"/>
+        <item x="50"/>
+        <item x="47"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2856,7 +2920,7 @@
   <colFields count="1">
     <field x="4"/>
   </colFields>
-  <colItems count="58">
+  <colItems count="59">
     <i>
       <x/>
     </i>
@@ -3027,6 +3091,9 @@
     </i>
     <i>
       <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
     </i>
     <i t="grand">
       <x/>
@@ -3366,26 +3433,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.875" customWidth="1"/>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3408,7 +3475,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -3428,7 +3495,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3448,7 +3515,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -3468,7 +3535,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -3488,7 +3555,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -3508,7 +3575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -3528,7 +3595,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>193</v>
       </c>
@@ -3548,7 +3615,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>193</v>
       </c>
@@ -3568,7 +3635,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3588,7 +3655,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3611,7 +3678,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -3631,7 +3698,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3651,7 +3718,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3671,75 +3738,75 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>2012</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
         <v>116</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>191</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>2011</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>2010</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>2009</v>
-      </c>
-      <c r="D17" t="s">
-        <v>199</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>202</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D18" t="s">
         <v>199</v>
@@ -3748,15 +3815,15 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>2011</v>
@@ -3765,15 +3832,15 @@
         <v>199</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
         <v>187</v>
@@ -3785,13 +3852,13 @@
         <v>199</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -3805,13 +3872,13 @@
         <v>199</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -3825,224 +3892,218 @@
         <v>199</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
         <v>187</v>
       </c>
       <c r="C23">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="D23" t="s">
         <v>199</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
       </c>
       <c r="C24">
+        <v>2009</v>
+      </c>
+      <c r="D24" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25">
+        <v>2012</v>
+      </c>
+      <c r="D25" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26">
         <v>2000</v>
       </c>
-      <c r="D24" t="s">
-        <v>199</v>
-      </c>
-      <c r="E24" s="9" t="s">
+      <c r="D26" t="s">
+        <v>199</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <v>2006</v>
       </c>
-      <c r="D25" t="s">
-        <v>199</v>
-      </c>
-      <c r="E25" s="9" t="s">
+      <c r="D27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>27</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <v>2007</v>
       </c>
-      <c r="D26" t="s">
-        <v>199</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
         <v>217</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>185</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>208</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>218</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
         <v>195</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>196</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>2012</v>
       </c>
-      <c r="D28" t="s">
-        <v>199</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="D30" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>201</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C29">
+      <c r="C31">
         <v>2011</v>
       </c>
-      <c r="D29" t="s">
-        <v>199</v>
-      </c>
-      <c r="E29" s="9" t="s">
+      <c r="D31" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>184</v>
       </c>
-      <c r="C30">
+      <c r="C32">
         <v>2002</v>
       </c>
-      <c r="D30" t="s">
-        <v>199</v>
-      </c>
-      <c r="E30" s="9" t="s">
+      <c r="D32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G32" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>186</v>
-      </c>
-      <c r="C31">
-        <v>2010</v>
-      </c>
-      <c r="D31" t="s">
-        <v>199</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>200</v>
-      </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32">
-        <v>2008</v>
-      </c>
-      <c r="D32" t="s">
-        <v>199</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" t="s">
-        <v>19</v>
       </c>
       <c r="C33">
         <v>2010</v>
@@ -4051,204 +4112,210 @@
         <v>199</v>
       </c>
       <c r="E33" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>200</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>2008</v>
+      </c>
+      <c r="D34" t="s">
+        <v>199</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35">
+        <v>2010</v>
+      </c>
+      <c r="D35" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G35" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="36" spans="1:7">
+      <c r="A36" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="C34">
+      <c r="C36">
         <v>2012</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>120</v>
       </c>
-      <c r="E34" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" t="s">
-        <v>213</v>
-      </c>
-      <c r="G34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C35">
-        <v>2011</v>
-      </c>
-      <c r="D35" t="s">
-        <v>199</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>210</v>
-      </c>
-      <c r="B36" t="s">
-        <v>211</v>
-      </c>
-      <c r="C36">
-        <v>2008</v>
-      </c>
-      <c r="D36" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" t="s">
         <v>120</v>
       </c>
       <c r="F36" t="s">
         <v>213</v>
       </c>
       <c r="G36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C37">
+        <v>2011</v>
+      </c>
+      <c r="D37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38">
+        <v>2008</v>
+      </c>
+      <c r="D38" t="s">
+        <v>199</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" t="s">
+        <v>213</v>
+      </c>
+      <c r="G38" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
         <v>96</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>97</v>
       </c>
-      <c r="C37">
+      <c r="C39">
         <v>2012</v>
       </c>
-      <c r="D37" t="s">
-        <v>199</v>
-      </c>
-      <c r="E37" s="9" t="s">
+      <c r="D39" t="s">
+        <v>199</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>187</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <v>2010</v>
       </c>
-      <c r="D38" t="s">
-        <v>199</v>
-      </c>
-      <c r="E38" s="9" t="s">
+      <c r="D40" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G40" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>19</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>2008</v>
       </c>
-      <c r="D39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="D41" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G41" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>19</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>2011</v>
       </c>
-      <c r="D40" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="D42" t="s">
+        <v>199</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>185</v>
-      </c>
-      <c r="C41">
-        <v>2009</v>
-      </c>
-      <c r="D41" t="s">
-        <v>199</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42">
-        <v>2009</v>
-      </c>
-      <c r="D42" t="s">
-        <v>199</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>100</v>
-      </c>
-      <c r="B43" t="s">
-        <v>187</v>
       </c>
       <c r="C43">
         <v>2009</v>
@@ -4257,18 +4324,18 @@
         <v>199</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="G43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>78</v>
       </c>
       <c r="C44">
         <v>2009</v>
@@ -4277,13 +4344,13 @@
         <v>199</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -4297,13 +4364,13 @@
         <v>199</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G45" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -4317,13 +4384,13 @@
         <v>199</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G46" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -4337,13 +4404,13 @@
         <v>199</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G47" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -4357,13 +4424,13 @@
         <v>199</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G48" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -4377,13 +4444,13 @@
         <v>199</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -4397,13 +4464,13 @@
         <v>199</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G50" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -4417,13 +4484,13 @@
         <v>199</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G51" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -4437,18 +4504,18 @@
         <v>199</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G52" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="C53">
         <v>2009</v>
@@ -4457,18 +4524,18 @@
         <v>199</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="G53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C54">
         <v>2009</v>
@@ -4477,21 +4544,21 @@
         <v>199</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="G54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="C55">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D55" t="s">
         <v>199</v>
@@ -4500,15 +4567,15 @@
         <v>37</v>
       </c>
       <c r="G55" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C56">
         <v>2009</v>
@@ -4517,158 +4584,158 @@
         <v>199</v>
       </c>
       <c r="E56" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57">
+        <v>2007</v>
+      </c>
+      <c r="D57" t="s">
+        <v>199</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58">
+        <v>2009</v>
+      </c>
+      <c r="D58" t="s">
+        <v>199</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G58" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
         <v>183</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>184</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>2012</v>
       </c>
-      <c r="D57" t="s">
-        <v>199</v>
-      </c>
-      <c r="E57" s="9" t="s">
+      <c r="D59" t="s">
+        <v>199</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G59" s="12" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
         <v>75</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>19</v>
       </c>
-      <c r="C58">
+      <c r="C60">
         <v>2011</v>
       </c>
-      <c r="D58" t="s">
-        <v>199</v>
-      </c>
-      <c r="E58" s="9" t="s">
+      <c r="D60" t="s">
+        <v>199</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G60" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
         <v>46</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>47</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>2010</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E61" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G61" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
         <v>205</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>26</v>
       </c>
-      <c r="C60">
+      <c r="C62">
         <v>2012</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E62" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G62" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
         <v>49</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>50</v>
       </c>
-      <c r="C61">
+      <c r="C63">
         <v>2009</v>
       </c>
-      <c r="D61" t="s">
-        <v>199</v>
-      </c>
-      <c r="E61" s="9" t="s">
+      <c r="D63" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G63" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
         <v>49</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>50</v>
-      </c>
-      <c r="C62">
-        <v>2009</v>
-      </c>
-      <c r="D62" t="s">
-        <v>199</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" t="s">
-        <v>185</v>
-      </c>
-      <c r="C63">
-        <v>2012</v>
-      </c>
-      <c r="D63" t="s">
-        <v>199</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B64" t="s">
-        <v>182</v>
       </c>
       <c r="C64">
         <v>2009</v>
@@ -4677,41 +4744,41 @@
         <v>199</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="G64" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C65">
-        <v>2002</v>
+        <v>2012</v>
       </c>
       <c r="D65" t="s">
         <v>199</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="C66">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="D66" t="s">
         <v>199</v>
@@ -4719,139 +4786,136 @@
       <c r="E66" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>54</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67">
+        <v>2002</v>
+      </c>
+      <c r="D67" t="s">
+        <v>199</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68">
+        <v>2006</v>
+      </c>
+      <c r="D68" t="s">
+        <v>199</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>87</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>26</v>
       </c>
-      <c r="C67">
+      <c r="C69">
         <v>2006</v>
       </c>
-      <c r="D67" t="s">
-        <v>199</v>
-      </c>
-      <c r="E67" s="9" t="s">
+      <c r="D69" t="s">
+        <v>199</v>
+      </c>
+      <c r="E69" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G69" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
         <v>111</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>112</v>
       </c>
-      <c r="C68">
+      <c r="C70">
         <v>2009</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F70" t="s">
         <v>121</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="G70" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
         <v>55</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>187</v>
       </c>
-      <c r="C69">
+      <c r="C71">
         <v>2005</v>
       </c>
-      <c r="D69" t="s">
-        <v>199</v>
-      </c>
-      <c r="E69" s="9" t="s">
+      <c r="D71" t="s">
+        <v>199</v>
+      </c>
+      <c r="E71" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="G71" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
         <v>160</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>184</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>208</v>
       </c>
-      <c r="D70" t="s">
-        <v>199</v>
-      </c>
-      <c r="E70" s="9" t="s">
+      <c r="D72" t="s">
+        <v>199</v>
+      </c>
+      <c r="E72" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
         <v>161</v>
-      </c>
-      <c r="B71" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71">
-        <v>2010</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F71" t="s">
-        <v>121</v>
-      </c>
-      <c r="G71" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>214</v>
-      </c>
-      <c r="B72" t="s">
-        <v>187</v>
-      </c>
-      <c r="C72">
-        <v>2012</v>
-      </c>
-      <c r="D72" t="s">
-        <v>199</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>57</v>
       </c>
       <c r="B73" t="s">
         <v>26</v>
@@ -4859,105 +4923,105 @@
       <c r="C73">
         <v>2010</v>
       </c>
-      <c r="D73" t="s">
-        <v>199</v>
-      </c>
-      <c r="E73" s="9" t="s">
+      <c r="D73" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F73" t="s">
+        <v>121</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74">
+        <v>2012</v>
+      </c>
+      <c r="D74" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75">
+        <v>2010</v>
+      </c>
+      <c r="D75" t="s">
+        <v>199</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G73" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>57</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>26</v>
       </c>
-      <c r="C74">
+      <c r="C76">
         <v>2010</v>
       </c>
-      <c r="D74" t="s">
-        <v>199</v>
-      </c>
-      <c r="E74" s="9" t="s">
+      <c r="D76" t="s">
+        <v>199</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G76" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
         <v>60</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>19</v>
       </c>
-      <c r="C75">
+      <c r="C77">
         <v>2005</v>
       </c>
-      <c r="D75" t="s">
-        <v>199</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="D77" t="s">
+        <v>199</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G77" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
         <v>173</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>174</v>
-      </c>
-      <c r="C76">
-        <v>2012</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F76" t="s">
-        <v>121</v>
-      </c>
-      <c r="G76" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>62</v>
-      </c>
-      <c r="B77" t="s">
-        <v>187</v>
-      </c>
-      <c r="C77">
-        <v>2011</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>113</v>
-      </c>
-      <c r="B78" t="s">
-        <v>185</v>
       </c>
       <c r="C78">
         <v>2012</v>
@@ -4968,19 +5032,22 @@
       <c r="E78" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G78" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>121</v>
+      </c>
+      <c r="G78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C79">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>120</v>
@@ -4989,98 +5056,98 @@
         <v>120</v>
       </c>
       <c r="G79" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80">
+        <v>2012</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81">
+        <v>2012</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G81" s="11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>229</v>
+      </c>
+      <c r="B82" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82">
+        <v>2012</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
         <v>63</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" t="s">
         <v>26</v>
       </c>
-      <c r="C80">
+      <c r="C83">
         <v>2009</v>
       </c>
-      <c r="D80" t="s">
-        <v>199</v>
-      </c>
-      <c r="E80" s="9" t="s">
+      <c r="D83" t="s">
+        <v>199</v>
+      </c>
+      <c r="E83" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G80" s="11" t="s">
+      <c r="G83" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
         <v>66</v>
-      </c>
-      <c r="B81" t="s">
-        <v>187</v>
-      </c>
-      <c r="C81">
-        <v>2006</v>
-      </c>
-      <c r="D81" t="s">
-        <v>199</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>67</v>
-      </c>
-      <c r="B82" t="s">
-        <v>187</v>
-      </c>
-      <c r="C82">
-        <v>2010</v>
-      </c>
-      <c r="D82" t="s">
-        <v>199</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G82" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>221</v>
-      </c>
-      <c r="B83" t="s">
-        <v>187</v>
-      </c>
-      <c r="C83" t="s">
-        <v>208</v>
-      </c>
-      <c r="D83" t="s">
-        <v>199</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>221</v>
       </c>
       <c r="B84" t="s">
         <v>187</v>
       </c>
-      <c r="C84" t="s">
-        <v>208</v>
+      <c r="C84">
+        <v>2006</v>
       </c>
       <c r="D84" t="s">
         <v>199</v>
@@ -5089,90 +5156,90 @@
         <v>65</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>221</v>
+        <v>67</v>
       </c>
       <c r="B85" t="s">
         <v>187</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85">
+        <v>2010</v>
+      </c>
+      <c r="D85" t="s">
+        <v>199</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>221</v>
+      </c>
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" t="s">
         <v>208</v>
       </c>
-      <c r="D85" t="s">
-        <v>199</v>
-      </c>
-      <c r="E85" s="9" t="s">
+      <c r="D86" t="s">
+        <v>199</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>221</v>
+      </c>
+      <c r="B87" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" t="s">
+        <v>208</v>
+      </c>
+      <c r="D87" t="s">
+        <v>199</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>221</v>
+      </c>
+      <c r="B88" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" t="s">
+        <v>208</v>
+      </c>
+      <c r="D88" t="s">
+        <v>199</v>
+      </c>
+      <c r="E88" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G88" s="11" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86">
-        <v>2010</v>
-      </c>
-      <c r="D86" t="s">
-        <v>199</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G86" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>68</v>
-      </c>
-      <c r="B87" t="s">
-        <v>19</v>
-      </c>
-      <c r="C87">
-        <v>2010</v>
-      </c>
-      <c r="D87" t="s">
-        <v>199</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>68</v>
-      </c>
-      <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88">
-        <v>2010</v>
-      </c>
-      <c r="D88" t="s">
-        <v>199</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>68</v>
       </c>
@@ -5186,13 +5253,13 @@
         <v>199</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>68</v>
       </c>
@@ -5206,13 +5273,13 @@
         <v>199</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G90" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -5226,9 +5293,69 @@
         <v>199</v>
       </c>
       <c r="E91" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92">
+        <v>2010</v>
+      </c>
+      <c r="D92" t="s">
+        <v>199</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93">
+        <v>2010</v>
+      </c>
+      <c r="D93" t="s">
+        <v>199</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>68</v>
+      </c>
+      <c r="B94" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94">
+        <v>2010</v>
+      </c>
+      <c r="D94" t="s">
+        <v>199</v>
+      </c>
+      <c r="E94" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G91" s="11" t="s">
+      <c r="G94" s="11" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5248,79 +5375,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BL62"/>
+  <dimension ref="A3:BM63"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.125" customWidth="1"/>
-    <col min="35" max="35" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" customWidth="1"/>
+    <col min="35" max="35" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.125" customWidth="1"/>
+    <col min="38" max="38" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.1640625" customWidth="1"/>
     <col min="41" max="41" width="11.5" customWidth="1"/>
-    <col min="42" max="42" width="11.875" customWidth="1"/>
-    <col min="43" max="43" width="21.125" customWidth="1"/>
-    <col min="44" max="44" width="17.125" customWidth="1"/>
-    <col min="45" max="45" width="14.625" customWidth="1"/>
-    <col min="46" max="46" width="6.875" customWidth="1"/>
-    <col min="47" max="47" width="22.875" customWidth="1"/>
-    <col min="48" max="48" width="21.875" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" customWidth="1"/>
+    <col min="43" max="43" width="21.1640625" customWidth="1"/>
+    <col min="44" max="44" width="17.1640625" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" customWidth="1"/>
+    <col min="46" max="46" width="6.83203125" customWidth="1"/>
+    <col min="47" max="47" width="22.83203125" customWidth="1"/>
+    <col min="48" max="48" width="21.83203125" customWidth="1"/>
     <col min="49" max="49" width="17.5" customWidth="1"/>
-    <col min="50" max="50" width="14.875" customWidth="1"/>
-    <col min="51" max="51" width="15.625" customWidth="1"/>
-    <col min="52" max="52" width="19.375" customWidth="1"/>
-    <col min="53" max="53" width="13.125" customWidth="1"/>
-    <col min="54" max="54" width="28.875" customWidth="1"/>
-    <col min="55" max="55" width="13.375" customWidth="1"/>
-    <col min="56" max="56" width="18.375" customWidth="1"/>
-    <col min="57" max="57" width="22.125" customWidth="1"/>
-    <col min="58" max="58" width="10.375" customWidth="1"/>
-    <col min="59" max="59" width="18.625" customWidth="1"/>
-    <col min="60" max="60" width="3.625" customWidth="1"/>
-    <col min="61" max="61" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.83203125" customWidth="1"/>
+    <col min="51" max="51" width="15.6640625" customWidth="1"/>
+    <col min="52" max="52" width="19.33203125" customWidth="1"/>
+    <col min="53" max="53" width="13.1640625" customWidth="1"/>
+    <col min="54" max="54" width="28.83203125" customWidth="1"/>
+    <col min="55" max="55" width="13.33203125" customWidth="1"/>
+    <col min="56" max="56" width="18.33203125" customWidth="1"/>
+    <col min="57" max="57" width="22.1640625" customWidth="1"/>
+    <col min="58" max="58" width="10.33203125" customWidth="1"/>
+    <col min="59" max="59" width="18.6640625" customWidth="1"/>
+    <col min="60" max="60" width="3.6640625" customWidth="1"/>
+    <col min="61" max="61" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="17" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
@@ -5331,7 +5459,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65">
       <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
@@ -5513,10 +5641,13 @@
         <v>222</v>
       </c>
       <c r="BL4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BM4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -5585,11 +5716,12 @@
       <c r="BI5" s="6"/>
       <c r="BJ5" s="6"/>
       <c r="BK5" s="6"/>
-      <c r="BL5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BL5" s="6"/>
+      <c r="BM5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -5658,11 +5790,12 @@
       <c r="BI6" s="6"/>
       <c r="BJ6" s="6"/>
       <c r="BK6" s="6"/>
-      <c r="BL6" s="6">
+      <c r="BL6" s="6"/>
+      <c r="BM6" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -5731,11 +5864,12 @@
       <c r="BI7" s="6"/>
       <c r="BJ7" s="6"/>
       <c r="BK7" s="6"/>
-      <c r="BL7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BL7" s="6"/>
+      <c r="BM7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65">
       <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
@@ -5804,11 +5938,12 @@
       <c r="BI8" s="6"/>
       <c r="BJ8" s="6"/>
       <c r="BK8" s="6"/>
-      <c r="BL8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BL8" s="6"/>
+      <c r="BM8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65">
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
@@ -5879,11 +6014,12 @@
       <c r="BI9" s="6"/>
       <c r="BJ9" s="6"/>
       <c r="BK9" s="6"/>
-      <c r="BL9" s="6">
+      <c r="BL9" s="6"/>
+      <c r="BM9" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -5958,11 +6094,12 @@
       <c r="BI10" s="6"/>
       <c r="BJ10" s="6"/>
       <c r="BK10" s="6"/>
-      <c r="BL10" s="6">
+      <c r="BL10" s="6"/>
+      <c r="BM10" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -6033,11 +6170,12 @@
       <c r="BI11" s="6"/>
       <c r="BJ11" s="6"/>
       <c r="BK11" s="6"/>
-      <c r="BL11" s="6">
+      <c r="BL11" s="6"/>
+      <c r="BM11" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -6110,11 +6248,12 @@
       <c r="BI12" s="6"/>
       <c r="BJ12" s="6"/>
       <c r="BK12" s="6"/>
-      <c r="BL12" s="6">
+      <c r="BL12" s="6"/>
+      <c r="BM12" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -6225,11 +6364,12 @@
       <c r="BI13" s="6"/>
       <c r="BJ13" s="6"/>
       <c r="BK13" s="6"/>
-      <c r="BL13" s="6">
+      <c r="BL13" s="6"/>
+      <c r="BM13" s="6">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -6336,11 +6476,12 @@
       <c r="BI14" s="6"/>
       <c r="BJ14" s="6"/>
       <c r="BK14" s="6"/>
-      <c r="BL14" s="6">
+      <c r="BL14" s="6"/>
+      <c r="BM14" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65">
       <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
@@ -6431,11 +6572,12 @@
       <c r="BI15" s="6"/>
       <c r="BJ15" s="6"/>
       <c r="BK15" s="6"/>
-      <c r="BL15" s="6">
+      <c r="BL15" s="6"/>
+      <c r="BM15" s="6">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -6460,7 +6602,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -6480,7 +6622,9 @@
       <c r="AG16" s="6">
         <v>1</v>
       </c>
-      <c r="AH16" s="6"/>
+      <c r="AH16" s="6">
+        <v>1</v>
+      </c>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
@@ -6525,15 +6669,18 @@
       <c r="BJ16" s="6"/>
       <c r="BK16" s="6"/>
       <c r="BL16" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BM16" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:65">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>91</v>
@@ -6596,8 +6743,9 @@
       <c r="BJ17" s="6"/>
       <c r="BK17" s="6"/>
       <c r="BL17" s="6"/>
-    </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BM17" s="6"/>
+    </row>
+    <row r="18" spans="1:65">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -6674,11 +6822,12 @@
       <c r="BK18" s="6">
         <v>1</v>
       </c>
-      <c r="BL18" s="6">
+      <c r="BL18" s="6"/>
+      <c r="BM18" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65">
       <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
@@ -6725,7 +6874,7 @@
         <v>4</v>
       </c>
       <c r="S19" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T19" s="6">
         <v>1</v>
@@ -6770,7 +6919,7 @@
         <v>2</v>
       </c>
       <c r="AH19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI19" s="6">
         <v>1</v>
@@ -6858,10 +7007,13 @@
         <v>1</v>
       </c>
       <c r="BL19" s="6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BM19" s="6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:65">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -6869,7 +7021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -6877,7 +7029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -6885,7 +7037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -6899,7 +7051,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65">
       <c r="A24" s="5" t="s">
         <v>81</v>
       </c>
@@ -6913,7 +7065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -6927,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65">
       <c r="A26" s="5" t="s">
         <v>72</v>
       </c>
@@ -6941,7 +7093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65">
       <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
@@ -6955,7 +7107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -6969,7 +7121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
@@ -6983,7 +7135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65">
       <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
@@ -6997,7 +7149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65">
       <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
@@ -7011,12 +7163,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="7">
         <v>2008</v>
@@ -7025,7 +7177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>73</v>
       </c>
@@ -7039,7 +7191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -7053,7 +7205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
@@ -7067,7 +7219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -7078,10 +7230,10 @@
         <v>2012</v>
       </c>
       <c r="G36" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>74</v>
       </c>
@@ -7095,7 +7247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>215</v>
       </c>
@@ -7103,7 +7255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
@@ -7111,7 +7263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>52</v>
       </c>
@@ -7120,7 +7272,7 @@
       </c>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
@@ -7129,7 +7281,7 @@
       </c>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>31</v>
       </c>
@@ -7138,7 +7290,7 @@
       </c>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>33</v>
       </c>
@@ -7147,14 +7299,14 @@
       </c>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B44" s="6"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>98</v>
       </c>
@@ -7163,7 +7315,7 @@
       </c>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
         <v>101</v>
       </c>
@@ -7172,7 +7324,7 @@
       </c>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>102</v>
       </c>
@@ -7181,7 +7333,7 @@
       </c>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>103</v>
       </c>
@@ -7190,7 +7342,7 @@
       </c>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
         <v>104</v>
       </c>
@@ -7199,7 +7351,7 @@
       </c>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
         <v>105</v>
       </c>
@@ -7208,7 +7360,7 @@
       </c>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
         <v>106</v>
       </c>
@@ -7217,7 +7369,7 @@
       </c>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="5" t="s">
         <v>107</v>
       </c>
@@ -7226,7 +7378,7 @@
       </c>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
         <v>108</v>
       </c>
@@ -7235,7 +7387,7 @@
       </c>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>109</v>
       </c>
@@ -7243,7 +7395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
         <v>110</v>
       </c>
@@ -7251,7 +7403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
         <v>117</v>
       </c>
@@ -7259,7 +7411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
         <v>197</v>
       </c>
@@ -7267,7 +7419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="5" t="s">
         <v>120</v>
       </c>
@@ -7275,7 +7427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
         <v>206</v>
       </c>
@@ -7283,7 +7435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
         <v>219</v>
       </c>
@@ -7291,7 +7443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
         <v>222</v>
       </c>
@@ -7299,12 +7451,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="6">
-        <v>90</v>
+      <c r="B63" s="6">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Messed up contour plot
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@947 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13665" yWindow="0" windowWidth="13665" windowHeight="14835" tabRatio="500"/>
+    <workbookView xWindow="27320" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="239">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -754,6 +754,15 @@
   </si>
   <si>
     <t>Metcalf CJE &amp; Pavard S (2007) Why evolutionary biologists should be demographers. Trends in Ecology and Evolution 22: 205-211</t>
+  </si>
+  <si>
+    <t>Jansen, Zuidema, Anten &amp; Martinez-Ramos</t>
+  </si>
+  <si>
+    <t>Chamaedorea elegans</t>
+  </si>
+  <si>
+    <t>Jansen M, Zuidema PA, Anten NPR &amp; Martinez-Ramos M (2012) Strong persistent growth differences govern individual performance and populaton dynamics in a tropical forest understory palm. Journal of Ecoloy 100: 1224-1232</t>
   </si>
 </sst>
 </file>
@@ -835,8 +844,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="297">
+  <cellStyleXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1153,7 +1164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="297">
+  <cellStyles count="299">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1302,6 +1313,7 @@
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1450,6 +1462,7 @@
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1465,7 +1478,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1555,46 +1568,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,11 +1622,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="48456448"/>
-        <c:axId val="48458368"/>
+        <c:axId val="2067327368"/>
+        <c:axId val="2067292328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48456448"/>
+        <c:axId val="2067327368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48458368"/>
+        <c:crossAx val="2067292328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +1662,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48458368"/>
+        <c:axId val="2067292328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,7 +1690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48456448"/>
+        <c:crossAx val="2067327368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1701,7 +1714,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2513,278 +2526,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B63" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="62">
-        <item x="12"/>
-        <item x="9"/>
-        <item x="49"/>
-        <item x="51"/>
-        <item x="25"/>
-        <item x="24"/>
-        <item x="0"/>
-        <item x="10"/>
-        <item x="52"/>
-        <item x="23"/>
-        <item m="1" x="58"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="40"/>
-        <item x="42"/>
-        <item x="48"/>
-        <item x="53"/>
-        <item x="46"/>
-        <item x="37"/>
-        <item x="5"/>
-        <item m="1" x="59"/>
-        <item x="2"/>
-        <item x="54"/>
-        <item x="38"/>
-        <item x="16"/>
-        <item x="13"/>
-        <item x="36"/>
-        <item x="19"/>
-        <item x="6"/>
-        <item x="55"/>
-        <item x="45"/>
-        <item x="44"/>
-        <item x="22"/>
-        <item x="56"/>
-        <item x="43"/>
-        <item x="3"/>
-        <item x="41"/>
-        <item x="1"/>
-        <item m="1" x="60"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="57"/>
-        <item x="11"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="20"/>
-        <item x="39"/>
-        <item x="14"/>
-        <item x="50"/>
-        <item x="47"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="59">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BM19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -3108,6 +2849,278 @@
     <i t="grand">
       <x/>
     </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:B63" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="62">
+        <item x="12"/>
+        <item x="9"/>
+        <item x="49"/>
+        <item x="51"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="52"/>
+        <item x="23"/>
+        <item m="1" x="58"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="40"/>
+        <item x="42"/>
+        <item x="48"/>
+        <item x="53"/>
+        <item x="46"/>
+        <item x="37"/>
+        <item x="5"/>
+        <item m="1" x="59"/>
+        <item x="2"/>
+        <item x="54"/>
+        <item x="38"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="36"/>
+        <item x="19"/>
+        <item x="6"/>
+        <item x="55"/>
+        <item x="45"/>
+        <item x="44"/>
+        <item x="22"/>
+        <item x="56"/>
+        <item x="43"/>
+        <item x="3"/>
+        <item x="41"/>
+        <item x="1"/>
+        <item m="1" x="60"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="57"/>
+        <item x="11"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="20"/>
+        <item x="39"/>
+        <item x="14"/>
+        <item x="50"/>
+        <item x="47"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="59">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -3443,26 +3456,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G59" sqref="G59"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.875" customWidth="1"/>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3498,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -3505,7 +3518,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3525,7 +3538,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -3545,7 +3558,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -3565,7 +3578,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -3585,7 +3598,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>191</v>
       </c>
@@ -3605,7 +3618,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -3625,7 +3638,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -3645,7 +3658,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3665,7 +3678,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3688,7 +3701,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -3708,7 +3721,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3728,7 +3741,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3748,7 +3761,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>225</v>
       </c>
@@ -3768,7 +3781,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -3788,7 +3801,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3808,7 +3821,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>200</v>
       </c>
@@ -3828,7 +3841,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>200</v>
       </c>
@@ -3848,7 +3861,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>201</v>
       </c>
@@ -3868,7 +3881,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -3888,7 +3901,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -3908,7 +3921,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3928,7 +3941,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -3948,7 +3961,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -3968,7 +3981,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3988,7 +4001,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -4008,7 +4021,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -4028,7 +4041,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -4048,7 +4061,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>193</v>
       </c>
@@ -4068,7 +4081,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>199</v>
       </c>
@@ -4088,7 +4101,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -4108,7 +4121,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4131,7 +4144,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>198</v>
       </c>
@@ -4154,7 +4167,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -4174,7 +4187,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="10" t="s">
         <v>119</v>
       </c>
@@ -4197,78 +4210,78 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37">
+        <v>2012</v>
+      </c>
+      <c r="D37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>185</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <v>2011</v>
       </c>
-      <c r="D37" t="s">
-        <v>197</v>
-      </c>
-      <c r="E37" s="9" t="s">
+      <c r="D38" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
         <v>208</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>209</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>2008</v>
       </c>
-      <c r="D38" t="s">
-        <v>197</v>
-      </c>
-      <c r="E38" s="9" t="s">
+      <c r="D39" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>211</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
         <v>96</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>2012</v>
-      </c>
-      <c r="D39" t="s">
-        <v>197</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40">
-        <v>2010</v>
       </c>
       <c r="D40" t="s">
         <v>197</v>
@@ -4276,76 +4289,76 @@
       <c r="E40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41">
+        <v>2010</v>
+      </c>
+      <c r="D41" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
         <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41">
-        <v>2008</v>
-      </c>
-      <c r="D41" t="s">
-        <v>197</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
       </c>
       <c r="C42">
+        <v>2008</v>
+      </c>
+      <c r="D42" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43">
         <v>2011</v>
       </c>
-      <c r="D42" t="s">
-        <v>197</v>
-      </c>
-      <c r="E42" s="9" t="s">
+      <c r="D43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>183</v>
-      </c>
-      <c r="C43">
-        <v>2009</v>
-      </c>
-      <c r="D43" t="s">
-        <v>197</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" t="s">
-        <v>78</v>
       </c>
       <c r="C44">
         <v>2009</v>
@@ -4354,18 +4367,18 @@
         <v>197</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="G44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>78</v>
       </c>
       <c r="C45">
         <v>2009</v>
@@ -4374,13 +4387,13 @@
         <v>197</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G45" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -4394,13 +4407,13 @@
         <v>197</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G46" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -4414,13 +4427,13 @@
         <v>197</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G47" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>100</v>
       </c>
@@ -4434,13 +4447,13 @@
         <v>197</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G48" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -4454,13 +4467,13 @@
         <v>197</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -4474,13 +4487,13 @@
         <v>197</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G50" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -4494,13 +4507,13 @@
         <v>197</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G51" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -4514,13 +4527,13 @@
         <v>197</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G52" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -4534,13 +4547,13 @@
         <v>197</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G53" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -4554,58 +4567,58 @@
         <v>197</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G54" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55">
+        <v>2009</v>
+      </c>
+      <c r="D55" t="s">
+        <v>197</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G55" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
         <v>230</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>231</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>206</v>
       </c>
-      <c r="D55" t="s">
-        <v>197</v>
-      </c>
-      <c r="E55" s="9" t="s">
+      <c r="D56" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
         <v>114</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>115</v>
-      </c>
-      <c r="C56">
-        <v>2009</v>
-      </c>
-      <c r="D56" t="s">
-        <v>197</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G56" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" t="s">
-        <v>190</v>
       </c>
       <c r="C57">
         <v>2009</v>
@@ -4614,153 +4627,153 @@
         <v>197</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G57" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="B58" t="s">
         <v>190</v>
       </c>
       <c r="C58">
+        <v>2009</v>
+      </c>
+      <c r="D58" t="s">
+        <v>197</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59">
         <v>2007</v>
       </c>
-      <c r="D58" t="s">
-        <v>197</v>
-      </c>
-      <c r="E58" s="9" t="s">
+      <c r="D59" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
         <v>45</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>180</v>
       </c>
-      <c r="C59">
+      <c r="C60">
         <v>2009</v>
       </c>
-      <c r="D59" t="s">
-        <v>197</v>
-      </c>
-      <c r="E59" s="9" t="s">
+      <c r="D60" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G60" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
         <v>181</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>182</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>2012</v>
       </c>
-      <c r="D60" t="s">
-        <v>197</v>
-      </c>
-      <c r="E60" s="9" t="s">
+      <c r="D61" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G60" s="12" t="s">
+      <c r="G61" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
         <v>75</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>19</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>2011</v>
       </c>
-      <c r="D61" t="s">
-        <v>197</v>
-      </c>
-      <c r="E61" s="9" t="s">
+      <c r="D62" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
         <v>46</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>47</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>2010</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G62" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>203</v>
-      </c>
-      <c r="B63" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63">
-        <v>2012</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E63" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64">
+        <v>2012</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>49</v>
-      </c>
-      <c r="B64" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64">
-        <v>2009</v>
-      </c>
-      <c r="D64" t="s">
-        <v>197</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G64" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -4774,93 +4787,93 @@
         <v>197</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G65" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>2009</v>
+      </c>
+      <c r="D66" t="s">
+        <v>197</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G66" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
         <v>118</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>183</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>2012</v>
       </c>
-      <c r="D66" t="s">
-        <v>197</v>
-      </c>
-      <c r="E66" s="9" t="s">
+      <c r="D67" t="s">
+        <v>197</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G67" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
         <v>53</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>180</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>2009</v>
       </c>
-      <c r="D67" t="s">
-        <v>197</v>
-      </c>
-      <c r="E67" s="9" t="s">
+      <c r="D68" t="s">
+        <v>197</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G68" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>54</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>186</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>2002</v>
       </c>
-      <c r="D68" t="s">
-        <v>197</v>
-      </c>
-      <c r="E68" s="9" t="s">
+      <c r="D69" t="s">
+        <v>197</v>
+      </c>
+      <c r="E69" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69">
-        <v>2006</v>
-      </c>
-      <c r="D69" t="s">
-        <v>197</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -4874,139 +4887,139 @@
         <v>197</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>2006</v>
+      </c>
+      <c r="D71" t="s">
+        <v>197</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
         <v>111</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>112</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>2009</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F72" t="s">
         <v>121</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
         <v>55</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>185</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>2005</v>
       </c>
-      <c r="D72" t="s">
-        <v>197</v>
-      </c>
-      <c r="E72" s="9" t="s">
+      <c r="D73" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
         <v>158</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>182</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>206</v>
       </c>
-      <c r="D73" t="s">
-        <v>197</v>
-      </c>
-      <c r="E73" s="9" t="s">
+      <c r="D74" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G73" s="11" t="s">
+      <c r="G74" s="11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>159</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>26</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>2010</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>121</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>212</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>185</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>2012</v>
       </c>
-      <c r="D75" t="s">
-        <v>197</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="D76" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="G76" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>57</v>
-      </c>
-      <c r="B76" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76">
-        <v>2010</v>
-      </c>
-      <c r="D76" t="s">
-        <v>197</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -5020,64 +5033,61 @@
         <v>197</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78">
+        <v>2010</v>
+      </c>
+      <c r="D78" t="s">
+        <v>197</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
         <v>60</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>19</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>2005</v>
       </c>
-      <c r="D78" t="s">
-        <v>197</v>
-      </c>
-      <c r="E78" s="9" t="s">
+      <c r="D79" t="s">
+        <v>197</v>
+      </c>
+      <c r="E79" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
         <v>171</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>172</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>2012</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F79" t="s">
-        <v>121</v>
-      </c>
-      <c r="G79" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>62</v>
-      </c>
-      <c r="B80" t="s">
-        <v>185</v>
-      </c>
-      <c r="C80">
-        <v>2011</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>120</v>
@@ -5085,19 +5095,22 @@
       <c r="E80" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G80" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>121</v>
+      </c>
+      <c r="G80" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C81">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>120</v>
@@ -5106,15 +5119,15 @@
         <v>120</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B82" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C82">
         <v>2012</v>
@@ -5126,110 +5139,110 @@
         <v>120</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>227</v>
+        <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>17</v>
+        <v>187</v>
       </c>
       <c r="C83">
         <v>2012</v>
       </c>
       <c r="D83" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>227</v>
+      </c>
+      <c r="B84" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84">
+        <v>2012</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E84" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="G83" s="11" t="s">
+      <c r="G84" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
         <v>63</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>26</v>
       </c>
-      <c r="C84">
+      <c r="C85">
         <v>2009</v>
       </c>
-      <c r="D84" t="s">
-        <v>197</v>
-      </c>
-      <c r="E84" s="9" t="s">
+      <c r="D85" t="s">
+        <v>197</v>
+      </c>
+      <c r="E85" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G84" s="11" t="s">
+      <c r="G85" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
         <v>66</v>
-      </c>
-      <c r="B85" t="s">
-        <v>185</v>
-      </c>
-      <c r="C85">
-        <v>2006</v>
-      </c>
-      <c r="D85" t="s">
-        <v>197</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G85" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>67</v>
       </c>
       <c r="B86" t="s">
         <v>185</v>
       </c>
       <c r="C86">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D86" t="s">
         <v>197</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
         <v>185</v>
       </c>
-      <c r="C87" t="s">
-        <v>206</v>
+      <c r="C87">
+        <v>2010</v>
       </c>
       <c r="D87" t="s">
         <v>197</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>220</v>
+        <v>64</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>219</v>
       </c>
@@ -5243,13 +5256,13 @@
         <v>197</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>65</v>
+        <v>220</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>219</v>
       </c>
@@ -5263,33 +5276,33 @@
         <v>197</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>219</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90">
-        <v>2010</v>
+        <v>185</v>
+      </c>
+      <c r="C90" t="s">
+        <v>206</v>
       </c>
       <c r="D90" t="s">
         <v>197</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -5303,13 +5316,13 @@
         <v>197</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>68</v>
       </c>
@@ -5323,13 +5336,13 @@
         <v>197</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>68</v>
       </c>
@@ -5343,13 +5356,13 @@
         <v>197</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>68</v>
       </c>
@@ -5363,13 +5376,13 @@
         <v>197</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>68</v>
       </c>
@@ -5383,14 +5396,34 @@
         <v>197</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="9"/>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96">
+        <v>2010</v>
+      </c>
+      <c r="D96" t="s">
+        <v>197</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="5:5">
+      <c r="E98" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:G75">
@@ -5414,74 +5447,74 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="5.125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.125" customWidth="1"/>
-    <col min="35" max="35" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" customWidth="1"/>
+    <col min="35" max="35" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.125" customWidth="1"/>
+    <col min="38" max="38" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.1640625" customWidth="1"/>
     <col min="41" max="41" width="11.5" customWidth="1"/>
-    <col min="42" max="42" width="11.875" customWidth="1"/>
-    <col min="43" max="43" width="21.125" customWidth="1"/>
-    <col min="44" max="44" width="17.125" customWidth="1"/>
-    <col min="45" max="45" width="14.625" customWidth="1"/>
-    <col min="46" max="46" width="6.875" customWidth="1"/>
-    <col min="47" max="47" width="22.875" customWidth="1"/>
-    <col min="48" max="48" width="21.875" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" customWidth="1"/>
+    <col min="43" max="43" width="21.1640625" customWidth="1"/>
+    <col min="44" max="44" width="17.1640625" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" customWidth="1"/>
+    <col min="46" max="46" width="6.83203125" customWidth="1"/>
+    <col min="47" max="47" width="22.83203125" customWidth="1"/>
+    <col min="48" max="48" width="21.83203125" customWidth="1"/>
     <col min="49" max="49" width="17.5" customWidth="1"/>
-    <col min="50" max="50" width="14.875" customWidth="1"/>
-    <col min="51" max="51" width="15.625" customWidth="1"/>
-    <col min="52" max="52" width="19.375" customWidth="1"/>
-    <col min="53" max="53" width="13.125" customWidth="1"/>
-    <col min="54" max="54" width="28.875" customWidth="1"/>
-    <col min="55" max="55" width="13.375" customWidth="1"/>
-    <col min="56" max="56" width="18.375" customWidth="1"/>
-    <col min="57" max="57" width="22.125" customWidth="1"/>
-    <col min="58" max="58" width="10.375" customWidth="1"/>
-    <col min="59" max="59" width="18.625" customWidth="1"/>
-    <col min="60" max="60" width="3.625" customWidth="1"/>
-    <col min="61" max="61" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.83203125" customWidth="1"/>
+    <col min="51" max="51" width="15.6640625" customWidth="1"/>
+    <col min="52" max="52" width="19.33203125" customWidth="1"/>
+    <col min="53" max="53" width="13.1640625" customWidth="1"/>
+    <col min="54" max="54" width="28.83203125" customWidth="1"/>
+    <col min="55" max="55" width="13.33203125" customWidth="1"/>
+    <col min="56" max="56" width="18.33203125" customWidth="1"/>
+    <col min="57" max="57" width="22.1640625" customWidth="1"/>
+    <col min="58" max="58" width="10.33203125" customWidth="1"/>
+    <col min="59" max="59" width="18.6640625" customWidth="1"/>
+    <col min="60" max="60" width="3.6640625" customWidth="1"/>
+    <col min="61" max="61" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="17" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
@@ -5492,7 +5525,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65">
       <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
@@ -5680,7 +5713,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:65">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -5754,7 +5787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -5828,7 +5861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -5902,7 +5935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65">
       <c r="A8" s="5" t="s">
         <v>69</v>
       </c>
@@ -5976,7 +6009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65">
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
@@ -6052,7 +6085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -6132,7 +6165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -6208,7 +6241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -6286,7 +6319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -6402,7 +6435,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -6514,7 +6547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65">
       <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
@@ -6610,7 +6643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -6708,7 +6741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
@@ -6778,7 +6811,7 @@
       <c r="BL17" s="6"/>
       <c r="BM17" s="6"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -6860,7 +6893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65">
       <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
@@ -7046,7 +7079,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -7054,7 +7087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65">
       <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
@@ -7062,7 +7095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65">
       <c r="A22" s="5" t="s">
         <v>61</v>
       </c>
@@ -7070,7 +7103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
@@ -7084,7 +7117,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65">
       <c r="A24" s="5" t="s">
         <v>81</v>
       </c>
@@ -7098,7 +7131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65">
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
@@ -7112,7 +7145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65">
       <c r="A26" s="5" t="s">
         <v>72</v>
       </c>
@@ -7126,7 +7159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65">
       <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
@@ -7140,7 +7173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -7154,7 +7187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
@@ -7168,7 +7201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65">
       <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
@@ -7182,7 +7215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65">
       <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
@@ -7196,7 +7229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
@@ -7210,7 +7243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
         <v>73</v>
       </c>
@@ -7224,7 +7257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -7238,7 +7271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
@@ -7252,7 +7285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>10</v>
       </c>
@@ -7266,7 +7299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>74</v>
       </c>
@@ -7280,7 +7313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
         <v>213</v>
       </c>
@@ -7288,7 +7321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
         <v>82</v>
       </c>
@@ -7296,7 +7329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
         <v>52</v>
       </c>
@@ -7305,7 +7338,7 @@
       </c>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
@@ -7314,7 +7347,7 @@
       </c>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
         <v>31</v>
       </c>
@@ -7323,7 +7356,7 @@
       </c>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
         <v>33</v>
       </c>
@@ -7332,14 +7365,14 @@
       </c>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B44" s="6"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
         <v>98</v>
       </c>
@@ -7348,7 +7381,7 @@
       </c>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
         <v>101</v>
       </c>
@@ -7357,7 +7390,7 @@
       </c>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>102</v>
       </c>
@@ -7366,7 +7399,7 @@
       </c>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>103</v>
       </c>
@@ -7375,7 +7408,7 @@
       </c>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
         <v>104</v>
       </c>
@@ -7384,7 +7417,7 @@
       </c>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="5" t="s">
         <v>105</v>
       </c>
@@ -7393,7 +7426,7 @@
       </c>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" s="5" t="s">
         <v>106</v>
       </c>
@@ -7402,7 +7435,7 @@
       </c>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="5" t="s">
         <v>107</v>
       </c>
@@ -7411,7 +7444,7 @@
       </c>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="5" t="s">
         <v>108</v>
       </c>
@@ -7420,7 +7453,7 @@
       </c>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="5" t="s">
         <v>109</v>
       </c>
@@ -7428,7 +7461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="5" t="s">
         <v>110</v>
       </c>
@@ -7436,7 +7469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="5" t="s">
         <v>117</v>
       </c>
@@ -7444,7 +7477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" s="5" t="s">
         <v>195</v>
       </c>
@@ -7452,7 +7485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="5" t="s">
         <v>120</v>
       </c>
@@ -7460,7 +7493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="5" t="s">
         <v>204</v>
       </c>
@@ -7468,7 +7501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
         <v>217</v>
       </c>
@@ -7476,7 +7509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
         <v>220</v>
       </c>
@@ -7484,7 +7517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="5" t="s">
         <v>228</v>
       </c>
@@ -7492,7 +7525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
Updated paging of new IPM publicaitons
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@950 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="13660" yWindow="0" windowWidth="13660" windowHeight="14840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="239">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -644,9 +644,6 @@
   </si>
   <si>
     <t>In press</t>
-  </si>
-  <si>
-    <t>Salguero-Gomez R, Siewert W, Casper BB &amp; Tielbörger K (In press) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B</t>
   </si>
   <si>
     <t>Jongejans, Skarpass &amp; Shea</t>
@@ -711,9 +708,6 @@
     <t>Agrostics hyemalis</t>
   </si>
   <si>
-    <t>Williams JL, Miller TX &amp; Ellner SP (In press) Avoiding unintentional eviction from integral projection models. Ecology x: xxx-xxx</t>
-  </si>
-  <si>
     <t>Eager, Rebarber &amp; Tenhumberg</t>
   </si>
   <si>
@@ -763,6 +757,12 @@
   </si>
   <si>
     <t>Jansen M, Zuidema PA, Anten NPR &amp; Martinez-Ramos M (2012) Strong persistent growth differences govern individual performance and populaton dynamics in a tropical forest understory palm. Journal of Ecoloy 100: 1224-1232</t>
+  </si>
+  <si>
+    <t>Salguero-Gomez R, Siewert W, Casper BB &amp; Tielbörger K (2012) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B 367: 3100-3114</t>
+  </si>
+  <si>
+    <t>Williams JL, Miller TX &amp; Ellner SP (2012) Avoiding unintentional eviction from integral projection models. Ecology 93: 2008-2014</t>
   </si>
 </sst>
 </file>
@@ -844,8 +844,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="299">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1164,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="299">
+  <cellStyles count="303">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1314,6 +1318,8 @@
     <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1463,6 +1469,8 @@
     <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1604,10 +1612,10 @@
                   <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,11 +1630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2066402088"/>
-        <c:axId val="2049025624"/>
+        <c:axId val="2116417848"/>
+        <c:axId val="2133979096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2066402088"/>
+        <c:axId val="2116417848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049025624"/>
+        <c:crossAx val="2133979096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1663,7 +1671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049025624"/>
+        <c:axId val="2133979096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,7 +1700,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066402088"/>
+        <c:crossAx val="2116417848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1758,7 +1766,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41178.958512037039" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="98">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41200.579778356485" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="98">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="Original reference list"/>
   </cacheSource>
@@ -2375,7 +2383,7 @@
   <r>
     <s v="Salguero-Gomez, Siewert, Casper &amp; Tielborger"/>
     <s v="Proc R Soc B"/>
-    <x v="9"/>
+    <x v="1"/>
     <s v="Plantae"/>
     <x v="44"/>
   </r>
@@ -2473,21 +2481,21 @@
   <r>
     <s v="Williams, Miller &amp; Ellner"/>
     <s v="Ecology"/>
-    <x v="9"/>
+    <x v="1"/>
     <s v="Plantae"/>
     <x v="52"/>
   </r>
   <r>
     <s v="Williams, Miller &amp; Ellner"/>
     <s v="Ecology"/>
-    <x v="9"/>
+    <x v="1"/>
     <s v="Plantae"/>
     <x v="51"/>
   </r>
   <r>
     <s v="Williams, Miller &amp; Ellner"/>
     <s v="Ecology"/>
-    <x v="9"/>
+    <x v="1"/>
     <s v="Plantae"/>
     <x v="38"/>
   </r>
@@ -2558,287 +2566,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:B65" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="64">
-        <item x="12"/>
-        <item x="9"/>
-        <item x="51"/>
-        <item x="53"/>
-        <item x="26"/>
-        <item x="25"/>
-        <item x="0"/>
-        <item x="10"/>
-        <item x="54"/>
-        <item x="24"/>
-        <item m="1" x="60"/>
-        <item x="22"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="42"/>
-        <item x="44"/>
-        <item x="50"/>
-        <item x="55"/>
-        <item x="48"/>
-        <item x="39"/>
-        <item x="5"/>
-        <item m="1" x="61"/>
-        <item x="2"/>
-        <item x="56"/>
-        <item x="40"/>
-        <item x="16"/>
-        <item x="13"/>
-        <item x="38"/>
-        <item x="19"/>
-        <item x="6"/>
-        <item x="57"/>
-        <item x="47"/>
-        <item x="46"/>
-        <item x="23"/>
-        <item x="58"/>
-        <item x="45"/>
-        <item x="3"/>
-        <item x="43"/>
-        <item x="1"/>
-        <item m="1" x="62"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="59"/>
-        <item x="11"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="8"/>
-        <item x="15"/>
-        <item x="20"/>
-        <item x="41"/>
-        <item x="14"/>
-        <item x="52"/>
-        <item x="49"/>
-        <item x="21"/>
-        <item x="37"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="61">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="62"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="F3:BO19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -3169,6 +2897,286 @@
     <i t="grand">
       <x/>
     </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:B65" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="64">
+        <item x="12"/>
+        <item x="9"/>
+        <item x="51"/>
+        <item x="53"/>
+        <item x="26"/>
+        <item x="25"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="54"/>
+        <item x="24"/>
+        <item m="1" x="60"/>
+        <item x="22"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="42"/>
+        <item x="44"/>
+        <item x="50"/>
+        <item x="55"/>
+        <item x="48"/>
+        <item x="39"/>
+        <item x="5"/>
+        <item m="1" x="61"/>
+        <item x="2"/>
+        <item x="56"/>
+        <item x="40"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="38"/>
+        <item x="19"/>
+        <item x="6"/>
+        <item x="57"/>
+        <item x="47"/>
+        <item x="46"/>
+        <item x="23"/>
+        <item x="58"/>
+        <item x="45"/>
+        <item x="3"/>
+        <item x="43"/>
+        <item x="1"/>
+        <item m="1" x="62"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="59"/>
+        <item x="11"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="8"/>
+        <item x="15"/>
+        <item x="20"/>
+        <item x="41"/>
+        <item x="14"/>
+        <item x="52"/>
+        <item x="49"/>
+        <item x="21"/>
+        <item x="37"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="61">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -3507,10 +3515,10 @@
   <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
+      <selection pane="bottomRight" activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3811,7 +3819,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -3826,7 +3834,7 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4011,10 +4019,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C25">
         <v>2012</v>
@@ -4026,7 +4034,7 @@
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -4091,7 +4099,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B29" t="s">
         <v>183</v>
@@ -4100,13 +4108,13 @@
         <v>206</v>
       </c>
       <c r="D29" t="s">
+        <v>215</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="G29" t="s">
         <v>217</v>
-      </c>
-      <c r="G29" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4252,7 +4260,7 @@
         <v>120</v>
       </c>
       <c r="F36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G36" t="s">
         <v>142</v>
@@ -4260,7 +4268,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
@@ -4272,10 +4280,10 @@
         <v>197</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G37" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -4300,10 +4308,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
         <v>208</v>
-      </c>
-      <c r="B39" t="s">
-        <v>209</v>
       </c>
       <c r="C39">
         <v>2008</v>
@@ -4315,10 +4323,10 @@
         <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -4643,10 +4651,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B56" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C56" t="s">
         <v>206</v>
@@ -4655,10 +4663,10 @@
         <v>197</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -4698,7 +4706,7 @@
         <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -4718,7 +4726,7 @@
         <v>37</v>
       </c>
       <c r="G59" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -5011,8 +5019,8 @@
       <c r="B74" t="s">
         <v>182</v>
       </c>
-      <c r="C74" t="s">
-        <v>206</v>
+      <c r="C74">
+        <v>2012</v>
       </c>
       <c r="D74" t="s">
         <v>197</v>
@@ -5021,7 +5029,7 @@
         <v>56</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5049,7 +5057,7 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
         <v>185</v>
@@ -5061,10 +5069,10 @@
         <v>197</v>
       </c>
       <c r="E76" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G76" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5212,7 +5220,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B84" t="s">
         <v>17</v>
@@ -5224,10 +5232,10 @@
         <v>79</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -5292,33 +5300,33 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B88" t="s">
         <v>185</v>
       </c>
-      <c r="C88" t="s">
-        <v>206</v>
+      <c r="C88">
+        <v>2012</v>
       </c>
       <c r="D88" t="s">
         <v>197</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B89" t="s">
         <v>185</v>
       </c>
-      <c r="C89" t="s">
-        <v>206</v>
+      <c r="C89">
+        <v>2012</v>
       </c>
       <c r="D89" t="s">
         <v>197</v>
@@ -5327,18 +5335,18 @@
         <v>65</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
         <v>185</v>
       </c>
-      <c r="C90" t="s">
-        <v>206</v>
+      <c r="C90">
+        <v>2012</v>
       </c>
       <c r="D90" t="s">
         <v>197</v>
@@ -5347,7 +5355,7 @@
         <v>44</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -5491,8 +5499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BO65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5684,7 +5692,7 @@
         <v>74</v>
       </c>
       <c r="AN4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AO4" t="s">
         <v>82</v>
@@ -5750,19 +5758,19 @@
         <v>204</v>
       </c>
       <c r="BJ4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BK4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BL4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BM4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BN4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BO4" t="s">
         <v>92</v>
@@ -6732,7 +6740,9 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -6748,7 +6758,9 @@
         <v>2</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
+      <c r="U16" s="6">
+        <v>1</v>
+      </c>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
@@ -6761,7 +6773,9 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
+      <c r="AF16" s="6">
+        <v>1</v>
+      </c>
       <c r="AG16" s="6">
         <v>1</v>
       </c>
@@ -6810,7 +6824,9 @@
         <v>1</v>
       </c>
       <c r="BJ16" s="6"/>
-      <c r="BK16" s="6"/>
+      <c r="BK16" s="6">
+        <v>1</v>
+      </c>
       <c r="BL16" s="6">
         <v>1</v>
       </c>
@@ -6819,7 +6835,7 @@
       </c>
       <c r="BN16" s="6"/>
       <c r="BO16" s="6">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:67">
@@ -6906,9 +6922,7 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="6">
-        <v>1</v>
-      </c>
+      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -6920,9 +6934,7 @@
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-      <c r="U18" s="6">
-        <v>1</v>
-      </c>
+      <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
@@ -6933,9 +6945,7 @@
       <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
-      <c r="AF18" s="6">
-        <v>1</v>
-      </c>
+      <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
@@ -6968,16 +6978,14 @@
       <c r="BJ18" s="6">
         <v>1</v>
       </c>
-      <c r="BK18" s="6">
-        <v>1</v>
-      </c>
+      <c r="BK18" s="6"/>
       <c r="BL18" s="6"/>
       <c r="BM18" s="6"/>
       <c r="BN18" s="6">
         <v>1</v>
       </c>
       <c r="BO18" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:67">
@@ -7389,7 +7397,7 @@
         <v>2012</v>
       </c>
       <c r="G36" s="8">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -7403,12 +7411,12 @@
         <v>206</v>
       </c>
       <c r="G37" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
@@ -7596,7 +7604,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B60" s="6">
         <v>1</v>
@@ -7604,7 +7612,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B61" s="6">
         <v>1</v>
@@ -7612,7 +7620,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B62" s="6">
         <v>1</v>
@@ -7620,7 +7628,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B63" s="6">
         <v>1</v>
@@ -7628,7 +7636,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B64" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Updated literature IPM list
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@957 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27320" yWindow="-5900" windowWidth="28000" windowHeight="21000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId3"/>
-    <pivotCache cacheId="29" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="4" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="252">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -791,6 +791,18 @@
   </si>
   <si>
     <t>Smallegange IM &amp; Coulson T (2012) Towards a general, population-level understanding of eco-evolutionary change. Trends in Ecology &amp; Evolution 1590, XXXX-XXXX</t>
+  </si>
+  <si>
+    <t>Madin, Hughes &amp; Connolly</t>
+  </si>
+  <si>
+    <t>PLoS One</t>
+  </si>
+  <si>
+    <t>Acropora hyacinthus</t>
+  </si>
+  <si>
+    <t>Madin JS, Hughes TP &amp; Connolly SR (2012) Calcification, storm damage and population resilience of tabular corals under climate change. PLoS One 7: 1-10</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1719,7 @@
                   <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2.0</c:v>
@@ -1726,12 +1738,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2117943736"/>
-        <c:axId val="2119181592"/>
+        <c:axId val="-2147008408"/>
+        <c:axId val="2109947976"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2117943736"/>
+        <c:axId val="-2147008408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,7 +1772,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119181592"/>
+        <c:crossAx val="2109947976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1768,7 +1780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119181592"/>
+        <c:axId val="2109947976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,7 +1809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117943736"/>
+        <c:crossAx val="-2147008408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1871,87 +1883,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41213.431295486109" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="101">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="E1:E1048576" sheet="Original reference list"/>
-  </cacheSource>
-  <cacheFields count="1">
-    <cacheField name="Species" numFmtId="0">
-      <sharedItems containsBlank="1" count="62">
-        <s v="Artemisia tripartita"/>
-        <s v="Pseudoroegneria spicata"/>
-        <s v="Hesperostipa comata"/>
-        <s v="Poa secunda"/>
-        <s v="Cirsium canescens"/>
-        <s v="Gorgonia ventalina"/>
-        <s v="Ovis aries"/>
-        <s v="Carlina vulgaris"/>
-        <s v="Canis lupus"/>
-        <s v="Actaea spicata"/>
-        <s v="Borderea pyrenaica"/>
-        <s v="Coryphantha robbinsorum"/>
-        <s v="Aconitum noveborancense"/>
-        <s v="Onopordum illyricum"/>
-        <s v="Lepidium latifolium"/>
-        <s v="Mammillaria gaumeri"/>
-        <s v="Oenothera glazioviana"/>
-        <s v="Mammillaria dixanthocentron"/>
-        <s v="Mammillaria hernandezii"/>
-        <s v="Vaccinium myrtillus"/>
-        <s v="Veratrum album"/>
-        <s v="Orchis purpurea"/>
-        <s v="NA"/>
-        <s v="Chamaedorea elegans"/>
-        <s v="Carduus nutans"/>
-        <s v="Phyteuma spicatum"/>
-        <s v="Campanula thyrsoides"/>
-        <s v="Artemisia ordosica"/>
-        <s v="Arabidopsis thaliana"/>
-        <s v="Penthaclethra macroloba"/>
-        <s v="Cecropia obtusifolia"/>
-        <s v="Cecropia insignis"/>
-        <s v="Simarouba amara"/>
-        <s v="Minquartia guianensis"/>
-        <s v="Balizia elegans"/>
-        <s v="Hymenolobium mesoamericanum"/>
-        <s v="Lecythis ampla"/>
-        <s v="Dipteryx panamensis"/>
-        <s v="Hyeronima alchorneoides"/>
-        <s v="Hypericum cumulicola"/>
-        <s v="Opuntia imbricata"/>
-        <s v="Dracocephalum austriacum"/>
-        <s v="Marmota flaviventris"/>
-        <s v="Sancassania berlesei"/>
-        <s v="Cirsium palustre"/>
-        <s v="Primula veris"/>
-        <s v="Cryptantha flava"/>
-        <s v="Plantago lanceolata"/>
-        <s v="Phylospadix serrulatus"/>
-        <s v="Phylospadix scouleri"/>
-        <s v="Digitalis purpurea"/>
-        <s v="Crocodylus niloticus"/>
-        <s v="Cynoglossum officinale"/>
-        <s v="Anemone patens"/>
-        <s v="Agrostics hyemalis"/>
-        <s v="Annamocarya sinensis"/>
-        <s v="Calocedrus macrolepis"/>
-        <s v="Dacrydium elatum"/>
-        <s v="Manglietia fordiana"/>
-        <s v="Parashorea chinensis"/>
-        <s v="Pinus kwangtungensis"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41213.431363773147" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="101">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="Original reference list"/>
@@ -2062,315 +1993,89 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="101">
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="19"/>
-  </r>
-  <r>
-    <x v="20"/>
-  </r>
-  <r>
-    <x v="21"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="23"/>
-  </r>
-  <r>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="25"/>
-  </r>
-  <r>
-    <x v="25"/>
-  </r>
-  <r>
-    <x v="26"/>
-  </r>
-  <r>
-    <x v="27"/>
-  </r>
-  <r>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="28"/>
-  </r>
-  <r>
-    <x v="29"/>
-  </r>
-  <r>
-    <x v="30"/>
-  </r>
-  <r>
-    <x v="31"/>
-  </r>
-  <r>
-    <x v="32"/>
-  </r>
-  <r>
-    <x v="33"/>
-  </r>
-  <r>
-    <x v="34"/>
-  </r>
-  <r>
-    <x v="35"/>
-  </r>
-  <r>
-    <x v="36"/>
-  </r>
-  <r>
-    <x v="37"/>
-  </r>
-  <r>
-    <x v="38"/>
-  </r>
-  <r>
-    <x v="39"/>
-  </r>
-  <r>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="40"/>
-  </r>
-  <r>
-    <x v="21"/>
-  </r>
-  <r>
-    <x v="41"/>
-  </r>
-  <r>
-    <x v="42"/>
-  </r>
-  <r>
-    <x v="43"/>
-  </r>
-  <r>
-    <x v="44"/>
-  </r>
-  <r>
-    <x v="45"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="46"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="47"/>
-  </r>
-  <r>
-    <x v="48"/>
-  </r>
-  <r>
-    <x v="49"/>
-  </r>
-  <r>
-    <x v="50"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="51"/>
-  </r>
-  <r>
-    <x v="52"/>
-  </r>
-  <r>
-    <x v="53"/>
-  </r>
-  <r>
-    <x v="52"/>
-  </r>
-  <r>
-    <x v="54"/>
-  </r>
-  <r>
-    <x v="53"/>
-  </r>
-  <r>
-    <x v="40"/>
-  </r>
-  <r>
-    <x v="55"/>
-  </r>
-  <r>
-    <x v="56"/>
-  </r>
-  <r>
-    <x v="57"/>
-  </r>
-  <r>
-    <x v="58"/>
-  </r>
-  <r>
-    <x v="59"/>
-  </r>
-  <r>
-    <x v="60"/>
-  </r>
-  <r>
-    <x v="61"/>
-  </r>
-  <r>
-    <x v="61"/>
-  </r>
-  <r>
-    <x v="61"/>
-  </r>
-</pivotCacheRecords>
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rob Salguero-Gomez" refreshedDate="41234.794667708331" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="102">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E1:E1048576" sheet="Original reference list"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Species" numFmtId="0">
+      <sharedItems containsBlank="1" count="63">
+        <s v="Artemisia tripartita"/>
+        <s v="Pseudoroegneria spicata"/>
+        <s v="Hesperostipa comata"/>
+        <s v="Poa secunda"/>
+        <s v="Cirsium canescens"/>
+        <s v="Gorgonia ventalina"/>
+        <s v="Ovis aries"/>
+        <s v="Carlina vulgaris"/>
+        <s v="Canis lupus"/>
+        <s v="Actaea spicata"/>
+        <s v="Borderea pyrenaica"/>
+        <s v="Coryphantha robbinsorum"/>
+        <s v="Aconitum noveborancense"/>
+        <s v="Onopordum illyricum"/>
+        <s v="Lepidium latifolium"/>
+        <s v="Mammillaria gaumeri"/>
+        <s v="Oenothera glazioviana"/>
+        <s v="Mammillaria dixanthocentron"/>
+        <s v="Mammillaria hernandezii"/>
+        <s v="Vaccinium myrtillus"/>
+        <s v="Veratrum album"/>
+        <s v="Orchis purpurea"/>
+        <s v="NA"/>
+        <s v="Chamaedorea elegans"/>
+        <s v="Carduus nutans"/>
+        <s v="Phyteuma spicatum"/>
+        <s v="Campanula thyrsoides"/>
+        <s v="Artemisia ordosica"/>
+        <s v="Acropora hyacinthus"/>
+        <s v="Arabidopsis thaliana"/>
+        <s v="Penthaclethra macroloba"/>
+        <s v="Cecropia obtusifolia"/>
+        <s v="Cecropia insignis"/>
+        <s v="Simarouba amara"/>
+        <s v="Minquartia guianensis"/>
+        <s v="Balizia elegans"/>
+        <s v="Hymenolobium mesoamericanum"/>
+        <s v="Lecythis ampla"/>
+        <s v="Dipteryx panamensis"/>
+        <s v="Hyeronima alchorneoides"/>
+        <s v="Hypericum cumulicola"/>
+        <s v="Opuntia imbricata"/>
+        <s v="Dracocephalum austriacum"/>
+        <s v="Marmota flaviventris"/>
+        <s v="Sancassania berlesei"/>
+        <s v="Cirsium palustre"/>
+        <s v="Primula veris"/>
+        <s v="Cryptantha flava"/>
+        <s v="Plantago lanceolata"/>
+        <s v="Phylospadix serrulatus"/>
+        <s v="Phylospadix scouleri"/>
+        <s v="Digitalis purpurea"/>
+        <s v="Crocodylus niloticus"/>
+        <s v="Cynoglossum officinale"/>
+        <s v="Anemone patens"/>
+        <s v="Agrostics hyemalis"/>
+        <s v="Annamocarya sinensis"/>
+        <s v="Calocedrus macrolepis"/>
+        <s v="Dacrydium elatum"/>
+        <s v="Manglietia fordiana"/>
+        <s v="Parashorea chinensis"/>
+        <s v="Pinus kwangtungensis"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="101">
   <r>
     <s v="Adler, Ellner &amp; Levine"/>
@@ -3082,8 +2787,604 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="102">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="39"/>
+  </r>
+  <r>
+    <x v="40"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="41"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="42"/>
+  </r>
+  <r>
+    <x v="43"/>
+  </r>
+  <r>
+    <x v="44"/>
+  </r>
+  <r>
+    <x v="45"/>
+  </r>
+  <r>
+    <x v="46"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="47"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="48"/>
+  </r>
+  <r>
+    <x v="49"/>
+  </r>
+  <r>
+    <x v="50"/>
+  </r>
+  <r>
+    <x v="51"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="52"/>
+  </r>
+  <r>
+    <x v="53"/>
+  </r>
+  <r>
+    <x v="54"/>
+  </r>
+  <r>
+    <x v="53"/>
+  </r>
+  <r>
+    <x v="55"/>
+  </r>
+  <r>
+    <x v="54"/>
+  </r>
+  <r>
+    <x v="41"/>
+  </r>
+  <r>
+    <x v="56"/>
+  </r>
+  <r>
+    <x v="57"/>
+  </r>
+  <r>
+    <x v="58"/>
+  </r>
+  <r>
+    <x v="59"/>
+  </r>
+  <r>
+    <x v="60"/>
+  </r>
+  <r>
+    <x v="61"/>
+  </r>
+  <r>
+    <x v="62"/>
+  </r>
+  <r>
+    <x v="62"/>
+  </r>
+  <r>
+    <x v="62"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A1:B66" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="64">
+        <item x="12"/>
+        <item x="9"/>
+        <item x="55"/>
+        <item x="54"/>
+        <item x="56"/>
+        <item x="29"/>
+        <item x="27"/>
+        <item x="0"/>
+        <item x="35"/>
+        <item x="10"/>
+        <item x="57"/>
+        <item x="26"/>
+        <item x="8"/>
+        <item x="24"/>
+        <item x="7"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="23"/>
+        <item x="4"/>
+        <item x="45"/>
+        <item x="11"/>
+        <item x="52"/>
+        <item x="47"/>
+        <item x="53"/>
+        <item x="58"/>
+        <item x="51"/>
+        <item x="38"/>
+        <item x="42"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="39"/>
+        <item x="36"/>
+        <item x="40"/>
+        <item x="37"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="15"/>
+        <item x="18"/>
+        <item x="59"/>
+        <item x="43"/>
+        <item x="34"/>
+        <item x="22"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="41"/>
+        <item x="21"/>
+        <item x="6"/>
+        <item x="60"/>
+        <item x="30"/>
+        <item x="50"/>
+        <item x="49"/>
+        <item x="25"/>
+        <item x="61"/>
+        <item x="48"/>
+        <item x="3"/>
+        <item x="46"/>
+        <item x="1"/>
+        <item x="44"/>
+        <item x="33"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="62"/>
+        <item x="28"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="64">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Species" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E3:BP19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -3425,287 +3726,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Authors" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A1:B65" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="63">
-        <item x="12"/>
-        <item x="9"/>
-        <item x="54"/>
-        <item x="53"/>
-        <item x="55"/>
-        <item x="28"/>
-        <item x="27"/>
-        <item x="0"/>
-        <item x="34"/>
-        <item x="10"/>
-        <item x="56"/>
-        <item x="26"/>
-        <item x="8"/>
-        <item x="24"/>
-        <item x="7"/>
-        <item x="31"/>
-        <item x="30"/>
-        <item x="23"/>
-        <item x="4"/>
-        <item x="44"/>
-        <item x="11"/>
-        <item x="51"/>
-        <item x="46"/>
-        <item x="52"/>
-        <item x="57"/>
-        <item x="50"/>
-        <item x="37"/>
-        <item x="41"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="38"/>
-        <item x="35"/>
-        <item x="39"/>
-        <item x="36"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="15"/>
-        <item x="18"/>
-        <item x="58"/>
-        <item x="42"/>
-        <item x="33"/>
-        <item x="22"/>
-        <item x="16"/>
-        <item x="13"/>
-        <item x="40"/>
-        <item x="21"/>
-        <item x="6"/>
-        <item x="59"/>
-        <item x="29"/>
-        <item x="49"/>
-        <item x="48"/>
-        <item x="25"/>
-        <item x="60"/>
-        <item x="47"/>
-        <item x="3"/>
-        <item x="45"/>
-        <item x="1"/>
-        <item x="43"/>
-        <item x="32"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="61"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="63">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Species" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -4041,13 +4061,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E82" sqref="E82"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5000,30 +5020,30 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>248</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>249</v>
       </c>
       <c r="C47">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>84</v>
+        <v>250</v>
       </c>
       <c r="G47" t="s">
-        <v>149</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>78</v>
       </c>
       <c r="C48">
         <v>2009</v>
@@ -5032,10 +5052,10 @@
         <v>196</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G48" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5052,7 +5072,7 @@
         <v>196</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G49" t="s">
         <v>148</v>
@@ -5072,7 +5092,7 @@
         <v>196</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G50" t="s">
         <v>148</v>
@@ -5092,7 +5112,7 @@
         <v>196</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G51" t="s">
         <v>148</v>
@@ -5112,7 +5132,7 @@
         <v>196</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G52" t="s">
         <v>148</v>
@@ -5132,7 +5152,7 @@
         <v>196</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G53" t="s">
         <v>148</v>
@@ -5152,7 +5172,7 @@
         <v>196</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G54" t="s">
         <v>148</v>
@@ -5172,7 +5192,7 @@
         <v>196</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G55" t="s">
         <v>148</v>
@@ -5192,7 +5212,7 @@
         <v>196</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G56" t="s">
         <v>148</v>
@@ -5212,7 +5232,7 @@
         <v>196</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G57" t="s">
         <v>148</v>
@@ -5220,50 +5240,50 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>227</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>228</v>
-      </c>
-      <c r="C58" t="s">
-        <v>205</v>
+        <v>185</v>
+      </c>
+      <c r="C58">
+        <v>2009</v>
       </c>
       <c r="D58" t="s">
         <v>196</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>229</v>
+        <v>110</v>
       </c>
       <c r="G58" t="s">
-        <v>230</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59">
-        <v>2009</v>
+        <v>228</v>
+      </c>
+      <c r="C59" t="s">
+        <v>205</v>
       </c>
       <c r="D59" t="s">
         <v>196</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>37</v>
+        <v>229</v>
       </c>
       <c r="G59" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="C60">
         <v>2009</v>
@@ -5272,150 +5292,150 @@
         <v>196</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G60" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
         <v>189</v>
       </c>
       <c r="C61">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D61" t="s">
         <v>196</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="C62">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="D62" t="s">
         <v>196</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G62" t="s">
-        <v>151</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C63">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D63" t="s">
         <v>196</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>238</v>
+        <v>44</v>
+      </c>
+      <c r="G63" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>181</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>182</v>
       </c>
       <c r="C64">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D64" t="s">
         <v>196</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G64" t="s">
-        <v>152</v>
+        <v>36</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C65">
-        <v>2010</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>79</v>
+        <v>2011</v>
+      </c>
+      <c r="D65" t="s">
+        <v>196</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="G65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C66">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>203</v>
+        <v>48</v>
       </c>
       <c r="G66" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>202</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C67">
-        <v>2009</v>
-      </c>
-      <c r="D67" t="s">
-        <v>196</v>
+        <v>2012</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>51</v>
+        <v>203</v>
       </c>
       <c r="G67" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5432,7 +5452,7 @@
         <v>196</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G68" t="s">
         <v>154</v>
@@ -5440,82 +5460,82 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>183</v>
+        <v>50</v>
       </c>
       <c r="C69">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D69" t="s">
         <v>196</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="G69" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C70">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D70" t="s">
         <v>196</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B71" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C71">
-        <v>2002</v>
+        <v>2009</v>
       </c>
       <c r="D71" t="s">
         <v>196</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="C72">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="D72" t="s">
         <v>196</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G72" s="11" t="s">
-        <v>176</v>
+        <v>30</v>
+      </c>
+      <c r="G72" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5532,7 +5552,7 @@
         <v>196</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>176</v>
@@ -5540,128 +5560,128 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="C74">
-        <v>2009</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F74" t="s">
-        <v>121</v>
+        <v>2006</v>
+      </c>
+      <c r="D74" t="s">
+        <v>196</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B75" t="s">
-        <v>185</v>
+        <v>112</v>
       </c>
       <c r="C75">
-        <v>2005</v>
-      </c>
-      <c r="D75" t="s">
-        <v>196</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>13</v>
+        <v>2009</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F75" t="s">
+        <v>121</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>158</v>
+        <v>55</v>
       </c>
       <c r="B76" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C76">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="D76" t="s">
         <v>196</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>236</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="C77">
-        <v>2010</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F77" t="s">
-        <v>121</v>
+        <v>2012</v>
+      </c>
+      <c r="D77" t="s">
+        <v>196</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
       <c r="B78" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C78">
-        <v>2012</v>
-      </c>
-      <c r="D78" t="s">
-        <v>196</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>211</v>
+        <v>2010</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F78" t="s">
+        <v>121</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>210</v>
       </c>
       <c r="B79" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="C79">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D79" t="s">
         <v>196</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>58</v>
+        <v>211</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>160</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5678,7 +5698,7 @@
         <v>196</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>160</v>
@@ -5686,50 +5706,50 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C81">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="D81" t="s">
         <v>196</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>245</v>
+        <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>246</v>
+        <v>19</v>
       </c>
       <c r="C82">
-        <v>2012</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>120</v>
+        <v>2005</v>
+      </c>
+      <c r="D82" t="s">
+        <v>196</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>247</v>
+        <v>175</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>171</v>
+        <v>245</v>
       </c>
       <c r="B83" t="s">
-        <v>172</v>
+        <v>246</v>
       </c>
       <c r="C83">
         <v>2012</v>
@@ -5740,22 +5760,19 @@
       <c r="E83" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F83" t="s">
-        <v>121</v>
-      </c>
-      <c r="G83" t="s">
-        <v>173</v>
+      <c r="G83" s="11" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="B84" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C84">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>120</v>
@@ -5763,19 +5780,22 @@
       <c r="E84" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G84" s="11" t="s">
-        <v>161</v>
+      <c r="F84" t="s">
+        <v>121</v>
+      </c>
+      <c r="G84" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C85">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>120</v>
@@ -5784,15 +5804,15 @@
         <v>120</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C86">
         <v>2012</v>
@@ -5804,107 +5824,107 @@
         <v>120</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>224</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>17</v>
+        <v>187</v>
       </c>
       <c r="C87">
         <v>2012</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>225</v>
+        <v>120</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>226</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="B88" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C88">
-        <v>2009</v>
-      </c>
-      <c r="D88" t="s">
-        <v>196</v>
+        <v>2012</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>64</v>
+        <v>225</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>163</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B89" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C89">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="D89" t="s">
         <v>196</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
         <v>185</v>
       </c>
       <c r="C90">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D90" t="s">
         <v>196</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="B91" t="s">
         <v>185</v>
       </c>
       <c r="C91">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D91" t="s">
         <v>196</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>218</v>
+        <v>64</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -5921,7 +5941,7 @@
         <v>196</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="G92" s="11" t="s">
         <v>237</v>
@@ -5941,7 +5961,7 @@
         <v>196</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>237</v>
@@ -5949,22 +5969,22 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>68</v>
+        <v>217</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="C94">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D94" t="s">
         <v>196</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>166</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -5981,7 +6001,7 @@
         <v>196</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G95" s="11" t="s">
         <v>166</v>
@@ -6001,7 +6021,7 @@
         <v>196</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>166</v>
@@ -6021,7 +6041,7 @@
         <v>196</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G97" s="11" t="s">
         <v>166</v>
@@ -6041,7 +6061,7 @@
         <v>196</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G98" s="11" t="s">
         <v>166</v>
@@ -6061,14 +6081,34 @@
         <v>196</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G99" s="11" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
-      <c r="E101" s="9"/>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>68</v>
+      </c>
+      <c r="B100" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100">
+        <v>2010</v>
+      </c>
+      <c r="D100" t="s">
+        <v>196</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="E102" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:G75">
@@ -6089,10 +6129,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:BP65"/>
+  <dimension ref="A1:BP66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8051,7 +8091,7 @@
         <v>2012</v>
       </c>
       <c r="F36" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -8284,10 +8324,18 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B65" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B65" s="6">
-        <v>98</v>
+      <c r="B66" s="6">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the excel publication list. not complete yet
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@1152 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="-5900" windowWidth="28000" windowHeight="21000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19005" windowHeight="11130" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
     <sheet name="Species statistics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="266">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -429,9 +430,6 @@
   </si>
   <si>
     <t>Easterling MR, Ellner SP &amp; Dixon PM (2000) Size-specific sensitivity: applying a new structured population model. Ecology 81: 694-708</t>
-  </si>
-  <si>
-    <t>Ellner SP &amp; Rees M (2006) Integral projection models for species with complex demography. The American Naturalist 167: 410-428</t>
   </si>
   <si>
     <t>Ellner SP &amp; Rees M (2007) Stochastic stable population growth in integral projection models: theory and application. Journal of Mathematical Biology 54: 227-256</t>
@@ -691,9 +689,6 @@
     <t>Ellner &amp; Schreiber</t>
   </si>
   <si>
-    <t>Planta</t>
-  </si>
-  <si>
     <t>Lepidium latifolium</t>
   </si>
   <si>
@@ -739,9 +734,6 @@
     <t>Hypericum cumulicola</t>
   </si>
   <si>
-    <t>Metcalf CJE, McMahon SM, Salguero-Gómez R &amp; Jongejans E (in press) IPMpack: an R package for Integral Projection Models. Methods in Ecology and Evolution</t>
-  </si>
-  <si>
     <t>Metcalf CJE, Rose KE &amp; Rees M (2003) Evolutionary demography of monocarpic perennials. Trends in Ecology and Evolution 18: 471-180</t>
   </si>
   <si>
@@ -803,6 +795,57 @@
   </si>
   <si>
     <t>Madin JS, Hughes TP &amp; Connolly SR (2012) Calcification, storm damage and population resilience of tabular corals under climate change. PLoS One 7: 1-10</t>
+  </si>
+  <si>
+    <t>Metcalf CJE, McMahon SM, Salguero-Gómez R &amp; Jongejans E (2013) IPMpack: an R package for Integral Projection Models. Methods in Ecology and Evolution 4: 195-200</t>
+  </si>
+  <si>
+    <t>Eager, Haridas, Pilson, Rebarber &amp; Tenhumberg</t>
+  </si>
+  <si>
+    <t>Eager EA, Haridas CV, Pilson D, Rebarber R &amp; Tenhumberg B (2013) Disturbance frequency and vertical distribution of seeds affect long-term population dynamics: a mechanistic seed bank model. American Naturalist 182: 180-190</t>
+  </si>
+  <si>
+    <t>Ellner SP &amp; Rees M (2006) Integral projection models for species with complex demography. American Naturalist 167: 410-428</t>
+  </si>
+  <si>
+    <t>Perkins, Phillips, Baskett &amp; Hastings</t>
+  </si>
+  <si>
+    <t>Rhinella marina</t>
+  </si>
+  <si>
+    <t>Urocitellus columbianus</t>
+  </si>
+  <si>
+    <t>Schindler, Neuhaus, Gaillard &amp; Coulson</t>
+  </si>
+  <si>
+    <t>Schindler S, Neuhaus P, Gaillard J-M &amp; Coulson T (2013) The influence of nonrandom mating on population growth. American Naturalist 182: 28–41</t>
+  </si>
+  <si>
+    <t>Gonzalez &amp; Martorell</t>
+  </si>
+  <si>
+    <t>Ecol Evol</t>
+  </si>
+  <si>
+    <t>González EJ &amp; Martorell C (2013) Reconstructing shifts in vital rates driven by long-term environmental change: a new demographic method based on readily available data. Ecology and Evolution 3: 2273–2284</t>
+  </si>
+  <si>
+    <t>Perkins TA, Phillips BL, Baskett ML &amp; Hastings A (2013) Evolution of dispersal and life history interact to drive accelerating spread of an invasive species. Ecology Letters 16: 1079–1087</t>
+  </si>
+  <si>
+    <t>Yule, Miller &amp; Rudgers</t>
+  </si>
+  <si>
+    <t>Agrostis hyemalis</t>
+  </si>
+  <si>
+    <t>Yule KM, Miller TEX &amp; Rudgers JA (in press) Costs, benefits, and loss of vertically transmitted symbionts affect host population dynamics. Oikos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1621,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1683,46 +1726,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,12 +1781,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2147008408"/>
-        <c:axId val="2109947976"/>
+        <c:axId val="158371840"/>
+        <c:axId val="158373760"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2147008408"/>
+        <c:axId val="158371840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,14 +1808,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109947976"/>
+        <c:crossAx val="158373760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109947976"/>
+        <c:axId val="158373760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,14 +1844,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147008408"/>
+        <c:crossAx val="158371840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1841,7 +1882,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3099,7 +3140,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A1:B66" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -3384,7 +3425,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="E3:BP19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -4061,26 +4102,26 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.875" customWidth="1"/>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4103,7 +4144,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -4114,7 +4155,7 @@
         <v>2010</v>
       </c>
       <c r="D2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>3</v>
@@ -4123,7 +4164,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -4134,7 +4175,7 @@
         <v>2010</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>1</v>
@@ -4143,7 +4184,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -4154,7 +4195,7 @@
         <v>2010</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>2</v>
@@ -4163,7 +4204,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -4174,7 +4215,7 @@
         <v>2010</v>
       </c>
       <c r="D5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>82</v>
@@ -4183,9 +4224,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -4194,18 +4235,18 @@
         <v>2012</v>
       </c>
       <c r="D6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -4214,18 +4255,18 @@
         <v>2012</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -4234,18 +4275,18 @@
         <v>2012</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -4254,16 +4295,16 @@
         <v>2012</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4274,7 +4315,7 @@
         <v>2010</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>13</v>
@@ -4283,12 +4324,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11">
         <v>2011</v>
@@ -4306,7 +4347,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -4323,21 +4364,21 @@
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13">
         <v>2003</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>15</v>
@@ -4346,18 +4387,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14">
         <v>2004</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>15</v>
@@ -4366,9 +4407,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -4383,15 +4424,15 @@
         <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16">
         <v>2011</v>
@@ -4406,7 +4447,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4426,9 +4467,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -4437,7 +4478,7 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>20</v>
@@ -4446,9 +4487,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -4457,7 +4498,7 @@
         <v>2011</v>
       </c>
       <c r="D19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>20</v>
@@ -4466,38 +4507,38 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C20">
         <v>2011</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21">
         <v>2011</v>
       </c>
       <c r="D21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>1</v>
@@ -4506,18 +4547,18 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C22">
         <v>2011</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>2</v>
@@ -4526,18 +4567,18 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23">
         <v>2011</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>3</v>
@@ -4546,1110 +4587,1107 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C24">
         <v>2009</v>
       </c>
       <c r="D24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>2013</v>
+      </c>
+      <c r="D25" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26">
+        <v>2012</v>
+      </c>
+      <c r="D26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
         <v>219</v>
       </c>
-      <c r="B25" t="s">
-        <v>220</v>
-      </c>
-      <c r="C25">
-        <v>2012</v>
-      </c>
-      <c r="D25" t="s">
-        <v>196</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B26" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26">
+      <c r="B27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27">
         <v>2000</v>
       </c>
-      <c r="D26" t="s">
-        <v>196</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D27" t="s">
+        <v>195</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27">
-        <v>2006</v>
-      </c>
-      <c r="D27" t="s">
-        <v>196</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>2007</v>
+      </c>
+      <c r="D29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C31">
+        <v>2012</v>
+      </c>
+      <c r="D31" t="s">
+        <v>195</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>2011</v>
+      </c>
+      <c r="D32" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33">
+        <v>2002</v>
+      </c>
+      <c r="D33" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>258</v>
+      </c>
+      <c r="B34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34">
+        <v>2013</v>
+      </c>
+      <c r="D34" t="s">
+        <v>195</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" t="s">
         <v>183</v>
       </c>
-      <c r="C29" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" t="s">
-        <v>214</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G29" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>192</v>
-      </c>
-      <c r="B30" t="s">
-        <v>193</v>
-      </c>
-      <c r="C30">
+      <c r="C35">
         <v>2012</v>
       </c>
-      <c r="D30" t="s">
-        <v>196</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="D35" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>198</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31">
-        <v>2011</v>
-      </c>
-      <c r="D31" t="s">
-        <v>196</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32">
-        <v>2002</v>
-      </c>
-      <c r="D32" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
+      <c r="E35" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G35" t="s">
         <v>239</v>
       </c>
-      <c r="B33" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36">
         <v>2012</v>
       </c>
-      <c r="D33" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="G33" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
+      <c r="D36" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" t="s">
         <v>239</v>
       </c>
-      <c r="B34" t="s">
-        <v>184</v>
-      </c>
-      <c r="C34">
-        <v>2012</v>
-      </c>
-      <c r="D34" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="G34" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B35" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35">
-        <v>2010</v>
-      </c>
-      <c r="D35" t="s">
-        <v>196</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>197</v>
-      </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36">
-        <v>2008</v>
-      </c>
-      <c r="D36" t="s">
-        <v>196</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>183</v>
       </c>
       <c r="C37">
         <v>2010</v>
       </c>
       <c r="D37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>196</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="10" t="s">
-        <v>119</v>
-      </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C38">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
-      </c>
-      <c r="E38" t="s">
-        <v>120</v>
-      </c>
-      <c r="F38" t="s">
-        <v>209</v>
+        <v>195</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="10" t="s">
-        <v>233</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39">
+        <v>2010</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40">
         <v>2012</v>
       </c>
-      <c r="D39" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G39" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" t="s">
+        <v>208</v>
+      </c>
+      <c r="G40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <v>2012</v>
+      </c>
+      <c r="D41" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40">
+      <c r="B42" t="s">
+        <v>184</v>
+      </c>
+      <c r="C42">
         <v>2011</v>
       </c>
-      <c r="D40" t="s">
-        <v>196</v>
-      </c>
-      <c r="E40" s="9" t="s">
+      <c r="D42" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" t="s">
+        <v>206</v>
+      </c>
+      <c r="C43">
+        <v>2008</v>
+      </c>
+      <c r="D43" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" t="s">
+        <v>208</v>
+      </c>
+      <c r="G43" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44">
+        <v>2012</v>
+      </c>
+      <c r="D44" t="s">
+        <v>195</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45">
+        <v>2010</v>
+      </c>
+      <c r="D45" t="s">
+        <v>195</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>206</v>
-      </c>
-      <c r="B41" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46">
         <v>2008</v>
       </c>
-      <c r="D41" t="s">
-        <v>196</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F41" t="s">
-        <v>209</v>
-      </c>
-      <c r="G41" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C42">
-        <v>2012</v>
-      </c>
-      <c r="D42" t="s">
-        <v>196</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" t="s">
-        <v>185</v>
-      </c>
-      <c r="C43">
-        <v>2010</v>
-      </c>
-      <c r="D43" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="D46" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
         <v>19</v>
       </c>
-      <c r="C44">
-        <v>2008</v>
-      </c>
-      <c r="D44" t="s">
-        <v>196</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="C47">
+        <v>2011</v>
+      </c>
+      <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45">
-        <v>2011</v>
-      </c>
-      <c r="D45" t="s">
-        <v>196</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B46" t="s">
-        <v>183</v>
-      </c>
-      <c r="C46">
-        <v>2009</v>
-      </c>
-      <c r="D46" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>248</v>
-      </c>
-      <c r="B47" t="s">
-        <v>249</v>
-      </c>
-      <c r="C47">
-        <v>2012</v>
-      </c>
-      <c r="D47" t="s">
-        <v>79</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="G47" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>83</v>
-      </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="C48">
         <v>2009</v>
       </c>
       <c r="D48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="G48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
-        <v>185</v>
+        <v>246</v>
       </c>
       <c r="C49">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="G49" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>2009</v>
       </c>
       <c r="D50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="G50" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C51">
         <v>2009</v>
       </c>
       <c r="D51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C52">
         <v>2009</v>
       </c>
       <c r="D52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C53">
         <v>2009</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G53" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C54">
         <v>2009</v>
       </c>
       <c r="D54" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G54" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C55">
         <v>2009</v>
       </c>
       <c r="D55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G55" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C56">
         <v>2009</v>
       </c>
       <c r="D56" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G56" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C57">
         <v>2009</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C58">
         <v>2009</v>
       </c>
       <c r="D58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>227</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>228</v>
-      </c>
-      <c r="C59" t="s">
-        <v>205</v>
+        <v>184</v>
+      </c>
+      <c r="C59">
+        <v>2009</v>
       </c>
       <c r="D59" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>229</v>
+        <v>109</v>
       </c>
       <c r="G59" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>184</v>
       </c>
       <c r="C60">
         <v>2009</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="G60" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>226</v>
       </c>
       <c r="C61">
+        <v>2013</v>
+      </c>
+      <c r="D61" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G61" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62">
         <v>2009</v>
       </c>
-      <c r="D61" t="s">
-        <v>196</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G61" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>150</v>
-      </c>
-      <c r="B62" t="s">
-        <v>189</v>
-      </c>
-      <c r="C62">
-        <v>2007</v>
-      </c>
       <c r="D62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G62" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C63">
         <v>2009</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E63" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>149</v>
+      </c>
+      <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64">
+        <v>2007</v>
+      </c>
+      <c r="D64" t="s">
+        <v>195</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65" t="s">
+        <v>179</v>
+      </c>
+      <c r="C65">
+        <v>2009</v>
+      </c>
+      <c r="D65" t="s">
+        <v>195</v>
+      </c>
+      <c r="E65" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66">
+        <v>2012</v>
+      </c>
+      <c r="D66" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67">
+        <v>2011</v>
+      </c>
+      <c r="D67" t="s">
+        <v>195</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G67" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68">
+        <v>2010</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G68" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>201</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69">
         <v>2012</v>
       </c>
-      <c r="D64" t="s">
-        <v>196</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G64" s="12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" t="s">
-        <v>75</v>
-      </c>
-      <c r="B65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65">
-        <v>2011</v>
-      </c>
-      <c r="D65" t="s">
-        <v>196</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" t="s">
-        <v>46</v>
-      </c>
-      <c r="B66" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66">
-        <v>2010</v>
-      </c>
-      <c r="D66" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E66" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G66" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" t="s">
+      <c r="E69" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B67" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67">
-        <v>2012</v>
-      </c>
-      <c r="D67" s="2" t="s">
+      <c r="G69" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70">
+        <v>2013</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="G67" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" t="s">
+      <c r="E70" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G70" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>49</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>50</v>
-      </c>
-      <c r="C68">
-        <v>2009</v>
-      </c>
-      <c r="D68" t="s">
-        <v>196</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>49</v>
-      </c>
-      <c r="B69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69">
-        <v>2009</v>
-      </c>
-      <c r="D69" t="s">
-        <v>196</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G69" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
-        <v>118</v>
-      </c>
-      <c r="B70" t="s">
-        <v>183</v>
-      </c>
-      <c r="C70">
-        <v>2012</v>
-      </c>
-      <c r="D70" t="s">
-        <v>196</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G70" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" t="s">
-        <v>180</v>
       </c>
       <c r="C71">
         <v>2009</v>
       </c>
       <c r="D71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E71" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72">
+        <v>2009</v>
+      </c>
+      <c r="D72" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>182</v>
+      </c>
+      <c r="C73">
+        <v>2012</v>
+      </c>
+      <c r="D73" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74">
+        <v>2009</v>
+      </c>
+      <c r="D74" t="s">
+        <v>195</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75">
+        <v>2002</v>
+      </c>
+      <c r="D75" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72">
-        <v>2002</v>
-      </c>
-      <c r="D72" t="s">
-        <v>196</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G72" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>87</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>26</v>
       </c>
-      <c r="C73">
+      <c r="C76">
         <v>2006</v>
       </c>
-      <c r="D73" t="s">
-        <v>196</v>
-      </c>
-      <c r="E73" s="9" t="s">
+      <c r="D76" t="s">
+        <v>195</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G73" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
+      <c r="G76" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>87</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>26</v>
       </c>
-      <c r="C74">
+      <c r="C77">
         <v>2006</v>
       </c>
-      <c r="D74" t="s">
-        <v>196</v>
-      </c>
-      <c r="E74" s="9" t="s">
+      <c r="D77" t="s">
+        <v>195</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G74" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
+      <c r="G77" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>111</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>112</v>
       </c>
-      <c r="C75">
+      <c r="C78">
         <v>2009</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F75" t="s">
-        <v>121</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" t="s">
-        <v>185</v>
-      </c>
-      <c r="C76">
-        <v>2005</v>
-      </c>
-      <c r="D76" t="s">
-        <v>196</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>158</v>
-      </c>
-      <c r="B77" t="s">
-        <v>182</v>
-      </c>
-      <c r="C77">
-        <v>2012</v>
-      </c>
-      <c r="D77" t="s">
-        <v>196</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>159</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78">
-        <v>2010</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>120</v>
@@ -5661,52 +5699,52 @@
         <v>121</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="B79" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C79">
+        <v>2005</v>
+      </c>
+      <c r="D79" t="s">
+        <v>195</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80">
         <v>2012</v>
       </c>
-      <c r="D79" t="s">
-        <v>196</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>57</v>
-      </c>
-      <c r="B80" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80">
-        <v>2010</v>
-      </c>
       <c r="D80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="B81" t="s">
         <v>26</v>
@@ -5714,125 +5752,125 @@
       <c r="C81">
         <v>2010</v>
       </c>
-      <c r="D81" t="s">
-        <v>196</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>59</v>
+      <c r="D81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F81" t="s">
+        <v>121</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="B82" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C82">
-        <v>2005</v>
-      </c>
-      <c r="D82" t="s">
-        <v>196</v>
+        <v>2013</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>61</v>
+        <v>255</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="B83" t="s">
-        <v>246</v>
+        <v>184</v>
       </c>
       <c r="C83">
         <v>2012</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>120</v>
+      <c r="D83" t="s">
+        <v>195</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="C84">
-        <v>2012</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" t="s">
-        <v>121</v>
-      </c>
-      <c r="G84" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+        <v>2010</v>
+      </c>
+      <c r="D84" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B85" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C85">
-        <v>2011</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>120</v>
+        <v>2010</v>
+      </c>
+      <c r="D85" t="s">
+        <v>195</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="B86" t="s">
-        <v>183</v>
+        <v>19</v>
       </c>
       <c r="C86">
-        <v>2012</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>120</v>
+        <v>2005</v>
+      </c>
+      <c r="D86" t="s">
+        <v>195</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>122</v>
+        <v>242</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="C87">
         <v>2012</v>
@@ -5844,250 +5882,256 @@
         <v>120</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>224</v>
+        <v>170</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="C88">
         <v>2012</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+        <v>120</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F88" t="s">
+        <v>121</v>
+      </c>
+      <c r="G88" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>184</v>
       </c>
       <c r="C89">
-        <v>2009</v>
-      </c>
-      <c r="D89" t="s">
-        <v>196</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>64</v>
+        <v>2011</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B90" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C90">
-        <v>2006</v>
-      </c>
-      <c r="D90" t="s">
-        <v>196</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>65</v>
+        <v>2012</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="B91" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C91">
-        <v>2010</v>
-      </c>
-      <c r="D91" t="s">
-        <v>196</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>64</v>
+        <v>2012</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>17</v>
       </c>
       <c r="C92">
         <v>2012</v>
       </c>
-      <c r="D92" t="s">
-        <v>196</v>
+      <c r="D92" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>217</v>
+        <v>63</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C93">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E93" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94">
+        <v>2006</v>
+      </c>
+      <c r="D94" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G93" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
-        <v>217</v>
-      </c>
-      <c r="B94" t="s">
-        <v>185</v>
-      </c>
-      <c r="C94">
-        <v>2012</v>
-      </c>
-      <c r="D94" t="s">
-        <v>196</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="G94" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B95" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="C95">
         <v>2010</v>
       </c>
       <c r="D95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="C96">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>70</v>
+        <v>216</v>
+      </c>
+      <c r="F96" t="s">
+        <v>265</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="B97" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="C97">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="B98" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="C98">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D98" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>68</v>
+        <v>262</v>
       </c>
       <c r="B99" t="s">
-        <v>19</v>
-      </c>
-      <c r="C99">
-        <v>2010</v>
+        <v>21</v>
+      </c>
+      <c r="C99" t="s">
+        <v>204</v>
       </c>
       <c r="D99" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>73</v>
+        <v>263</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>68</v>
       </c>
@@ -6098,24 +6142,124 @@
         <v>2010</v>
       </c>
       <c r="D100" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E100" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101">
+        <v>2010</v>
+      </c>
+      <c r="D101" t="s">
+        <v>195</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102">
+        <v>2010</v>
+      </c>
+      <c r="D102" t="s">
+        <v>195</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>68</v>
+      </c>
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103">
+        <v>2010</v>
+      </c>
+      <c r="D103" t="s">
+        <v>195</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G103" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B104" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104">
+        <v>2010</v>
+      </c>
+      <c r="D104" t="s">
+        <v>195</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>68</v>
+      </c>
+      <c r="B105" t="s">
+        <v>19</v>
+      </c>
+      <c r="C105">
+        <v>2010</v>
+      </c>
+      <c r="D105" t="s">
+        <v>195</v>
+      </c>
+      <c r="E105" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G100" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="E102" s="9"/>
+      <c r="G105" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:G75">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6131,86 +6275,86 @@
   </sheetPr>
   <dimension ref="A1:BP66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.875" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.125" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="19.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18.5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.1640625" customWidth="1"/>
-    <col min="34" max="34" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.125" customWidth="1"/>
+    <col min="34" max="34" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.1640625" customWidth="1"/>
+    <col min="37" max="37" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.125" customWidth="1"/>
     <col min="40" max="40" width="11.5" customWidth="1"/>
-    <col min="41" max="41" width="11.83203125" customWidth="1"/>
-    <col min="42" max="42" width="21.1640625" customWidth="1"/>
-    <col min="43" max="43" width="17.1640625" customWidth="1"/>
-    <col min="44" max="44" width="14.6640625" customWidth="1"/>
-    <col min="45" max="45" width="6.83203125" customWidth="1"/>
-    <col min="46" max="46" width="22.83203125" customWidth="1"/>
-    <col min="47" max="47" width="21.83203125" customWidth="1"/>
+    <col min="41" max="41" width="11.875" customWidth="1"/>
+    <col min="42" max="42" width="21.125" customWidth="1"/>
+    <col min="43" max="43" width="17.125" customWidth="1"/>
+    <col min="44" max="44" width="14.625" customWidth="1"/>
+    <col min="45" max="45" width="6.875" customWidth="1"/>
+    <col min="46" max="46" width="22.875" customWidth="1"/>
+    <col min="47" max="47" width="21.875" customWidth="1"/>
     <col min="48" max="48" width="17.5" customWidth="1"/>
-    <col min="49" max="49" width="14.83203125" customWidth="1"/>
-    <col min="50" max="50" width="15.6640625" customWidth="1"/>
-    <col min="51" max="51" width="19.33203125" customWidth="1"/>
-    <col min="52" max="52" width="13.1640625" customWidth="1"/>
-    <col min="53" max="53" width="28.83203125" customWidth="1"/>
-    <col min="54" max="54" width="13.33203125" customWidth="1"/>
-    <col min="55" max="55" width="18.33203125" customWidth="1"/>
-    <col min="56" max="56" width="22.1640625" customWidth="1"/>
-    <col min="57" max="57" width="10.33203125" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" customWidth="1"/>
-    <col min="59" max="59" width="3.6640625" customWidth="1"/>
-    <col min="60" max="60" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.875" customWidth="1"/>
+    <col min="50" max="50" width="15.625" customWidth="1"/>
+    <col min="51" max="51" width="19.375" customWidth="1"/>
+    <col min="52" max="52" width="13.125" customWidth="1"/>
+    <col min="53" max="53" width="28.875" customWidth="1"/>
+    <col min="54" max="54" width="13.375" customWidth="1"/>
+    <col min="55" max="55" width="18.375" customWidth="1"/>
+    <col min="56" max="56" width="22.125" customWidth="1"/>
+    <col min="57" max="57" width="10.375" customWidth="1"/>
+    <col min="58" max="58" width="18.625" customWidth="1"/>
+    <col min="59" max="59" width="3.625" customWidth="1"/>
+    <col min="60" max="60" width="17.875" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="17" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="65" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="19.375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="25.5" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:68">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>90</v>
       </c>
@@ -6218,7 +6362,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:68">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -6232,7 +6376,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:68">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -6342,7 +6486,7 @@
         <v>74</v>
       </c>
       <c r="AM4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AN4" t="s">
         <v>82</v>
@@ -6399,42 +6543,42 @@
         <v>117</v>
       </c>
       <c r="BF4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BG4" t="s">
         <v>120</v>
       </c>
       <c r="BH4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="BI4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BJ4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="BK4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="BL4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="BM4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BN4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="BO4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="BP4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:68">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -6510,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:68">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>65</v>
       </c>
@@ -6588,7 +6732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:68">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -6666,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:68">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -6744,7 +6888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:68">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -6824,7 +6968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:68">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -6908,7 +7052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:68">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>106</v>
       </c>
@@ -6988,7 +7132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:68">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7070,7 +7214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:68">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -7190,7 +7334,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:68">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -7306,7 +7450,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:68">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>117</v>
       </c>
@@ -7406,7 +7550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:68">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -7522,7 +7666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:68">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -7596,7 +7740,7 @@
       <c r="BO17" s="6"/>
       <c r="BP17" s="6"/>
     </row>
-    <row r="18" spans="1:68">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>103</v>
       </c>
@@ -7604,7 +7748,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -7676,7 +7820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:68">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>102</v>
       </c>
@@ -7874,15 +8018,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:68">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:68">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -7890,7 +8034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:68">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -7898,7 +8042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:68">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>98</v>
       </c>
@@ -7906,15 +8050,15 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:68">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B24" s="6">
         <v>1</v>
@@ -7926,7 +8070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:68">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>56</v>
       </c>
@@ -7940,7 +8084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:68">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>64</v>
       </c>
@@ -7954,7 +8098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:68">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -7968,7 +8112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:68">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -7982,7 +8126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:68">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>109</v>
       </c>
@@ -7996,7 +8140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:68">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>76</v>
       </c>
@@ -8010,7 +8154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:68">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>81</v>
       </c>
@@ -8024,7 +8168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:68">
+    <row r="32" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -8038,7 +8182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
@@ -8052,7 +8196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -8066,9 +8210,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
@@ -8080,7 +8224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>108</v>
       </c>
@@ -8094,45 +8238,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B37" s="6">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F37" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B38" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B39" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B40" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>72</v>
       </c>
@@ -8140,7 +8284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -8148,7 +8292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>105</v>
       </c>
@@ -8156,7 +8300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>120</v>
       </c>
@@ -8164,7 +8308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>30</v>
       </c>
@@ -8172,7 +8316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>24</v>
       </c>
@@ -8180,7 +8324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>44</v>
       </c>
@@ -8188,7 +8332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>36</v>
       </c>
@@ -8196,7 +8340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
@@ -8204,7 +8348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>73</v>
       </c>
@@ -8212,7 +8356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>101</v>
       </c>
@@ -8220,7 +8364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -8228,7 +8372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>58</v>
       </c>
@@ -8236,7 +8380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>10</v>
       </c>
@@ -8244,7 +8388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>74</v>
       </c>
@@ -8252,15 +8396,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B56" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>82</v>
       </c>
@@ -8268,7 +8412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>52</v>
       </c>
@@ -8276,7 +8420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -8284,15 +8428,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B60" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>104</v>
       </c>
@@ -8300,7 +8444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>31</v>
       </c>
@@ -8308,7 +8452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>33</v>
       </c>
@@ -8316,21 +8460,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B64" s="6"/>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B65" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
added Li et al. to excel publist
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@1155 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="19005" windowHeight="11130" tabRatio="500"/>
@@ -10,8 +10,7 @@
     <sheet name="Original reference list" sheetId="1" r:id="rId1"/>
     <sheet name="Species statistics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
     <pivotCache cacheId="1" r:id="rId4"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="269">
   <si>
     <t>Dalgleish, Koons, Hooten, Moffet &amp; Adler</t>
   </si>
@@ -847,12 +846,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Li, Yu, Werger, Dong, Ramula &amp; Zuidema</t>
+  </si>
+  <si>
+    <t>Caragana intermedia</t>
+  </si>
+  <si>
+    <t>Li S-L, Yu F-H, Werger MJA, Dong M, Ramula S &amp; Zuidema PA (2013) Understanding the effects of a new grazing policy: the impact of seasonal grazing on shrub demography in the Inner Mongolian steppe. Journal of Applied Ecology in press</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1620,40 +1628,18 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
       <c:perspective val="30"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1668,7 +1654,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Species statistics'!$E$24:$E$37</c:f>
@@ -1771,26 +1756,17 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:dLbls/>
         <c:shape val="box"/>
-        <c:axId val="158371840"/>
-        <c:axId val="158373760"/>
+        <c:axId val="78372864"/>
+        <c:axId val="78374784"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="158371840"/>
+        <c:axId val="78372864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1808,25 +1784,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158373760"/>
+        <c:crossAx val="78374784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158373760"/>
+        <c:axId val="78374784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1844,20 +1815,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158371840"/>
+        <c:crossAx val="78372864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1882,7 +1849,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4098,20 +4065,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="33.875" customWidth="1"/>
     <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
@@ -4121,7 +4088,7 @@
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4144,7 +4111,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -4164,7 +4131,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -4184,7 +4151,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -4204,7 +4171,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -4224,7 +4191,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -4244,7 +4211,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -4264,7 +4231,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>189</v>
       </c>
@@ -4284,7 +4251,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -4304,7 +4271,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4324,7 +4291,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -4347,7 +4314,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -4367,7 +4334,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4387,7 +4354,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4407,7 +4374,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>220</v>
       </c>
@@ -4427,7 +4394,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -4447,7 +4414,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4467,7 +4434,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -4487,7 +4454,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -4507,7 +4474,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -4527,7 +4494,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -4547,7 +4514,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -4567,7 +4534,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -4587,7 +4554,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -4607,7 +4574,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>250</v>
       </c>
@@ -4627,7 +4594,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>217</v>
       </c>
@@ -4647,7 +4614,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -4667,7 +4634,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -4687,7 +4654,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -4707,7 +4674,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -4727,7 +4694,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -4747,7 +4714,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>197</v>
       </c>
@@ -4767,7 +4734,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -4787,7 +4754,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>258</v>
       </c>
@@ -4807,7 +4774,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>236</v>
       </c>
@@ -4827,7 +4794,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>236</v>
       </c>
@@ -4847,7 +4814,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -4870,7 +4837,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>196</v>
       </c>
@@ -4893,7 +4860,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -4913,7 +4880,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="10" t="s">
         <v>119</v>
       </c>
@@ -4936,7 +4903,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
         <v>230</v>
       </c>
@@ -4956,7 +4923,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -4976,7 +4943,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>205</v>
       </c>
@@ -4999,7 +4966,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -5019,7 +4986,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -5039,7 +5006,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -5059,92 +5026,92 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>204</v>
+      </c>
+      <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G47" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
         <v>41</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>19</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <v>2011</v>
       </c>
-      <c r="D47" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="9" t="s">
+      <c r="D48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>182</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>2009</v>
       </c>
-      <c r="D48" t="s">
-        <v>195</v>
-      </c>
-      <c r="E48" s="9" t="s">
+      <c r="D49" t="s">
+        <v>195</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
         <v>245</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>246</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>2012</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E50" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
         <v>83</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>78</v>
-      </c>
-      <c r="C50">
-        <v>2009</v>
-      </c>
-      <c r="D50" t="s">
-        <v>195</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" t="s">
-        <v>184</v>
       </c>
       <c r="C51">
         <v>2009</v>
@@ -5153,13 +5120,13 @@
         <v>195</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="G51" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -5173,13 +5140,13 @@
         <v>195</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G52" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -5193,13 +5160,13 @@
         <v>195</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G53" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -5213,13 +5180,13 @@
         <v>195</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G54" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -5233,13 +5200,13 @@
         <v>195</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G55" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>100</v>
       </c>
@@ -5253,13 +5220,13 @@
         <v>195</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G56" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -5273,13 +5240,13 @@
         <v>195</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G57" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -5293,13 +5260,13 @@
         <v>195</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G58" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>100</v>
       </c>
@@ -5313,13 +5280,13 @@
         <v>195</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G59" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -5333,58 +5300,58 @@
         <v>195</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G60" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C61">
+        <v>2009</v>
+      </c>
+      <c r="D61" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G61" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
         <v>225</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>226</v>
       </c>
-      <c r="C61">
+      <c r="C62">
         <v>2013</v>
       </c>
-      <c r="D61" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" s="9" t="s">
+      <c r="D62" t="s">
+        <v>195</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
         <v>114</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>115</v>
-      </c>
-      <c r="C62">
-        <v>2009</v>
-      </c>
-      <c r="D62" t="s">
-        <v>195</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G62" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" t="s">
-        <v>188</v>
       </c>
       <c r="C63">
         <v>2009</v>
@@ -5393,173 +5360,173 @@
         <v>195</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G63" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="B64" t="s">
         <v>188</v>
       </c>
       <c r="C64">
+        <v>2009</v>
+      </c>
+      <c r="D64" t="s">
+        <v>195</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65">
         <v>2007</v>
       </c>
-      <c r="D64" t="s">
-        <v>195</v>
-      </c>
-      <c r="E64" s="9" t="s">
+      <c r="D65" t="s">
+        <v>195</v>
+      </c>
+      <c r="E65" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
         <v>45</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>179</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>2009</v>
       </c>
-      <c r="D65" t="s">
-        <v>195</v>
-      </c>
-      <c r="E65" s="9" t="s">
+      <c r="D66" t="s">
+        <v>195</v>
+      </c>
+      <c r="E66" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G66" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
         <v>180</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>181</v>
       </c>
-      <c r="C66">
+      <c r="C67">
         <v>2012</v>
       </c>
-      <c r="D66" t="s">
-        <v>195</v>
-      </c>
-      <c r="E66" s="9" t="s">
+      <c r="D67" t="s">
+        <v>195</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G66" s="12" t="s">
+      <c r="G67" s="12" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
         <v>75</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>19</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>2011</v>
       </c>
-      <c r="D67" t="s">
-        <v>195</v>
-      </c>
-      <c r="E67" s="9" t="s">
+      <c r="D68" t="s">
+        <v>195</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G68" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>46</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>47</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>2010</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G68" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>201</v>
-      </c>
-      <c r="B69" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69">
-        <v>2012</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="G69" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C70">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E70" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G70" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>253</v>
+      </c>
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71">
+        <v>2013</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G71" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" t="s">
-        <v>50</v>
-      </c>
-      <c r="C71">
-        <v>2009</v>
-      </c>
-      <c r="D71" t="s">
-        <v>195</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -5573,93 +5540,93 @@
         <v>195</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G72" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73">
+        <v>2009</v>
+      </c>
+      <c r="D73" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
         <v>118</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>182</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>2012</v>
       </c>
-      <c r="D73" t="s">
-        <v>195</v>
-      </c>
-      <c r="E73" s="9" t="s">
+      <c r="D74" t="s">
+        <v>195</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G74" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>53</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>179</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>2009</v>
       </c>
-      <c r="D74" t="s">
-        <v>195</v>
-      </c>
-      <c r="E74" s="9" t="s">
+      <c r="D75" t="s">
+        <v>195</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G75" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
         <v>54</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>185</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>2002</v>
       </c>
-      <c r="D75" t="s">
-        <v>195</v>
-      </c>
-      <c r="E75" s="9" t="s">
+      <c r="D76" t="s">
+        <v>195</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G76" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76">
-        <v>2006</v>
-      </c>
-      <c r="D76" t="s">
-        <v>195</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -5673,159 +5640,159 @@
         <v>195</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G77" s="11" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78">
+        <v>2006</v>
+      </c>
+      <c r="D78" t="s">
+        <v>195</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
         <v>111</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>112</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>2009</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F79" t="s">
         <v>121</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
         <v>55</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>184</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>2005</v>
       </c>
-      <c r="D79" t="s">
-        <v>195</v>
-      </c>
-      <c r="E79" s="9" t="s">
+      <c r="D80" t="s">
+        <v>195</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="G80" s="11" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
         <v>157</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>181</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>2012</v>
       </c>
-      <c r="D80" t="s">
-        <v>195</v>
-      </c>
-      <c r="E80" s="9" t="s">
+      <c r="D81" t="s">
+        <v>195</v>
+      </c>
+      <c r="E81" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G80" s="11" t="s">
+      <c r="G81" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
         <v>158</v>
-      </c>
-      <c r="B81" t="s">
-        <v>26</v>
-      </c>
-      <c r="C81">
-        <v>2010</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F81" t="s">
-        <v>121</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>256</v>
       </c>
       <c r="B82" t="s">
         <v>26</v>
       </c>
       <c r="C82">
+        <v>2010</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F82" t="s">
+        <v>121</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>256</v>
+      </c>
+      <c r="B83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83">
         <v>2013</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E83" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="G82" s="11" t="s">
+      <c r="G83" s="11" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
         <v>209</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>184</v>
       </c>
-      <c r="C83">
+      <c r="C84">
         <v>2012</v>
       </c>
-      <c r="D83" t="s">
-        <v>195</v>
-      </c>
-      <c r="E83" s="9" t="s">
+      <c r="D84" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="G83" s="11" t="s">
+      <c r="G84" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>57</v>
-      </c>
-      <c r="B84" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84">
-        <v>2010</v>
-      </c>
-      <c r="D84" t="s">
-        <v>195</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>57</v>
       </c>
@@ -5839,58 +5806,58 @@
         <v>195</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86">
+        <v>2010</v>
+      </c>
+      <c r="D86" t="s">
+        <v>195</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
         <v>60</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>19</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>2005</v>
       </c>
-      <c r="D86" t="s">
-        <v>195</v>
-      </c>
-      <c r="E86" s="9" t="s">
+      <c r="D87" t="s">
+        <v>195</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G86" s="11" t="s">
+      <c r="G87" s="11" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
         <v>242</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>243</v>
-      </c>
-      <c r="C87">
-        <v>2012</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>170</v>
-      </c>
-      <c r="B88" t="s">
-        <v>171</v>
       </c>
       <c r="C88">
         <v>2012</v>
@@ -5901,22 +5868,19 @@
       <c r="E88" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F88" t="s">
-        <v>121</v>
-      </c>
-      <c r="G88" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G88" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>62</v>
+        <v>170</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C89">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>120</v>
@@ -5924,19 +5888,22 @@
       <c r="E89" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G89" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>121</v>
+      </c>
+      <c r="G89" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C90">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>120</v>
@@ -5945,15 +5912,15 @@
         <v>120</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B91" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C91">
         <v>2012</v>
@@ -5965,113 +5932,110 @@
         <v>120</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>222</v>
+        <v>122</v>
       </c>
       <c r="B92" t="s">
-        <v>17</v>
+        <v>186</v>
       </c>
       <c r="C92">
         <v>2012</v>
       </c>
       <c r="D92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>222</v>
+      </c>
+      <c r="B93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93">
+        <v>2012</v>
+      </c>
+      <c r="D93" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E92" s="9" t="s">
+      <c r="E93" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G93" s="11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
         <v>63</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>26</v>
       </c>
-      <c r="C93">
+      <c r="C94">
         <v>2009</v>
       </c>
-      <c r="D93" t="s">
-        <v>195</v>
-      </c>
-      <c r="E93" s="9" t="s">
+      <c r="D94" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G93" s="11" t="s">
+      <c r="G94" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
         <v>66</v>
-      </c>
-      <c r="B94" t="s">
-        <v>184</v>
-      </c>
-      <c r="C94">
-        <v>2006</v>
-      </c>
-      <c r="D94" t="s">
-        <v>195</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G94" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>67</v>
       </c>
       <c r="B95" t="s">
         <v>184</v>
       </c>
       <c r="C95">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D95" t="s">
         <v>195</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>215</v>
+        <v>67</v>
       </c>
       <c r="B96" t="s">
         <v>184</v>
       </c>
       <c r="C96">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D96" t="s">
         <v>195</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="F96" t="s">
-        <v>265</v>
+        <v>64</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>215</v>
       </c>
@@ -6085,13 +6049,16 @@
         <v>195</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>65</v>
+        <v>216</v>
+      </c>
+      <c r="F97" t="s">
+        <v>265</v>
       </c>
       <c r="G97" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -6105,53 +6072,53 @@
         <v>195</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="G98" s="11" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
+        <v>215</v>
+      </c>
+      <c r="B99" t="s">
+        <v>184</v>
+      </c>
+      <c r="C99">
+        <v>2012</v>
+      </c>
+      <c r="D99" t="s">
+        <v>195</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
         <v>262</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>21</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>204</v>
       </c>
-      <c r="D99" t="s">
-        <v>195</v>
-      </c>
-      <c r="E99" s="9" t="s">
+      <c r="D100" t="s">
+        <v>195</v>
+      </c>
+      <c r="E100" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="G99" s="11" t="s">
+      <c r="G100" s="11" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>68</v>
-      </c>
-      <c r="B100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100">
-        <v>2010</v>
-      </c>
-      <c r="D100" t="s">
-        <v>195</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G100" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -6165,13 +6132,13 @@
         <v>195</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>68</v>
       </c>
@@ -6185,13 +6152,13 @@
         <v>195</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G102" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>68</v>
       </c>
@@ -6205,13 +6172,13 @@
         <v>195</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G103" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>68</v>
       </c>
@@ -6225,13 +6192,13 @@
         <v>195</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>68</v>
       </c>
@@ -6245,14 +6212,34 @@
         <v>195</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G105" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E107" s="9"/>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106">
+        <v>2010</v>
+      </c>
+      <c r="D106" t="s">
+        <v>195</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="E108" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:G75">
@@ -6269,7 +6256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -6279,7 +6266,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.875" customWidth="1"/>
     <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
@@ -6349,12 +6336,12 @@
     <col min="68" max="68" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68">
       <c r="A1" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68">
       <c r="A2" s="4" t="s">
         <v>90</v>
       </c>
@@ -6362,7 +6349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -6376,7 +6363,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -6576,7 +6563,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68">
       <c r="A5" s="5" t="s">
         <v>216</v>
       </c>
@@ -6654,7 +6641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68">
       <c r="A6" s="5" t="s">
         <v>65</v>
       </c>
@@ -6732,7 +6719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -6810,7 +6797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68">
       <c r="A8" s="5" t="s">
         <v>84</v>
       </c>
@@ -6888,7 +6875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68">
       <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
@@ -6968,7 +6955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -7052,7 +7039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68">
       <c r="A11" s="5" t="s">
         <v>106</v>
       </c>
@@ -7132,7 +7119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -7214,7 +7201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -7334,7 +7321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -7450,7 +7437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68">
       <c r="A15" s="5" t="s">
         <v>117</v>
       </c>
@@ -7550,7 +7537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -7666,7 +7653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:68">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -7740,7 +7727,7 @@
       <c r="BO17" s="6"/>
       <c r="BP17" s="6"/>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:68">
       <c r="A18" s="5" t="s">
         <v>103</v>
       </c>
@@ -7820,7 +7807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:68">
       <c r="A19" s="5" t="s">
         <v>102</v>
       </c>
@@ -8018,7 +8005,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:68">
       <c r="A20" s="5" t="s">
         <v>231</v>
       </c>
@@ -8026,7 +8013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:68">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -8034,7 +8021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:68">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -8042,7 +8029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:68">
       <c r="A23" s="5" t="s">
         <v>98</v>
       </c>
@@ -8056,7 +8043,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:68">
       <c r="A24" s="5" t="s">
         <v>223</v>
       </c>
@@ -8070,7 +8057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:68">
       <c r="A25" s="5" t="s">
         <v>56</v>
       </c>
@@ -8084,7 +8071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:68">
       <c r="A26" s="5" t="s">
         <v>64</v>
       </c>
@@ -8098,7 +8085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:68">
       <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
@@ -8112,7 +8099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:68">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -8126,7 +8113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:68">
       <c r="A29" s="5" t="s">
         <v>109</v>
       </c>
@@ -8140,7 +8127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:68">
       <c r="A30" s="5" t="s">
         <v>76</v>
       </c>
@@ -8154,7 +8141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:68">
       <c r="A31" s="5" t="s">
         <v>81</v>
       </c>
@@ -8168,7 +8155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:68">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -8182,7 +8169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
@@ -8196,7 +8183,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="5" t="s">
         <v>107</v>
       </c>
@@ -8210,7 +8197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
         <v>227</v>
       </c>
@@ -8224,7 +8211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="5" t="s">
         <v>108</v>
       </c>
@@ -8238,7 +8225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
         <v>213</v>
       </c>
@@ -8252,7 +8239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">
         <v>237</v>
       </c>
@@ -8260,7 +8247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
         <v>193</v>
       </c>
@@ -8268,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="5" t="s">
         <v>238</v>
       </c>
@@ -8276,7 +8263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="5" t="s">
         <v>72</v>
       </c>
@@ -8284,7 +8271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="5" t="s">
         <v>48</v>
       </c>
@@ -8292,7 +8279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
         <v>105</v>
       </c>
@@ -8300,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
         <v>120</v>
       </c>
@@ -8308,7 +8295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
         <v>30</v>
       </c>
@@ -8316,7 +8303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
         <v>24</v>
       </c>
@@ -8324,7 +8311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="5" t="s">
         <v>44</v>
       </c>
@@ -8332,7 +8319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
         <v>36</v>
       </c>
@@ -8340,7 +8327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
@@ -8348,7 +8335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="5" t="s">
         <v>73</v>
       </c>
@@ -8356,7 +8343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="5" t="s">
         <v>101</v>
       </c>
@@ -8364,7 +8351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="5" t="s">
         <v>59</v>
       </c>
@@ -8372,7 +8359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="5" t="s">
         <v>58</v>
       </c>
@@ -8380,7 +8367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="5" t="s">
         <v>10</v>
       </c>
@@ -8388,7 +8375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="5" t="s">
         <v>74</v>
       </c>
@@ -8396,7 +8383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="5" t="s">
         <v>210</v>
       </c>
@@ -8404,7 +8391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="5" t="s">
         <v>82</v>
       </c>
@@ -8412,7 +8399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="5" t="s">
         <v>52</v>
       </c>
@@ -8420,7 +8407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -8428,7 +8415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="5" t="s">
         <v>202</v>
       </c>
@@ -8436,7 +8423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="5" t="s">
         <v>104</v>
       </c>
@@ -8444,7 +8431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
         <v>31</v>
       </c>
@@ -8452,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="5" t="s">
         <v>33</v>
       </c>
@@ -8460,13 +8447,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B64" s="6"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="5" t="s">
         <v>247</v>
       </c>
@@ -8474,7 +8461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
added ref to list
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@1170 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="270">
   <si>
     <t>Authors</t>
   </si>
@@ -321,9 +321,6 @@
     <t>Veratrum album</t>
   </si>
   <si>
-    <t>Hesse E, Rees M &amp; Müller-Schärer (2008) Life-history variation in contrasting habitats: flowering decision in a clonal perennial herb (Veratrum album). The American Naturalist 172: 196-213</t>
-  </si>
-  <si>
     <t>Jacquemyn, Brys &amp; Jongejans</t>
   </si>
   <si>
@@ -555,9 +552,6 @@
     <t>Sancassania berlesei</t>
   </si>
   <si>
-    <t>Ozgul A, Coulson T, Reynolds A, Cameron TC &amp; Benton TG (2012) Population responses to perturbations: the importance of trait-based analysis illustrated through a microcosm experiment. The American Naturalist 179: 582-594</t>
-  </si>
-  <si>
     <t>Perkins, Phillips, Baskett &amp; Hastings</t>
   </si>
   <si>
@@ -597,9 +591,6 @@
     <t>Phil Trans B</t>
   </si>
   <si>
-    <t>Rees M &amp; Rose KE (2002) Evolution of flowering strategies in Oenothera glazioviana: an integral projection model approach. Proceedings of the Royal Society of London, Series B 269: 1509-1515</t>
-  </si>
-  <si>
     <t>Rees, Childs, Metcalf, Rose, Sheppard &amp; Grubb</t>
   </si>
   <si>
@@ -621,22 +612,13 @@
     <t>Rose, Louda &amp; Rees</t>
   </si>
   <si>
-    <t>Rose KE, Louda SM &amp; Rees M (2005) Demographic and evolutionary impacts of native and invasive herbivores on Cirsium canescens. Ecology 86: 453-465</t>
-  </si>
-  <si>
     <t>Salguero-Gomez, Siewert, Casper &amp; Tielborger</t>
   </si>
   <si>
     <t>Cryptantha flava</t>
   </si>
   <si>
-    <t>Salguero-Gomez R, Siewert W, Casper BB &amp; Tielbörger K (2012) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B 367: 3100-3114</t>
-  </si>
-  <si>
     <t>Salguero-Gomez &amp; Plotkin</t>
-  </si>
-  <si>
-    <t>Salguero-Gomez R &amp; Plotkin BJ (2010) Matrix dimensions bias demographic inferences: implications for comparative plant demography. The American Naturalist 176: 710-722</t>
   </si>
   <si>
     <t>Schindler, Neuhaus, Gaillard &amp; Coulson</t>
@@ -686,9 +668,6 @@
     <t>Phylospadix serrulatus</t>
   </si>
   <si>
-    <t>Shelton AO (2010) The ecological and evolutionary drivers of female-biased sex ratios: two-sex models of perennial seagrasses. The American Naturalist 175: 302-315</t>
-  </si>
-  <si>
     <t>Phylospadix scouleri</t>
   </si>
   <si>
@@ -707,9 +686,6 @@
     <t>TREE</t>
   </si>
   <si>
-    <t>Smallegange IM &amp; Coulson T (2012) Towards a general, population-level understanding of eco-evolutionary change. Trends in Ecology &amp; Evolution 1590, XXXX-XXXX</t>
-  </si>
-  <si>
     <t>Townley, Rebarber &amp; Tenhumberg</t>
   </si>
   <si>
@@ -753,9 +729,6 @@
   </si>
   <si>
     <t>Cynoglossum officinale</t>
-  </si>
-  <si>
-    <t>Williams JL (2009) Flowering life-history strategies differ between the native and introduced ranges of a monocarpic perennial. The American Naturalist 174: 660-672</t>
   </si>
   <si>
     <t>Williams &amp; Crone</t>
@@ -861,7 +834,135 @@
     <t>Polygonum cuspidatum</t>
   </si>
   <si>
-    <t>Dauer JT &amp; Jongejans E (2013) Elucidating the population dynamics of Japanese knotweed using integral projection models. PLoS ONE in press</t>
+    <t>van der Meer S, Dahlgren JP, Mildén M &amp; Ehrlén J</t>
+  </si>
+  <si>
+    <t>Succisa pratensis</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">van der Meer S, Dahlgren JP, Mildén M &amp; Ehrlén J (2013) Differential effects of abandonment on the demography of the grassland perennial </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Succisa pratensis. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Population Ecology, in press</t>
+    </r>
+  </si>
+  <si>
+    <t>Williams JL (2009) Flowering life-history strategies differ between the native and introduced ranges of a monocarpic perennial. American Naturalist 174: 660-672</t>
+  </si>
+  <si>
+    <t>Shelton AO (2010) The ecological and evolutionary drivers of female-biased sex ratios: two-sex models of perennial seagrasses. American Naturalist 175: 302-315</t>
+  </si>
+  <si>
+    <t>Salguero-Gómez R &amp; Plotkin BJ (2010) Matrix dimensions bias demographic inferences: implications for comparative plant demography. American Naturalist 176: 710-722</t>
+  </si>
+  <si>
+    <t>Salguero-Gómez R, Siewert W, Casper BB &amp; Tielbörger K (2012) A demographic approach to study effects of climate change in desert plants. Philosophical Transaction of the Royal Society Series B 367: 3100-3114</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rees M &amp; Rose KE (2002) Evolution of flowering strategies in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Oenothera glazioviana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: an integral projection model approach. Proceedings of the Royal Society of London, Series B 269: 1509-1515</t>
+    </r>
+  </si>
+  <si>
+    <t>Ozgul A, Coulson T, Reynolds A, Cameron TC &amp; Benton TG (2012) Population responses to perturbations: the importance of trait-based analysis illustrated through a microcosm experiment. American Naturalist 179: 582-594</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rose KE, Louda SM &amp; Rees M (2005) Demographic and evolutionary impacts of native and invasive herbivores on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cirsium canescens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Ecology 86: 453-465</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hesse E, Rees M &amp; Müller-Schärer (2008) Life-history variation in contrasting habitats: flowering decision in a clonal perennial herb (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Veratrum album</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). American Naturalist 172: 196-213</t>
+    </r>
+  </si>
+  <si>
+    <t>Dauer JT &amp; Jongejans E (2013) Elucidating the population dynamics of Japanese knotweed using integral projection models. PLOS ONE in 8:e75181</t>
+  </si>
+  <si>
+    <t>Smallegange IM &amp; Coulson T (2012) Towards a general, population-level understanding of eco-evolutionary change. Trends in Ecology and Evolution 1590, XXXX-XXXX</t>
   </si>
 </sst>
 </file>
@@ -1917,11 +2018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2421,10 +2522,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>76</v>
@@ -2433,11 +2534,11 @@
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2756,12 +2857,12 @@
         <v>26</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>101</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>16</v>
@@ -2773,16 +2874,16 @@
         <v>9</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>16</v>
@@ -2797,15 +2898,15 @@
         <v>61</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>16</v>
@@ -2817,16 +2918,16 @@
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>51</v>
@@ -2838,19 +2939,19 @@
         <v>9</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C44" s="1">
         <v>2008</v>
@@ -2862,18 +2963,18 @@
         <v>61</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C45" s="1">
         <v>2012</v>
@@ -2882,16 +2983,16 @@
         <v>9</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>51</v>
@@ -2903,16 +3004,16 @@
         <v>9</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>16</v>
@@ -2924,19 +3025,19 @@
         <v>9</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>76</v>
@@ -2945,16 +3046,16 @@
         <v>9</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>16</v>
@@ -2966,16 +3067,16 @@
         <v>9</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>75</v>
@@ -2991,15 +3092,15 @@
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C51" s="1">
         <v>2012</v>
@@ -3008,16 +3109,16 @@
         <v>24</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
@@ -3029,16 +3130,16 @@
         <v>9</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>51</v>
@@ -3050,16 +3151,16 @@
         <v>9</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>51</v>
@@ -3071,16 +3172,16 @@
         <v>9</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>51</v>
@@ -3092,16 +3193,16 @@
         <v>9</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>51</v>
@@ -3113,16 +3214,16 @@
         <v>9</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>51</v>
@@ -3134,16 +3235,16 @@
         <v>9</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>51</v>
@@ -3155,16 +3256,16 @@
         <v>9</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>51</v>
@@ -3176,16 +3277,16 @@
         <v>9</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>51</v>
@@ -3197,16 +3298,16 @@
         <v>9</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>51</v>
@@ -3218,16 +3319,16 @@
         <v>9</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>51</v>
@@ -3239,19 +3340,19 @@
         <v>9</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C63" s="1">
         <v>2013</v>
@@ -3260,19 +3361,19 @@
         <v>9</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C64" s="1">
         <v>2009</v>
@@ -3281,19 +3382,19 @@
         <v>9</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="C65" s="1">
         <v>2009</v>
@@ -3306,15 +3407,15 @@
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C66" s="1">
         <v>2007</v>
@@ -3323,16 +3424,16 @@
         <v>9</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>23</v>
@@ -3344,16 +3445,16 @@
         <v>9</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>32</v>
@@ -3365,16 +3466,16 @@
         <v>9</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>16</v>
@@ -3386,19 +3487,19 @@
         <v>9</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="C70" s="1">
         <v>2010</v>
@@ -3407,16 +3508,16 @@
         <v>24</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>60</v>
@@ -3428,16 +3529,16 @@
         <v>24</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
@@ -3449,19 +3550,19 @@
         <v>24</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C73" s="1">
         <v>2009</v>
@@ -3470,19 +3571,19 @@
         <v>9</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C74" s="1">
         <v>2009</v>
@@ -3491,16 +3592,16 @@
         <v>9</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>75</v>
@@ -3516,12 +3617,12 @@
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>23</v>
@@ -3537,15 +3638,15 @@
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C77" s="1">
         <v>2002</v>
@@ -3558,12 +3659,12 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>193</v>
+        <v>264</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>60</v>
@@ -3579,12 +3680,12 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>60</v>
@@ -3596,19 +3697,19 @@
         <v>9</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C80" s="1">
         <v>2009</v>
@@ -3620,15 +3721,15 @@
         <v>61</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>51</v>
@@ -3644,12 +3745,12 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="7" t="s">
-        <v>201</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
@@ -3661,16 +3762,16 @@
         <v>9</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="7" t="s">
-        <v>204</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>60</v>
@@ -3685,15 +3786,15 @@
         <v>61</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>60</v>
@@ -3705,16 +3806,16 @@
         <v>24</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>51</v>
@@ -3726,16 +3827,16 @@
         <v>9</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>60</v>
@@ -3747,16 +3848,16 @@
         <v>9</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="7" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>60</v>
@@ -3768,16 +3869,16 @@
         <v>9</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="7" t="s">
-        <v>215</v>
+        <v>261</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>16</v>
@@ -3789,19 +3890,19 @@
         <v>9</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="7" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C89" s="1">
         <v>2012</v>
@@ -3814,15 +3915,15 @@
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="7" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C90" s="1">
         <v>2012</v>
@@ -3834,42 +3935,42 @@
         <v>61</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>226</v>
+        <v>257</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C91" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="F91" s="1"/>
-      <c r="G91" s="7" t="s">
-        <v>227</v>
+      <c r="G91" s="1" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C92" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>61</v>
@@ -3879,161 +3980,159 @@
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2012</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>262</v>
+        <v>61</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F93" s="1"/>
-      <c r="G93" s="1" t="s">
-        <v>263</v>
+      <c r="G93" s="7" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C94" s="1">
-        <v>2012</v>
+        <v>51</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="F94" s="1"/>
-      <c r="G94" s="7" t="s">
-        <v>232</v>
+      <c r="G94" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>44</v>
+        <v>223</v>
       </c>
       <c r="C95" s="1">
         <v>2012</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>234</v>
+        <v>61</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="7" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C96" s="1">
-        <v>2009</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>9</v>
+        <v>2012</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="7" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C97" s="1">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="7" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C98" s="1">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C99" s="1">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="F99" s="1"/>
       <c r="G99" s="7" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>51</v>
@@ -4045,16 +4144,18 @@
         <v>9</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="F100" s="1"/>
+        <v>236</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="G100" s="7" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>51</v>
@@ -4066,58 +4167,58 @@
         <v>9</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>166</v>
+        <v>231</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="7" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>76</v>
+        <v>51</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2012</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>249</v>
+        <v>165</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="7" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="1">
-        <v>2010</v>
+        <v>37</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="7" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>16</v>
@@ -4129,16 +4230,16 @@
         <v>9</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="7" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>16</v>
@@ -4150,16 +4251,16 @@
         <v>9</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="7" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>16</v>
@@ -4171,16 +4272,16 @@
         <v>9</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="7" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>16</v>
@@ -4192,16 +4293,16 @@
         <v>9</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="7" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>16</v>
@@ -4213,11 +4314,32 @@
         <v>9</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="7" t="s">
-        <v>253</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="7" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to IPM list
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/ipmpack@1183 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/www/IPMpublications.xlsx
+++ b/www/IPMpublications.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19005" windowHeight="11130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="270">
   <si>
     <t>Authors</t>
   </si>
@@ -250,9 +251,6 @@
   </si>
   <si>
     <t>Lepidium latifolium</t>
-  </si>
-  <si>
-    <t>Ellner SP &amp; Schreiber SJ (In press) Temporarilly variable dispersal and demography can accelerate the spread of invading species. Theoretical Population Biology x: xxx-xxx</t>
   </si>
   <si>
     <t>Ferrer-Cervantes, Mendez-Gonzalez, Quintana-Ascencio, Dorantes, Dzib &amp; Duran</t>
@@ -794,9 +792,6 @@
     <t>Dauer &amp; Jongejans</t>
   </si>
   <si>
-    <t>PLoS ONE</t>
-  </si>
-  <si>
     <t>Perspect Plant Ecol Evol Syst</t>
   </si>
   <si>
@@ -963,6 +958,12 @@
   </si>
   <si>
     <t>Smallegange IM &amp; Coulson T (2012) Towards a general, population-level understanding of eco-evolutionary change. Trends in Ecology and Evolution 1590, XXXX-XXXX</t>
+  </si>
+  <si>
+    <t>PLOS ONE</t>
+  </si>
+  <si>
+    <t>Ellner SP &amp; Schreiber SJ (2012) Temporarilly variable dispersal and demography can accelerate the spread of invading species. Theoretical Population Biology 82: 283-298</t>
   </si>
 </sst>
 </file>
@@ -2020,9 +2021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,23 +2523,23 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>268</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2013</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2674,8 +2675,8 @@
       <c r="B31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>76</v>
+      <c r="C31" s="1">
+        <v>2012</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
@@ -2685,15 +2686,15 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>78</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C32" s="1">
         <v>2012</v>
@@ -2702,16 +2703,16 @@
         <v>9</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>16</v>
@@ -2727,12 +2728,12 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>32</v>
@@ -2744,19 +2745,19 @@
         <v>9</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C35" s="1">
         <v>2013</v>
@@ -2765,19 +2766,19 @@
         <v>9</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C36" s="1">
         <v>2012</v>
@@ -2786,19 +2787,19 @@
         <v>9</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C37" s="1">
         <v>2012</v>
@@ -2807,19 +2808,19 @@
         <v>9</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="1">
         <v>2010</v>
@@ -2828,18 +2829,18 @@
         <v>9</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>60</v>
@@ -2851,18 +2852,18 @@
         <v>9</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>16</v>
@@ -2874,16 +2875,16 @@
         <v>9</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>16</v>
@@ -2898,15 +2899,15 @@
         <v>61</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>16</v>
@@ -2918,16 +2919,16 @@
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>51</v>
@@ -2939,19 +2940,19 @@
         <v>9</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C44" s="1">
         <v>2008</v>
@@ -2963,18 +2964,18 @@
         <v>61</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C45" s="1">
         <v>2012</v>
@@ -2983,16 +2984,16 @@
         <v>9</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>51</v>
@@ -3004,16 +3005,16 @@
         <v>9</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>16</v>
@@ -3025,19 +3026,19 @@
         <v>9</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>76</v>
@@ -3046,16 +3047,16 @@
         <v>9</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>16</v>
@@ -3067,16 +3068,16 @@
         <v>9</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>75</v>
@@ -3092,15 +3093,15 @@
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C51" s="1">
         <v>2012</v>
@@ -3109,16 +3110,16 @@
         <v>24</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
@@ -3130,16 +3131,16 @@
         <v>9</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>51</v>
@@ -3151,16 +3152,16 @@
         <v>9</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>51</v>
@@ -3172,16 +3173,16 @@
         <v>9</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>51</v>
@@ -3193,16 +3194,16 @@
         <v>9</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>51</v>
@@ -3214,16 +3215,16 @@
         <v>9</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>51</v>
@@ -3235,16 +3236,16 @@
         <v>9</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>51</v>
@@ -3256,16 +3257,16 @@
         <v>9</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>51</v>
@@ -3277,16 +3278,16 @@
         <v>9</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>51</v>
@@ -3298,16 +3299,16 @@
         <v>9</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>51</v>
@@ -3319,16 +3320,16 @@
         <v>9</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>51</v>
@@ -3340,19 +3341,19 @@
         <v>9</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="C63" s="1">
         <v>2013</v>
@@ -3361,19 +3362,19 @@
         <v>9</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="C64" s="1">
         <v>2009</v>
@@ -3382,19 +3383,19 @@
         <v>9</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="C65" s="1">
         <v>2009</v>
@@ -3403,19 +3404,19 @@
         <v>9</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C66" s="1">
         <v>2007</v>
@@ -3424,16 +3425,16 @@
         <v>9</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>23</v>
@@ -3445,16 +3446,16 @@
         <v>9</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>32</v>
@@ -3466,16 +3467,16 @@
         <v>9</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>16</v>
@@ -3487,19 +3488,19 @@
         <v>9</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="C70" s="1">
         <v>2010</v>
@@ -3508,16 +3509,16 @@
         <v>24</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>60</v>
@@ -3529,16 +3530,16 @@
         <v>24</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
@@ -3550,19 +3551,19 @@
         <v>24</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C73" s="1">
         <v>2009</v>
@@ -3571,19 +3572,19 @@
         <v>9</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C74" s="1">
         <v>2009</v>
@@ -3592,16 +3593,16 @@
         <v>9</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>75</v>
@@ -3617,12 +3618,12 @@
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>23</v>
@@ -3638,15 +3639,15 @@
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C77" s="1">
         <v>2002</v>
@@ -3655,16 +3656,16 @@
         <v>9</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>60</v>
@@ -3680,12 +3681,12 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>60</v>
@@ -3697,19 +3698,19 @@
         <v>9</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="C80" s="1">
         <v>2009</v>
@@ -3721,15 +3722,15 @@
         <v>61</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G80" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>51</v>
@@ -3745,12 +3746,12 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>32</v>
@@ -3762,16 +3763,16 @@
         <v>9</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>60</v>
@@ -3786,15 +3787,15 @@
         <v>61</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>60</v>
@@ -3806,16 +3807,16 @@
         <v>24</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>51</v>
@@ -3827,16 +3828,16 @@
         <v>9</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>60</v>
@@ -3848,16 +3849,16 @@
         <v>9</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>60</v>
@@ -3869,16 +3870,16 @@
         <v>9</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>16</v>
@@ -3890,19 +3891,19 @@
         <v>9</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="C89" s="1">
         <v>2012</v>
@@ -3915,15 +3916,15 @@
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="C90" s="1">
         <v>2012</v>
@@ -3935,18 +3936,18 @@
         <v>61</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C91" s="1">
         <v>2013</v>
@@ -3955,16 +3956,16 @@
         <v>9</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>51</v>
@@ -3980,12 +3981,12 @@
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>75</v>
@@ -4001,12 +4002,12 @@
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>51</v>
@@ -4018,19 +4019,19 @@
         <v>9</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="C95" s="1">
         <v>2012</v>
@@ -4043,12 +4044,12 @@
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>44</v>
@@ -4060,16 +4061,16 @@
         <v>24</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>60</v>
@@ -4081,16 +4082,16 @@
         <v>9</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>51</v>
@@ -4102,16 +4103,16 @@
         <v>9</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>51</v>
@@ -4123,16 +4124,16 @@
         <v>9</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>51</v>
@@ -4144,18 +4145,18 @@
         <v>9</v>
       </c>
       <c r="E100" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="G100" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>51</v>
@@ -4167,16 +4168,16 @@
         <v>9</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>51</v>
@@ -4188,16 +4189,16 @@
         <v>9</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>37</v>
@@ -4209,16 +4210,16 @@
         <v>9</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>16</v>
@@ -4230,16 +4231,16 @@
         <v>9</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>16</v>
@@ -4251,16 +4252,16 @@
         <v>9</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>16</v>
@@ -4272,16 +4273,16 @@
         <v>9</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>16</v>
@@ -4293,16 +4294,16 @@
         <v>9</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>16</v>
@@ -4314,16 +4315,16 @@
         <v>9</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>16</v>
@@ -4335,11 +4336,11 @@
         <v>9</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>